<commit_message>
Some errors fixed in the enumeration values.
The validation of the example file resulted in many fixes of the
example files and a few fixes in waardelijsten document.
</commit_message>
<xml_diff>
--- a/3. waardelijsten/IMKL2015 - 0.9 waardelijsten.xlsx
+++ b/3. waardelijsten/IMKL2015 - 0.9 waardelijsten.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="26024"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="1660" yWindow="0" windowWidth="28620" windowHeight="19480" tabRatio="645" activeTab="1"/>
+    <workbookView xWindow="37560" yWindow="1240" windowWidth="28620" windowHeight="19480" tabRatio="645" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Toelichting" sheetId="8" r:id="rId1"/>
@@ -14,11 +14,11 @@
     <sheet name="Olie-gas-chemie" sheetId="4" state="hidden" r:id="rId5"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Waardelijst!#REF!</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Waardelijst!$A$1:$G$227</definedName>
     <definedName name="IMKL">Toelichting!$B$22</definedName>
     <definedName name="INSPIRE">Toelichting!$B$23</definedName>
   </definedNames>
-  <calcPr calcId="125725" concurrentCalc="0"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -1220,9 +1220,6 @@
     <t>imkl:extraTopografieType</t>
   </si>
   <si>
-    <t>imkl:extraTopografieTypeValue</t>
-  </si>
-  <si>
     <t>imkl:maatvoeringsType</t>
   </si>
   <si>
@@ -1312,6 +1309,9 @@
   </si>
   <si>
     <t>URL</t>
+  </si>
+  <si>
+    <t>ExtraTopografieTypeValue</t>
   </si>
 </sst>
 </file>
@@ -1484,12 +1484,19 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="12">
+  <cellStyleXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="top"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1578,7 +1585,7 @@
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
-  <cellStyles count="12">
+  <cellStyles count="19">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
@@ -1589,6 +1596,13 @@
     <cellStyle name="Followed Hyperlink" xfId="9" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="11" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="13" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="15" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="17" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
@@ -2187,7 +2201,7 @@
   <sheetData>
     <row r="22" spans="2:3">
       <c r="B22" s="35" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="C22" t="s">
         <v>279</v>
@@ -2221,13 +2235,13 @@
   <dimension ref="A1:G227"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G1" sqref="G1:G1048576"/>
+      <selection activeCell="G91" sqref="G91"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
     <col min="2" max="2" width="12.6640625" customWidth="1"/>
-    <col min="3" max="3" width="26.6640625" customWidth="1"/>
+    <col min="3" max="3" width="37" customWidth="1"/>
     <col min="4" max="4" width="31.33203125" customWidth="1"/>
     <col min="5" max="5" width="16.6640625" customWidth="1"/>
     <col min="6" max="6" width="42.6640625" customWidth="1"/>
@@ -2236,7 +2250,7 @@
   <sheetData>
     <row r="1" spans="1:7" s="4" customFormat="1">
       <c r="A1" s="5" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="B1" s="5" t="s">
         <v>2</v>
@@ -2254,12 +2268,12 @@
         <v>247</v>
       </c>
       <c r="G1" s="5" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
     </row>
     <row r="2" spans="1:7" s="1" customFormat="1">
       <c r="A2" s="1" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="B2" s="12" t="s">
         <v>82</v>
@@ -2277,13 +2291,13 @@
         <v>248</v>
       </c>
       <c r="G2" t="str">
-        <f>IF(B2="inspire",INSPIRE,IMKL) &amp; F2 &amp; "/" &amp; D2</f>
+        <f t="shared" ref="G2:G65" si="0">IF(B2="inspire",INSPIRE,IMKL) &amp; F2 &amp; "/" &amp; D2</f>
         <v>http://www.geonovum.nl/imkl2015/1.0/def/AnnotatieTypeValue/annotatiePijl</v>
       </c>
     </row>
     <row r="3" spans="1:7" s="1" customFormat="1">
       <c r="A3" s="1" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="B3" s="12" t="s">
         <v>82</v>
@@ -2298,13 +2312,13 @@
         <v>248</v>
       </c>
       <c r="G3" t="str">
-        <f>IF(B3="inspire",INSPIRE,IMKL) &amp; F3 &amp; "/" &amp; D3</f>
+        <f t="shared" si="0"/>
         <v>http://www.geonovum.nl/imkl2015/1.0/def/AnnotatieTypeValue/annotatieLijn</v>
       </c>
     </row>
     <row r="4" spans="1:7" s="1" customFormat="1">
       <c r="A4" s="1" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="B4" s="12" t="s">
         <v>82</v>
@@ -2319,13 +2333,13 @@
         <v>248</v>
       </c>
       <c r="G4" t="str">
-        <f>IF(B4="inspire",INSPIRE,IMKL) &amp; F4 &amp; "/" &amp; D4</f>
+        <f t="shared" si="0"/>
         <v>http://www.geonovum.nl/imkl2015/1.0/def/AnnotatieTypeValue/annotatieLabel</v>
       </c>
     </row>
     <row r="5" spans="1:7" s="1" customFormat="1">
       <c r="A5" s="1" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="B5" s="12" t="s">
         <v>82</v>
@@ -2340,13 +2354,13 @@
         <v>249</v>
       </c>
       <c r="G5" t="str">
-        <f>IF(B5="inspire",INSPIRE,IMKL) &amp; F5 &amp; "/" &amp; D5</f>
+        <f t="shared" si="0"/>
         <v>http://www.geonovum.nl/imkl2015/1.0/def/BestandMediaTypeValue/PNG</v>
       </c>
     </row>
     <row r="6" spans="1:7" s="1" customFormat="1">
       <c r="A6" s="1" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="B6" s="12" t="s">
         <v>82</v>
@@ -2361,13 +2375,13 @@
         <v>249</v>
       </c>
       <c r="G6" t="str">
-        <f>IF(B6="inspire",INSPIRE,IMKL) &amp; F6 &amp; "/" &amp; D6</f>
+        <f t="shared" si="0"/>
         <v>http://www.geonovum.nl/imkl2015/1.0/def/BestandMediaTypeValue/PDF</v>
       </c>
     </row>
     <row r="7" spans="1:7" s="1" customFormat="1">
       <c r="A7" s="1" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="B7" s="12" t="s">
         <v>82</v>
@@ -2382,13 +2396,13 @@
         <v>249</v>
       </c>
       <c r="G7" t="str">
-        <f>IF(B7="inspire",INSPIRE,IMKL) &amp; F7 &amp; "/" &amp; D7</f>
+        <f t="shared" si="0"/>
         <v>http://www.geonovum.nl/imkl2015/1.0/def/BestandMediaTypeValue/JPEG</v>
       </c>
     </row>
     <row r="8" spans="1:7" s="1" customFormat="1">
       <c r="A8" s="1" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="B8" s="12" t="s">
         <v>82</v>
@@ -2403,19 +2417,19 @@
         <v>249</v>
       </c>
       <c r="G8" t="str">
-        <f>IF(B8="inspire",INSPIRE,IMKL) &amp; F8 &amp; "/" &amp; D8</f>
+        <f t="shared" si="0"/>
         <v>http://www.geonovum.nl/imkl2015/1.0/def/BestandMediaTypeValue/TIFF</v>
       </c>
     </row>
     <row r="9" spans="1:7" s="1" customFormat="1">
       <c r="A9" s="1" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="B9" s="21" t="s">
         <v>28</v>
       </c>
       <c r="C9" s="12" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="D9" s="12" t="s">
         <v>118</v>
@@ -2425,19 +2439,19 @@
         <v>250</v>
       </c>
       <c r="G9" t="str">
-        <f>IF(B9="inspire",INSPIRE,IMKL) &amp; F9 &amp; "/" &amp; D9</f>
+        <f t="shared" si="0"/>
         <v>http://inspire.ec.europa.eu/codelist/ConditionOfFacilityValue/functional</v>
       </c>
     </row>
     <row r="10" spans="1:7" s="1" customFormat="1">
       <c r="A10" s="1" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="B10" s="21" t="s">
         <v>28</v>
       </c>
       <c r="C10" s="12" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="D10" s="12" t="s">
         <v>119</v>
@@ -2447,19 +2461,19 @@
         <v>250</v>
       </c>
       <c r="G10" t="str">
-        <f>IF(B10="inspire",INSPIRE,IMKL) &amp; F10 &amp; "/" &amp; D10</f>
+        <f t="shared" si="0"/>
         <v>http://inspire.ec.europa.eu/codelist/ConditionOfFacilityValue/projected</v>
       </c>
     </row>
     <row r="11" spans="1:7" s="1" customFormat="1">
       <c r="A11" s="1" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="B11" s="21" t="s">
         <v>28</v>
       </c>
       <c r="C11" s="12" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="D11" s="12" t="s">
         <v>120</v>
@@ -2469,13 +2483,13 @@
         <v>250</v>
       </c>
       <c r="G11" t="str">
-        <f>IF(B11="inspire",INSPIRE,IMKL) &amp; F11 &amp; "/" &amp; D11</f>
+        <f t="shared" si="0"/>
         <v>http://inspire.ec.europa.eu/codelist/ConditionOfFacilityValue/disused</v>
       </c>
     </row>
     <row r="12" spans="1:7" s="1" customFormat="1" ht="15" customHeight="1">
       <c r="A12" s="1" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="B12" s="12" t="s">
         <v>82</v>
@@ -2490,13 +2504,13 @@
         <v>251</v>
       </c>
       <c r="G12" t="str">
-        <f>IF(B12="inspire",INSPIRE,IMKL) &amp; F12 &amp; "/" &amp; D12</f>
+        <f t="shared" si="0"/>
         <v>http://www.geonovum.nl/imkl2015/1.0/def/NauwkeurigheidDiepteValue/tot30cm</v>
       </c>
     </row>
     <row r="13" spans="1:7" s="1" customFormat="1" ht="15.75" customHeight="1">
       <c r="A13" s="1" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="B13" s="12" t="s">
         <v>82</v>
@@ -2511,13 +2525,13 @@
         <v>251</v>
       </c>
       <c r="G13" t="str">
-        <f>IF(B13="inspire",INSPIRE,IMKL) &amp; F13 &amp; "/" &amp; D13</f>
+        <f t="shared" si="0"/>
         <v>http://www.geonovum.nl/imkl2015/1.0/def/NauwkeurigheidDiepteValue/tot50cm</v>
       </c>
     </row>
     <row r="14" spans="1:7" s="1" customFormat="1" ht="15.75" customHeight="1">
       <c r="A14" s="1" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="B14" s="12" t="s">
         <v>82</v>
@@ -2532,13 +2546,13 @@
         <v>251</v>
       </c>
       <c r="G14" t="str">
-        <f>IF(B14="inspire",INSPIRE,IMKL) &amp; F14 &amp; "/" &amp; D14</f>
+        <f t="shared" si="0"/>
         <v>http://www.geonovum.nl/imkl2015/1.0/def/NauwkeurigheidDiepteValue/tot100cm</v>
       </c>
     </row>
     <row r="15" spans="1:7" s="1" customFormat="1" ht="14.25" customHeight="1">
       <c r="A15" s="1" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="B15" s="12" t="s">
         <v>82</v>
@@ -2553,13 +2567,13 @@
         <v>251</v>
       </c>
       <c r="G15" t="str">
-        <f>IF(B15="inspire",INSPIRE,IMKL) &amp; F15 &amp; "/" &amp; D15</f>
+        <f t="shared" si="0"/>
         <v>http://www.geonovum.nl/imkl2015/1.0/def/NauwkeurigheidDiepteValue/onbekend</v>
       </c>
     </row>
     <row r="16" spans="1:7" s="1" customFormat="1">
       <c r="A16" s="1" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="B16" s="12" t="s">
         <v>103</v>
@@ -2574,13 +2588,13 @@
         <v>252</v>
       </c>
       <c r="G16" t="str">
-        <f>IF(B16="inspire",INSPIRE,IMKL) &amp; F16 &amp; "/" &amp; D16</f>
+        <f t="shared" si="0"/>
         <v>http://www.geonovum.nl/imkl2015/1.0/def/ExtraDetailInfoTypeValue/huisaansluiting</v>
       </c>
     </row>
     <row r="17" spans="1:7" s="1" customFormat="1">
       <c r="A17" s="1" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="B17" s="12" t="s">
         <v>103</v>
@@ -2595,13 +2609,13 @@
         <v>252</v>
       </c>
       <c r="G17" t="str">
-        <f>IF(B17="inspire",INSPIRE,IMKL) &amp; F17 &amp; "/" &amp; D17</f>
+        <f t="shared" si="0"/>
         <v>http://www.geonovum.nl/imkl2015/1.0/def/ExtraDetailInfoTypeValue/lengteprofiel</v>
       </c>
     </row>
     <row r="18" spans="1:7" s="1" customFormat="1">
       <c r="A18" s="1" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="B18" s="12" t="s">
         <v>103</v>
@@ -2616,13 +2630,13 @@
         <v>252</v>
       </c>
       <c r="G18" t="str">
-        <f>IF(B18="inspire",INSPIRE,IMKL) &amp; F18 &amp; "/" &amp; D18</f>
+        <f t="shared" si="0"/>
         <v>http://www.geonovum.nl/imkl2015/1.0/def/ExtraDetailInfoTypeValue/gestuurdeBoring</v>
       </c>
     </row>
     <row r="19" spans="1:7" s="1" customFormat="1">
       <c r="A19" s="1" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="B19" s="12" t="s">
         <v>103</v>
@@ -2637,13 +2651,13 @@
         <v>252</v>
       </c>
       <c r="G19" t="str">
-        <f>IF(B19="inspire",INSPIRE,IMKL) &amp; F19 &amp; "/" &amp; D19</f>
+        <f t="shared" si="0"/>
         <v>http://www.geonovum.nl/imkl2015/1.0/def/ExtraDetailInfoTypeValue/dwarsprofiel</v>
       </c>
     </row>
     <row r="20" spans="1:7" s="1" customFormat="1" ht="12.75" customHeight="1">
       <c r="A20" s="1" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="B20" s="12" t="s">
         <v>82</v>
@@ -2655,16 +2669,16 @@
         <v>89</v>
       </c>
       <c r="F20" s="9" t="s">
-        <v>357</v>
+        <v>382</v>
       </c>
       <c r="G20" t="str">
-        <f>IF(B20="inspire",INSPIRE,IMKL) &amp; F20 &amp; "/" &amp; D20</f>
-        <v>http://www.geonovum.nl/imkl2015/1.0/def/imkl:extraTopografieTypeValue/eigen</v>
+        <f t="shared" si="0"/>
+        <v>http://www.geonovum.nl/imkl2015/1.0/def/ExtraTopografieTypeValue/eigen</v>
       </c>
     </row>
     <row r="21" spans="1:7" s="1" customFormat="1">
       <c r="A21" s="1" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="B21" s="12" t="s">
         <v>82</v>
@@ -2676,16 +2690,16 @@
         <v>90</v>
       </c>
       <c r="F21" s="9" t="s">
-        <v>357</v>
+        <v>382</v>
       </c>
       <c r="G21" t="str">
-        <f>IF(B21="inspire",INSPIRE,IMKL) &amp; F21 &amp; "/" &amp; D21</f>
-        <v>http://www.geonovum.nl/imkl2015/1.0/def/imkl:extraTopografieTypeValue/ontwerp</v>
+        <f t="shared" si="0"/>
+        <v>http://www.geonovum.nl/imkl2015/1.0/def/ExtraTopografieTypeValue/ontwerp</v>
       </c>
     </row>
     <row r="22" spans="1:7" s="1" customFormat="1" ht="14.25" customHeight="1">
       <c r="A22" s="1" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="B22" s="12" t="s">
         <v>82</v>
@@ -2700,13 +2714,13 @@
         <v>253</v>
       </c>
       <c r="G22" t="str">
-        <f>IF(B22="inspire",INSPIRE,IMKL) &amp; F22 &amp; "/" &amp; D22</f>
+        <f t="shared" si="0"/>
         <v>http://www.geonovum.nl/imkl2015/1.0/def/NauwkeurigheidXYvalue/tot30cm</v>
       </c>
     </row>
     <row r="23" spans="1:7" s="1" customFormat="1" ht="14.25" customHeight="1">
       <c r="A23" s="1" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="B23" s="12" t="s">
         <v>82</v>
@@ -2721,13 +2735,13 @@
         <v>253</v>
       </c>
       <c r="G23" t="str">
-        <f>IF(B23="inspire",INSPIRE,IMKL) &amp; F23 &amp; "/" &amp; D23</f>
+        <f t="shared" si="0"/>
         <v>http://www.geonovum.nl/imkl2015/1.0/def/NauwkeurigheidXYvalue/tot50cm</v>
       </c>
     </row>
     <row r="24" spans="1:7" s="1" customFormat="1">
       <c r="A24" s="1" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="B24" s="12" t="s">
         <v>82</v>
@@ -2742,104 +2756,104 @@
         <v>253</v>
       </c>
       <c r="G24" t="str">
-        <f>IF(B24="inspire",INSPIRE,IMKL) &amp; F24 &amp; "/" &amp; D24</f>
+        <f t="shared" si="0"/>
         <v>http://www.geonovum.nl/imkl2015/1.0/def/NauwkeurigheidXYvalue/tot100cm</v>
       </c>
     </row>
     <row r="25" spans="1:7" s="1" customFormat="1">
       <c r="A25" s="1" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="B25" s="21" t="s">
         <v>206</v>
       </c>
       <c r="C25" s="12" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="D25" s="12" t="s">
         <v>233</v>
       </c>
       <c r="F25" s="9" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="G25" t="str">
-        <f>IF(B25="inspire",INSPIRE,IMKL) &amp; F25 &amp; "/" &amp; D25</f>
+        <f t="shared" si="0"/>
         <v>http://www.geonovum.nl/imkl2015/1.0/def/MaatvoeringsTypeValue/maatvoeringshulplijn</v>
       </c>
     </row>
     <row r="26" spans="1:7" s="1" customFormat="1">
       <c r="A26" s="1" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="B26" s="21" t="s">
         <v>206</v>
       </c>
       <c r="C26" s="12" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="D26" s="12" t="s">
         <v>231</v>
       </c>
       <c r="F26" s="9" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="G26" t="str">
-        <f>IF(B26="inspire",INSPIRE,IMKL) &amp; F26 &amp; "/" &amp; D26</f>
+        <f t="shared" si="0"/>
         <v>http://www.geonovum.nl/imkl2015/1.0/def/MaatvoeringsTypeValue/maatvoeringslijn</v>
       </c>
     </row>
     <row r="27" spans="1:7" s="1" customFormat="1">
       <c r="A27" s="1" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="B27" s="21" t="s">
         <v>206</v>
       </c>
       <c r="C27" s="12" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="D27" s="21" t="s">
         <v>230</v>
       </c>
       <c r="F27" s="9" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="G27" t="str">
-        <f>IF(B27="inspire",INSPIRE,IMKL) &amp; F27 &amp; "/" &amp; D27</f>
+        <f t="shared" si="0"/>
         <v>http://www.geonovum.nl/imkl2015/1.0/def/MaatvoeringsTypeValue/maatvoeringspijl</v>
       </c>
     </row>
     <row r="28" spans="1:7">
       <c r="A28" s="1" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="B28" s="21" t="s">
         <v>206</v>
       </c>
       <c r="C28" s="12" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="D28" s="12" t="s">
         <v>232</v>
       </c>
       <c r="E28" s="1"/>
       <c r="F28" s="9" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="G28" t="str">
-        <f>IF(B28="inspire",INSPIRE,IMKL) &amp; F28 &amp; "/" &amp; D28</f>
+        <f t="shared" si="0"/>
         <v>http://www.geonovum.nl/imkl2015/1.0/def/MaatvoeringsTypeValue/maatvoeringslabel</v>
       </c>
     </row>
     <row r="29" spans="1:7">
       <c r="A29" s="1" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="B29" s="12" t="s">
         <v>103</v>
       </c>
       <c r="C29" s="12" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="D29" s="12" t="s">
         <v>282</v>
@@ -2851,19 +2865,19 @@
         <v>254</v>
       </c>
       <c r="G29" t="str">
-        <f>IF(B29="inspire",INSPIRE,IMKL) &amp; F29 &amp; "/" &amp; D29</f>
+        <f t="shared" si="0"/>
         <v>http://www.geonovum.nl/imkl2015/1.0/def/Thema/buisleidingGevaarlijkeInhoud</v>
       </c>
     </row>
     <row r="30" spans="1:7">
       <c r="A30" s="1" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="B30" s="12" t="s">
         <v>103</v>
       </c>
       <c r="C30" s="12" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="D30" s="12" t="s">
         <v>121</v>
@@ -2872,19 +2886,19 @@
         <v>254</v>
       </c>
       <c r="G30" t="str">
-        <f>IF(B30="inspire",INSPIRE,IMKL) &amp; F30 &amp; "/" &amp; D30</f>
+        <f t="shared" si="0"/>
         <v>http://www.geonovum.nl/imkl2015/1.0/def/Thema/datatransport</v>
       </c>
     </row>
     <row r="31" spans="1:7">
       <c r="A31" s="1" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="B31" s="12" t="s">
         <v>103</v>
       </c>
       <c r="C31" s="12" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="D31" s="12" t="s">
         <v>284</v>
@@ -2896,19 +2910,19 @@
         <v>254</v>
       </c>
       <c r="G31" t="str">
-        <f>IF(B31="inspire",INSPIRE,IMKL) &amp; F31 &amp; "/" &amp; D31</f>
+        <f t="shared" si="0"/>
         <v>http://www.geonovum.nl/imkl2015/1.0/def/Thema/gasLageDruk</v>
       </c>
     </row>
     <row r="32" spans="1:7">
       <c r="A32" s="1" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="B32" s="12" t="s">
         <v>103</v>
       </c>
       <c r="C32" s="12" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="D32" s="12" t="s">
         <v>285</v>
@@ -2920,19 +2934,19 @@
         <v>254</v>
       </c>
       <c r="G32" t="str">
-        <f>IF(B32="inspire",INSPIRE,IMKL) &amp; F32 &amp; "/" &amp; D32</f>
+        <f t="shared" si="0"/>
         <v>http://www.geonovum.nl/imkl2015/1.0/def/Thema/gasHogeDruk</v>
       </c>
     </row>
     <row r="33" spans="1:7">
       <c r="A33" s="1" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="B33" s="12" t="s">
         <v>103</v>
       </c>
       <c r="C33" s="12" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="D33" s="12" t="s">
         <v>286</v>
@@ -2944,19 +2958,19 @@
         <v>254</v>
       </c>
       <c r="G33" t="str">
-        <f>IF(B33="inspire",INSPIRE,IMKL) &amp; F33 &amp; "/" &amp; D33</f>
+        <f t="shared" si="0"/>
         <v>http://www.geonovum.nl/imkl2015/1.0/def/Thema/petrochemie</v>
       </c>
     </row>
     <row r="34" spans="1:7">
       <c r="A34" s="1" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="B34" s="12" t="s">
         <v>103</v>
       </c>
       <c r="C34" s="12" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="D34" s="12" t="s">
         <v>283</v>
@@ -2968,19 +2982,19 @@
         <v>254</v>
       </c>
       <c r="G34" t="str">
-        <f>IF(B34="inspire",INSPIRE,IMKL) &amp; F34 &amp; "/" &amp; D34</f>
+        <f t="shared" si="0"/>
         <v>http://www.geonovum.nl/imkl2015/1.0/def/Thema/landelijkHoogspanningsnet</v>
       </c>
     </row>
     <row r="35" spans="1:7">
       <c r="A35" s="1" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="B35" s="12" t="s">
         <v>103</v>
       </c>
       <c r="C35" s="12" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="D35" s="12" t="s">
         <v>126</v>
@@ -2992,19 +3006,19 @@
         <v>254</v>
       </c>
       <c r="G35" t="str">
-        <f>IF(B35="inspire",INSPIRE,IMKL) &amp; F35 &amp; "/" &amp; D35</f>
+        <f t="shared" si="0"/>
         <v>http://www.geonovum.nl/imkl2015/1.0/def/Thema/hoogspanning</v>
       </c>
     </row>
     <row r="36" spans="1:7">
       <c r="A36" s="1" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="B36" s="12" t="s">
         <v>103</v>
       </c>
       <c r="C36" s="12" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="D36" s="12" t="s">
         <v>127</v>
@@ -3016,19 +3030,19 @@
         <v>254</v>
       </c>
       <c r="G36" t="str">
-        <f>IF(B36="inspire",INSPIRE,IMKL) &amp; F36 &amp; "/" &amp; D36</f>
+        <f t="shared" si="0"/>
         <v>http://www.geonovum.nl/imkl2015/1.0/def/Thema/laagspanning</v>
       </c>
     </row>
     <row r="37" spans="1:7">
       <c r="A37" s="1" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="B37" s="12" t="s">
         <v>103</v>
       </c>
       <c r="C37" s="12" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="D37" s="12" t="s">
         <v>128</v>
@@ -3040,22 +3054,22 @@
         <v>254</v>
       </c>
       <c r="G37" t="str">
-        <f>IF(B37="inspire",INSPIRE,IMKL) &amp; F37 &amp; "/" &amp; D37</f>
+        <f t="shared" si="0"/>
         <v>http://www.geonovum.nl/imkl2015/1.0/def/Thema/middenspanning</v>
       </c>
     </row>
     <row r="38" spans="1:7">
       <c r="A38" s="1" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="B38" s="12" t="s">
         <v>103</v>
       </c>
       <c r="C38" s="12" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="D38" s="12" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="E38" s="12" t="s">
         <v>129</v>
@@ -3064,22 +3078,22 @@
         <v>254</v>
       </c>
       <c r="G38" t="str">
-        <f>IF(B38="inspire",INSPIRE,IMKL) &amp; F38 &amp; "/" &amp; D38</f>
+        <f t="shared" si="0"/>
         <v>http://www.geonovum.nl/imkl2015/1.0/def/Thema/rioolVrijverval</v>
       </c>
     </row>
     <row r="39" spans="1:7">
       <c r="A39" s="1" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="B39" s="12" t="s">
         <v>103</v>
       </c>
       <c r="C39" s="12" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="D39" s="12" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="E39" s="12" t="s">
         <v>130</v>
@@ -3088,19 +3102,19 @@
         <v>254</v>
       </c>
       <c r="G39" t="str">
-        <f>IF(B39="inspire",INSPIRE,IMKL) &amp; F39 &amp; "/" &amp; D39</f>
+        <f t="shared" si="0"/>
         <v>http://www.geonovum.nl/imkl2015/1.0/def/Thema/rioolOnderDruk</v>
       </c>
     </row>
     <row r="40" spans="1:7">
       <c r="A40" s="1" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="B40" s="12" t="s">
         <v>103</v>
       </c>
       <c r="C40" s="12" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="D40" s="12" t="s">
         <v>131</v>
@@ -3112,19 +3126,19 @@
         <v>254</v>
       </c>
       <c r="G40" t="str">
-        <f>IF(B40="inspire",INSPIRE,IMKL) &amp; F40 &amp; "/" &amp; D40</f>
+        <f t="shared" si="0"/>
         <v>http://www.geonovum.nl/imkl2015/1.0/def/Thema/warmte</v>
       </c>
     </row>
     <row r="41" spans="1:7">
       <c r="A41" s="1" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="B41" s="12" t="s">
         <v>103</v>
       </c>
       <c r="C41" s="12" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="D41" s="12" t="s">
         <v>114</v>
@@ -3136,19 +3150,19 @@
         <v>254</v>
       </c>
       <c r="G41" t="str">
-        <f>IF(B41="inspire",INSPIRE,IMKL) &amp; F41 &amp; "/" &amp; D41</f>
+        <f t="shared" si="0"/>
         <v>http://www.geonovum.nl/imkl2015/1.0/def/Thema/water</v>
       </c>
     </row>
     <row r="42" spans="1:7">
       <c r="A42" s="1" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="B42" s="12" t="s">
         <v>103</v>
       </c>
       <c r="C42" s="12" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="D42" s="12" t="s">
         <v>133</v>
@@ -3160,19 +3174,19 @@
         <v>254</v>
       </c>
       <c r="G42" t="str">
-        <f>IF(B42="inspire",INSPIRE,IMKL) &amp; F42 &amp; "/" &amp; D42</f>
+        <f t="shared" si="0"/>
         <v>http://www.geonovum.nl/imkl2015/1.0/def/Thema/wees</v>
       </c>
     </row>
     <row r="43" spans="1:7">
       <c r="A43" s="1" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="B43" s="12" t="s">
         <v>103</v>
       </c>
       <c r="C43" s="12" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="D43" s="12" t="s">
         <v>134</v>
@@ -3184,13 +3198,13 @@
         <v>254</v>
       </c>
       <c r="G43" t="str">
-        <f>IF(B43="inspire",INSPIRE,IMKL) &amp; F43 &amp; "/" &amp; D43</f>
+        <f t="shared" si="0"/>
         <v>http://www.geonovum.nl/imkl2015/1.0/def/Thema/overig</v>
       </c>
     </row>
     <row r="44" spans="1:7">
       <c r="A44" s="1" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="B44" s="21" t="s">
         <v>28</v>
@@ -3205,13 +3219,13 @@
         <v>255</v>
       </c>
       <c r="G44" t="str">
-        <f>IF(B44="inspire",INSPIRE,IMKL) &amp; F44 &amp; "/" &amp; D44</f>
+        <f t="shared" si="0"/>
         <v>http://inspire.ec.europa.eu/codelist/UtilityDeliveryTypeValue/collection</v>
       </c>
     </row>
     <row r="45" spans="1:7">
       <c r="A45" s="1" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="B45" s="21" t="s">
         <v>28</v>
@@ -3226,13 +3240,13 @@
         <v>255</v>
       </c>
       <c r="G45" t="str">
-        <f>IF(B45="inspire",INSPIRE,IMKL) &amp; F45 &amp; "/" &amp; D45</f>
+        <f t="shared" si="0"/>
         <v>http://inspire.ec.europa.eu/codelist/UtilityDeliveryTypeValue/distribution</v>
       </c>
     </row>
     <row r="46" spans="1:7">
       <c r="A46" s="1" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="B46" s="21" t="s">
         <v>28</v>
@@ -3247,13 +3261,13 @@
         <v>255</v>
       </c>
       <c r="G46" t="str">
-        <f>IF(B46="inspire",INSPIRE,IMKL) &amp; F46 &amp; "/" &amp; D46</f>
+        <f t="shared" si="0"/>
         <v>http://inspire.ec.europa.eu/codelist/UtilityDeliveryTypeValue/private</v>
       </c>
     </row>
     <row r="47" spans="1:7">
       <c r="A47" s="1" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="B47" s="21" t="s">
         <v>28</v>
@@ -3268,19 +3282,19 @@
         <v>255</v>
       </c>
       <c r="G47" t="str">
-        <f>IF(B47="inspire",INSPIRE,IMKL) &amp; F47 &amp; "/" &amp; D47</f>
+        <f t="shared" si="0"/>
         <v>http://inspire.ec.europa.eu/codelist/UtilityDeliveryTypeValue/transport</v>
       </c>
     </row>
     <row r="48" spans="1:7">
       <c r="A48" s="1" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="B48" s="21" t="s">
         <v>28</v>
       </c>
       <c r="C48" s="12" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="D48" s="12" t="s">
         <v>112</v>
@@ -3289,40 +3303,40 @@
         <v>256</v>
       </c>
       <c r="G48" t="str">
-        <f>IF(B48="inspire",INSPIRE,IMKL) &amp; F48 &amp; "/" &amp; D48</f>
+        <f t="shared" si="0"/>
         <v>http://inspire.ec.europa.eu/codelist/UtilityNetworkTypeValue/electricity</v>
       </c>
     </row>
     <row r="49" spans="1:7">
       <c r="A49" s="1" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="B49" s="21" t="s">
         <v>28</v>
       </c>
       <c r="C49" s="12" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="D49" s="12" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="F49" s="9" t="s">
         <v>256</v>
       </c>
       <c r="G49" t="str">
-        <f>IF(B49="inspire",INSPIRE,IMKL) &amp; F49 &amp; "/" &amp; D49</f>
+        <f t="shared" si="0"/>
         <v>http://inspire.ec.europa.eu/codelist/UtilityNetworkTypeValue/oilGasChemical</v>
       </c>
     </row>
     <row r="50" spans="1:7">
       <c r="A50" s="1" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="B50" s="21" t="s">
         <v>28</v>
       </c>
       <c r="C50" s="12" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="D50" s="12" t="s">
         <v>113</v>
@@ -3331,19 +3345,19 @@
         <v>256</v>
       </c>
       <c r="G50" t="str">
-        <f>IF(B50="inspire",INSPIRE,IMKL) &amp; F50 &amp; "/" &amp; D50</f>
+        <f t="shared" si="0"/>
         <v>http://inspire.ec.europa.eu/codelist/UtilityNetworkTypeValue/sewer</v>
       </c>
     </row>
     <row r="51" spans="1:7">
       <c r="A51" s="1" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="B51" s="21" t="s">
         <v>28</v>
       </c>
       <c r="C51" s="12" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="D51" s="12" t="s">
         <v>114</v>
@@ -3352,19 +3366,19 @@
         <v>256</v>
       </c>
       <c r="G51" t="str">
-        <f>IF(B51="inspire",INSPIRE,IMKL) &amp; F51 &amp; "/" &amp; D51</f>
+        <f t="shared" si="0"/>
         <v>http://inspire.ec.europa.eu/codelist/UtilityNetworkTypeValue/water</v>
       </c>
     </row>
     <row r="52" spans="1:7">
       <c r="A52" s="1" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="B52" s="21" t="s">
         <v>28</v>
       </c>
       <c r="C52" s="12" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="D52" s="12" t="s">
         <v>115</v>
@@ -3373,19 +3387,19 @@
         <v>256</v>
       </c>
       <c r="G52" t="str">
-        <f>IF(B52="inspire",INSPIRE,IMKL) &amp; F52 &amp; "/" &amp; D52</f>
+        <f t="shared" si="0"/>
         <v>http://inspire.ec.europa.eu/codelist/UtilityNetworkTypeValue/thermal</v>
       </c>
     </row>
     <row r="53" spans="1:7">
       <c r="A53" s="1" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="B53" s="21" t="s">
         <v>28</v>
       </c>
       <c r="C53" s="12" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="D53" s="12" t="s">
         <v>116</v>
@@ -3394,19 +3408,19 @@
         <v>256</v>
       </c>
       <c r="G53" t="str">
-        <f>IF(B53="inspire",INSPIRE,IMKL) &amp; F53 &amp; "/" &amp; D53</f>
+        <f t="shared" si="0"/>
         <v>http://inspire.ec.europa.eu/codelist/UtilityNetworkTypeValue/telecommunications</v>
       </c>
     </row>
     <row r="54" spans="1:7">
       <c r="A54" s="1" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="B54" s="21" t="s">
         <v>28</v>
       </c>
       <c r="C54" s="12" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="D54" s="12" t="s">
         <v>117</v>
@@ -3415,13 +3429,13 @@
         <v>256</v>
       </c>
       <c r="G54" t="str">
-        <f>IF(B54="inspire",INSPIRE,IMKL) &amp; F54 &amp; "/" &amp; D54</f>
+        <f t="shared" si="0"/>
         <v>http://inspire.ec.europa.eu/codelist/UtilityNetworkTypeValue/crossTheme</v>
       </c>
     </row>
     <row r="55" spans="1:7">
       <c r="A55" s="1" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="B55" s="21" t="s">
         <v>28</v>
@@ -3436,13 +3450,13 @@
         <v>257</v>
       </c>
       <c r="G55" t="str">
-        <f>IF(B55="inspire",INSPIRE,IMKL) &amp; F55 &amp; "/" &amp; D55</f>
+        <f t="shared" si="0"/>
         <v>http://inspire.ec.europa.eu/codelist/WarningTypeValue/net</v>
       </c>
     </row>
     <row r="56" spans="1:7">
       <c r="A56" s="1" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="B56" s="21" t="s">
         <v>28</v>
@@ -3457,13 +3471,13 @@
         <v>257</v>
       </c>
       <c r="G56" t="str">
-        <f>IF(B56="inspire",INSPIRE,IMKL) &amp; F56 &amp; "/" &amp; D56</f>
+        <f t="shared" si="0"/>
         <v>http://inspire.ec.europa.eu/codelist/WarningTypeValue/tape</v>
       </c>
     </row>
     <row r="57" spans="1:7" ht="15" thickBot="1">
       <c r="A57" s="1" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="B57" s="21" t="s">
         <v>28</v>
@@ -3478,13 +3492,13 @@
         <v>257</v>
       </c>
       <c r="G57" t="str">
-        <f>IF(B57="inspire",INSPIRE,IMKL) &amp; F57 &amp; "/" &amp; D57</f>
+        <f t="shared" si="0"/>
         <v>http://inspire.ec.europa.eu/codelist/WarningTypeValue/concretePaving</v>
       </c>
     </row>
     <row r="58" spans="1:7" ht="15" thickBot="1">
       <c r="A58" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="B58" s="12" t="s">
         <v>82</v>
@@ -3502,13 +3516,13 @@
         <v>258</v>
       </c>
       <c r="G58" t="str">
-        <f>IF(B58="inspire",INSPIRE,IMKL) &amp; F58 &amp; "/" &amp; D58</f>
+        <f t="shared" si="0"/>
         <v>http://www.geonovum.nl/imkl2015/1.0/def/ElectricityAppurtenanceTypeIMKLValue/aarding</v>
       </c>
     </row>
     <row r="59" spans="1:7" ht="15" thickBot="1">
       <c r="A59" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="B59" s="12" t="s">
         <v>82</v>
@@ -3526,13 +3540,13 @@
         <v>258</v>
       </c>
       <c r="G59" t="str">
-        <f>IF(B59="inspire",INSPIRE,IMKL) &amp; F59 &amp; "/" &amp; D59</f>
+        <f t="shared" si="0"/>
         <v>http://www.geonovum.nl/imkl2015/1.0/def/ElectricityAppurtenanceTypeIMKLValue/mof</v>
       </c>
     </row>
     <row r="60" spans="1:7" ht="15" thickBot="1">
       <c r="A60" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="B60" s="12" t="s">
         <v>206</v>
@@ -3550,13 +3564,13 @@
         <v>258</v>
       </c>
       <c r="G60" t="str">
-        <f>IF(B60="inspire",INSPIRE,IMKL) &amp; F60 &amp; "/" &amp; D60</f>
+        <f t="shared" si="0"/>
         <v>http://www.geonovum.nl/imkl2015/1.0/def/ElectricityAppurtenanceTypeIMKLValue/hoogteligging</v>
       </c>
     </row>
     <row r="61" spans="1:7" ht="15" thickBot="1">
       <c r="A61" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="B61" s="12" t="s">
         <v>207</v>
@@ -3574,13 +3588,13 @@
         <v>258</v>
       </c>
       <c r="G61" t="str">
-        <f>IF(B61="inspire",INSPIRE,IMKL) &amp; F61 &amp; "/" &amp; D61</f>
+        <f t="shared" si="0"/>
         <v>http://www.geonovum.nl/imkl2015/1.0/def/ElectricityAppurtenanceTypeIMKLValue/Adrespunt</v>
       </c>
     </row>
     <row r="62" spans="1:7" ht="15" thickBot="1">
       <c r="A62" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="B62" s="13" t="s">
         <v>28</v>
@@ -3589,22 +3603,22 @@
         <v>348</v>
       </c>
       <c r="D62" s="16" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="E62" s="16" t="s">
         <v>3</v>
       </c>
       <c r="F62" s="8" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="G62" t="str">
-        <f>IF(B62="inspire",INSPIRE,IMKL) &amp; F62 &amp; "/" &amp; D62</f>
+        <f t="shared" si="0"/>
         <v>http://inspire.ec.europa.eu/codelist/ElectricityAppurtenanceTypeValue/connectionBox</v>
       </c>
     </row>
     <row r="63" spans="1:7" ht="15" thickBot="1">
       <c r="A63" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="B63" s="13" t="s">
         <v>28</v>
@@ -3619,16 +3633,16 @@
         <v>5</v>
       </c>
       <c r="F63" s="8" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="G63" t="str">
-        <f>IF(B63="inspire",INSPIRE,IMKL) &amp; F63 &amp; "/" &amp; D63</f>
+        <f t="shared" si="0"/>
         <v>http://inspire.ec.europa.eu/codelist/ElectricityAppurtenanceTypeValue/mainStation</v>
       </c>
     </row>
     <row r="64" spans="1:7" ht="15" thickBot="1">
       <c r="A64" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="B64" s="13" t="s">
         <v>28</v>
@@ -3643,16 +3657,16 @@
         <v>12</v>
       </c>
       <c r="F64" s="8" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="G64" t="str">
-        <f>IF(B64="inspire",INSPIRE,IMKL) &amp; F64 &amp; "/" &amp; D64</f>
+        <f t="shared" si="0"/>
         <v>http://inspire.ec.europa.eu/codelist/ElectricityAppurtenanceTypeValue/generator</v>
       </c>
     </row>
     <row r="65" spans="1:7" ht="15" thickBot="1">
       <c r="A65" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="B65" s="13" t="s">
         <v>28</v>
@@ -3667,16 +3681,16 @@
         <v>17</v>
       </c>
       <c r="F65" s="8" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="G65" t="str">
-        <f>IF(B65="inspire",INSPIRE,IMKL) &amp; F65 &amp; "/" &amp; D65</f>
+        <f t="shared" si="0"/>
         <v>http://inspire.ec.europa.eu/codelist/ElectricityAppurtenanceTypeValue/netStation</v>
       </c>
     </row>
     <row r="66" spans="1:7" ht="15" thickBot="1">
       <c r="A66" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="B66" s="13" t="s">
         <v>28</v>
@@ -3691,16 +3705,16 @@
         <v>18</v>
       </c>
       <c r="F66" s="8" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="G66" t="str">
-        <f>IF(B66="inspire",INSPIRE,IMKL) &amp; F66 &amp; "/" &amp; D66</f>
+        <f t="shared" ref="G66:G129" si="1">IF(B66="inspire",INSPIRE,IMKL) &amp; F66 &amp; "/" &amp; D66</f>
         <v>http://inspire.ec.europa.eu/codelist/ElectricityAppurtenanceTypeValue/subStation</v>
       </c>
     </row>
     <row r="67" spans="1:7" ht="15" thickBot="1">
       <c r="A67" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="B67" s="13" t="s">
         <v>28</v>
@@ -3715,16 +3729,16 @@
         <v>21</v>
       </c>
       <c r="F67" s="8" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="G67" t="str">
-        <f>IF(B67="inspire",INSPIRE,IMKL) &amp; F67 &amp; "/" &amp; D67</f>
+        <f t="shared" si="1"/>
         <v>http://inspire.ec.europa.eu/codelist/ElectricityAppurtenanceTypeValue/deliveryPoint</v>
       </c>
     </row>
     <row r="68" spans="1:7" ht="15" thickBot="1">
       <c r="A68" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="B68" s="13" t="s">
         <v>28</v>
@@ -3739,16 +3753,16 @@
         <v>26</v>
       </c>
       <c r="F68" s="8" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="G68" t="str">
-        <f>IF(B68="inspire",INSPIRE,IMKL) &amp; F68 &amp; "/" &amp; D68</f>
+        <f t="shared" si="1"/>
         <v>http://inspire.ec.europa.eu/codelist/ElectricityAppurtenanceTypeValue/streetLight</v>
       </c>
     </row>
     <row r="69" spans="1:7" ht="15" thickBot="1">
       <c r="A69" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="C69" s="13" t="s">
         <v>348</v>
@@ -3763,13 +3777,13 @@
         <v>258</v>
       </c>
       <c r="G69" t="str">
-        <f>IF(B69="inspire",INSPIRE,IMKL) &amp; F69 &amp; "/" &amp; D69</f>
+        <f t="shared" si="1"/>
         <v>http://www.geonovum.nl/imkl2015/1.0/def/ElectricityAppurtenanceTypeIMKLValue/puntVanLevering</v>
       </c>
     </row>
     <row r="70" spans="1:7" ht="15" thickBot="1">
       <c r="A70" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="C70" s="13" t="s">
         <v>348</v>
@@ -3784,13 +3798,13 @@
         <v>258</v>
       </c>
       <c r="G70" t="str">
-        <f>IF(B70="inspire",INSPIRE,IMKL) &amp; F70 &amp; "/" &amp; D70</f>
+        <f t="shared" si="1"/>
         <v>http://www.geonovum.nl/imkl2015/1.0/def/ElectricityAppurtenanceTypeIMKLValue/geulmof</v>
       </c>
     </row>
     <row r="71" spans="1:7">
       <c r="A71" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="B71" s="32" t="s">
         <v>206</v>
@@ -3808,13 +3822,13 @@
         <v>258</v>
       </c>
       <c r="G71" t="str">
-        <f>IF(B71="inspire",INSPIRE,IMKL) &amp; F71 &amp; "/" &amp; D71</f>
+        <f t="shared" si="1"/>
         <v>http://www.geonovum.nl/imkl2015/1.0/def/ElectricityAppurtenanceTypeIMKLValue/kbMeetpunt</v>
       </c>
     </row>
     <row r="72" spans="1:7">
       <c r="A72" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="B72" s="32" t="s">
         <v>206</v>
@@ -3832,13 +3846,13 @@
         <v>258</v>
       </c>
       <c r="G72" t="str">
-        <f>IF(B72="inspire",INSPIRE,IMKL) &amp; F72 &amp; "/" &amp; D72</f>
+        <f t="shared" si="1"/>
         <v>http://www.geonovum.nl/imkl2015/1.0/def/ElectricityAppurtenanceTypeIMKLValue/kbInstallatie</v>
       </c>
     </row>
     <row r="73" spans="1:7">
       <c r="A73" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="B73" s="32" t="s">
         <v>206</v>
@@ -3856,13 +3870,13 @@
         <v>258</v>
       </c>
       <c r="G73" t="str">
-        <f>IF(B73="inspire",INSPIRE,IMKL) &amp; F73 &amp; "/" &amp; D73</f>
+        <f t="shared" si="1"/>
         <v>http://www.geonovum.nl/imkl2015/1.0/def/ElectricityAppurtenanceTypeIMKLValue/kbEindpunt</v>
       </c>
     </row>
     <row r="74" spans="1:7">
       <c r="A74" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="B74" s="32" t="s">
         <v>206</v>
@@ -3871,7 +3885,7 @@
         <v>348</v>
       </c>
       <c r="D74" s="29" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="E74" s="29" t="s">
         <v>276</v>
@@ -3880,13 +3894,13 @@
         <v>258</v>
       </c>
       <c r="G74" t="str">
-        <f>IF(B74="inspire",INSPIRE,IMKL) &amp; F74 &amp; "/" &amp; D74</f>
+        <f t="shared" si="1"/>
         <v>http://www.geonovum.nl/imkl2015/1.0/def/ElectricityAppurtenanceTypeIMKLValue/kbContact</v>
       </c>
     </row>
     <row r="75" spans="1:7" ht="15" thickBot="1">
       <c r="A75" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="B75" s="32" t="s">
         <v>206</v>
@@ -3904,13 +3918,13 @@
         <v>258</v>
       </c>
       <c r="G75" t="str">
-        <f>IF(B75="inspire",INSPIRE,IMKL) &amp; F75 &amp; "/" &amp; D75</f>
+        <f t="shared" si="1"/>
         <v>http://www.geonovum.nl/imkl2015/1.0/def/ElectricityAppurtenanceTypeIMKLValue/hoogbouwkoppelpunt</v>
       </c>
     </row>
     <row r="76" spans="1:7">
       <c r="A76" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="B76" s="13" t="s">
         <v>28</v>
@@ -3928,13 +3942,13 @@
         <v>259</v>
       </c>
       <c r="G76" t="str">
-        <f>IF(B76="inspire",INSPIRE,IMKL) &amp; F76 &amp; "/" &amp; D76</f>
+        <f t="shared" si="1"/>
         <v>http://inspire.ec.europa.eu/codelist/TelecommunicationsAppurtenanceIMKLTypeValue/antenna</v>
       </c>
     </row>
     <row r="77" spans="1:7">
       <c r="A77" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="B77" s="13" t="s">
         <v>28</v>
@@ -3952,13 +3966,13 @@
         <v>259</v>
       </c>
       <c r="G77" t="str">
-        <f>IF(B77="inspire",INSPIRE,IMKL) &amp; F77 &amp; "/" &amp; D77</f>
+        <f t="shared" si="1"/>
         <v>http://inspire.ec.europa.eu/codelist/TelecommunicationsAppurtenanceIMKLTypeValue/termination</v>
       </c>
     </row>
     <row r="78" spans="1:7">
       <c r="A78" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="B78" s="13" t="s">
         <v>206</v>
@@ -3976,13 +3990,13 @@
         <v>259</v>
       </c>
       <c r="G78" t="str">
-        <f>IF(B78="inspire",INSPIRE,IMKL) &amp; F78 &amp; "/" &amp; D78</f>
+        <f t="shared" si="1"/>
         <v>http://www.geonovum.nl/imkl2015/1.0/def/TelecommunicationsAppurtenanceIMKLTypeValue/handhole</v>
       </c>
     </row>
     <row r="79" spans="1:7">
       <c r="A79" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="B79" s="13" t="s">
         <v>206</v>
@@ -4000,13 +4014,13 @@
         <v>259</v>
       </c>
       <c r="G79" t="str">
-        <f>IF(B79="inspire",INSPIRE,IMKL) &amp; F79 &amp; "/" &amp; D79</f>
+        <f t="shared" si="1"/>
         <v>http://www.geonovum.nl/imkl2015/1.0/def/TelecommunicationsAppurtenanceIMKLTypeValue/mof</v>
       </c>
     </row>
     <row r="80" spans="1:7">
       <c r="A80" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="B80" s="13" t="s">
         <v>206</v>
@@ -4015,7 +4029,7 @@
         <v>348</v>
       </c>
       <c r="D80" s="13" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="E80" s="13" t="s">
         <v>191</v>
@@ -4024,13 +4038,13 @@
         <v>259</v>
       </c>
       <c r="G80" t="str">
-        <f>IF(B80="inspire",INSPIRE,IMKL) &amp; F80 &amp; "/" &amp; D80</f>
+        <f t="shared" si="1"/>
         <v>http://www.geonovum.nl/imkl2015/1.0/def/TelecommunicationsAppurtenanceIMKLTypeValue/verzameltermOndergrondseLeidingelementenOpnemen</v>
       </c>
     </row>
     <row r="81" spans="1:7">
       <c r="A81" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="B81" s="13" t="s">
         <v>206</v>
@@ -4048,13 +4062,13 @@
         <v>259</v>
       </c>
       <c r="G81" t="str">
-        <f>IF(B81="inspire",INSPIRE,IMKL) &amp; F81 &amp; "/" &amp; D81</f>
+        <f t="shared" si="1"/>
         <v>http://www.geonovum.nl/imkl2015/1.0/def/TelecommunicationsAppurtenanceIMKLTypeValue/kabelverdeler</v>
       </c>
     </row>
     <row r="82" spans="1:7">
       <c r="A82" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="B82" s="13" t="s">
         <v>206</v>
@@ -4072,13 +4086,13 @@
         <v>259</v>
       </c>
       <c r="G82" t="str">
-        <f>IF(B82="inspire",INSPIRE,IMKL) &amp; F82 &amp; "/" &amp; D82</f>
+        <f t="shared" si="1"/>
         <v>http://www.geonovum.nl/imkl2015/1.0/def/TelecommunicationsAppurtenanceIMKLTypeValue/Stijgleiding</v>
       </c>
     </row>
     <row r="83" spans="1:7">
       <c r="A83" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="B83" s="13" t="s">
         <v>206</v>
@@ -4096,13 +4110,13 @@
         <v>259</v>
       </c>
       <c r="G83" t="str">
-        <f>IF(B83="inspire",INSPIRE,IMKL) &amp; F83 &amp; "/" &amp; D83</f>
+        <f t="shared" si="1"/>
         <v>http://www.geonovum.nl/imkl2015/1.0/def/TelecommunicationsAppurtenanceIMKLTypeValue/GTWPOpnemen</v>
       </c>
     </row>
     <row r="84" spans="1:7">
       <c r="A84" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="B84" s="13" t="s">
         <v>206</v>
@@ -4120,13 +4134,13 @@
         <v>259</v>
       </c>
       <c r="G84" t="str">
-        <f>IF(B84="inspire",INSPIRE,IMKL) &amp; F84 &amp; "/" &amp; D84</f>
+        <f t="shared" si="1"/>
         <v>http://www.geonovum.nl/imkl2015/1.0/def/TelecommunicationsAppurtenanceIMKLTypeValue/afdekplaten</v>
       </c>
     </row>
     <row r="85" spans="1:7">
       <c r="A85" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="B85" s="13" t="s">
         <v>206</v>
@@ -4144,13 +4158,13 @@
         <v>259</v>
       </c>
       <c r="G85" t="str">
-        <f>IF(B85="inspire",INSPIRE,IMKL) &amp; F85 &amp; "/" &amp; D85</f>
+        <f t="shared" si="1"/>
         <v>http://www.geonovum.nl/imkl2015/1.0/def/TelecommunicationsAppurtenanceIMKLTypeValue/doorvoerramen</v>
       </c>
     </row>
     <row r="86" spans="1:7">
       <c r="A86" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="B86" s="17" t="s">
         <v>28</v>
@@ -4165,16 +4179,16 @@
         <v>136</v>
       </c>
       <c r="F86" s="8" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="G86" t="str">
-        <f>IF(B86="inspire",INSPIRE,IMKL) &amp; F86 &amp; "/" &amp; D86</f>
+        <f t="shared" si="1"/>
         <v>http://inspire.ec.europa.eu/codelist/TelecommunicationsCableMaterialTypeValue/coaxial</v>
       </c>
     </row>
     <row r="87" spans="1:7">
       <c r="A87" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="B87" s="17" t="s">
         <v>28</v>
@@ -4189,16 +4203,16 @@
         <v>137</v>
       </c>
       <c r="F87" s="8" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="G87" t="str">
-        <f>IF(B87="inspire",INSPIRE,IMKL) &amp; F87 &amp; "/" &amp; D87</f>
+        <f t="shared" si="1"/>
         <v>http://inspire.ec.europa.eu/codelist/TelecommunicationsCableMaterialTypeValue/opticalFiber</v>
       </c>
     </row>
     <row r="88" spans="1:7">
       <c r="A88" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="B88" s="17" t="s">
         <v>28</v>
@@ -4213,16 +4227,16 @@
         <v>138</v>
       </c>
       <c r="F88" s="8" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="G88" t="str">
-        <f>IF(B88="inspire",INSPIRE,IMKL) &amp; F88 &amp; "/" &amp; D88</f>
+        <f t="shared" si="1"/>
         <v>http://inspire.ec.europa.eu/codelist/TelecommunicationsCableMaterialTypeValue/twistedPair</v>
       </c>
     </row>
     <row r="89" spans="1:7" ht="15" thickBot="1">
       <c r="A89" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="C89" t="s">
         <v>348</v>
@@ -4237,13 +4251,13 @@
         <v>259</v>
       </c>
       <c r="G89" t="str">
-        <f>IF(B89="inspire",INSPIRE,IMKL) &amp; F89 &amp; "/" &amp; D89</f>
+        <f t="shared" si="1"/>
         <v>http://www.geonovum.nl/imkl2015/1.0/def/TelecommunicationsAppurtenanceIMKLTypeValue/puntVanLevering</v>
       </c>
     </row>
     <row r="90" spans="1:7" ht="15" thickBot="1">
       <c r="A90" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="B90" s="12" t="s">
         <v>206</v>
@@ -4261,13 +4275,13 @@
         <v>310</v>
       </c>
       <c r="G90" t="str">
-        <f>IF(B90="inspire",INSPIRE,IMKL) &amp; F90 &amp; "/" &amp; D90</f>
+        <f t="shared" si="1"/>
         <v>http://www.geonovum.nl/imkl2015/1.0/def/OilGasChemicalsAppurtenanceIMKLTypeValue/buis</v>
       </c>
     </row>
     <row r="91" spans="1:7" ht="15" thickBot="1">
       <c r="A91" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="B91" s="12" t="s">
         <v>206</v>
@@ -4285,13 +4299,13 @@
         <v>310</v>
       </c>
       <c r="G91" t="str">
-        <f>IF(B91="inspire",INSPIRE,IMKL) &amp; F91 &amp; "/" &amp; D91</f>
+        <f t="shared" si="1"/>
         <v>http://www.geonovum.nl/imkl2015/1.0/def/OilGasChemicalsAppurtenanceIMKLTypeValue/bocht</v>
       </c>
     </row>
     <row r="92" spans="1:7" ht="15" thickBot="1">
       <c r="A92" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="B92" s="12" t="s">
         <v>206</v>
@@ -4309,13 +4323,13 @@
         <v>310</v>
       </c>
       <c r="G92" t="str">
-        <f>IF(B92="inspire",INSPIRE,IMKL) &amp; F92 &amp; "/" &amp; D92</f>
+        <f t="shared" si="1"/>
         <v>http://www.geonovum.nl/imkl2015/1.0/def/OilGasChemicalsAppurtenanceIMKLTypeValue/tstuk</v>
       </c>
     </row>
     <row r="93" spans="1:7" ht="15" thickBot="1">
       <c r="A93" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="B93" s="12" t="s">
         <v>206</v>
@@ -4324,7 +4338,7 @@
         <v>348</v>
       </c>
       <c r="D93" s="20" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="E93" s="20" t="s">
         <v>236</v>
@@ -4333,13 +4347,13 @@
         <v>310</v>
       </c>
       <c r="G93" t="str">
-        <f>IF(B93="inspire",INSPIRE,IMKL) &amp; F93 &amp; "/" &amp; D93</f>
+        <f t="shared" si="1"/>
         <v>http://www.geonovum.nl/imkl2015/1.0/def/OilGasChemicalsAppurtenanceIMKLTypeValue/bodem</v>
       </c>
     </row>
     <row r="94" spans="1:7" ht="15" thickBot="1">
       <c r="A94" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="B94" s="12" t="s">
         <v>206</v>
@@ -4357,13 +4371,13 @@
         <v>310</v>
       </c>
       <c r="G94" t="str">
-        <f>IF(B94="inspire",INSPIRE,IMKL) &amp; F94 &amp; "/" &amp; D94</f>
+        <f t="shared" si="1"/>
         <v>http://www.geonovum.nl/imkl2015/1.0/def/OilGasChemicalsAppurtenanceIMKLTypeValue/lasnok</v>
       </c>
     </row>
     <row r="95" spans="1:7" ht="15" thickBot="1">
       <c r="A95" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="B95" s="12" t="s">
         <v>206</v>
@@ -4381,13 +4395,13 @@
         <v>310</v>
       </c>
       <c r="G95" t="str">
-        <f>IF(B95="inspire",INSPIRE,IMKL) &amp; F95 &amp; "/" &amp; D95</f>
+        <f t="shared" si="1"/>
         <v>http://www.geonovum.nl/imkl2015/1.0/def/OilGasChemicalsAppurtenanceIMKLTypeValue/expansiestuk</v>
       </c>
     </row>
     <row r="96" spans="1:7" ht="15" thickBot="1">
       <c r="A96" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="B96" s="12" t="s">
         <v>206</v>
@@ -4405,13 +4419,13 @@
         <v>310</v>
       </c>
       <c r="G96" t="str">
-        <f>IF(B96="inspire",INSPIRE,IMKL) &amp; F96 &amp; "/" &amp; D96</f>
+        <f t="shared" si="1"/>
         <v>http://www.geonovum.nl/imkl2015/1.0/def/OilGasChemicalsAppurtenanceIMKLTypeValue/isolatieKoppeling</v>
       </c>
     </row>
     <row r="97" spans="1:7" ht="15" thickBot="1">
       <c r="A97" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="B97" s="12" t="s">
         <v>206</v>
@@ -4429,13 +4443,13 @@
         <v>310</v>
       </c>
       <c r="G97" t="str">
-        <f>IF(B97="inspire",INSPIRE,IMKL) &amp; F97 &amp; "/" &amp; D97</f>
+        <f t="shared" si="1"/>
         <v>http://www.geonovum.nl/imkl2015/1.0/def/OilGasChemicalsAppurtenanceIMKLTypeValue/vloeistofvanger</v>
       </c>
     </row>
     <row r="98" spans="1:7" ht="15" thickBot="1">
       <c r="A98" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="B98" s="12" t="s">
         <v>206</v>
@@ -4444,7 +4458,7 @@
         <v>348</v>
       </c>
       <c r="D98" s="20" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="E98" s="20" t="s">
         <v>241</v>
@@ -4453,13 +4467,13 @@
         <v>310</v>
       </c>
       <c r="G98" t="str">
-        <f>IF(B98="inspire",INSPIRE,IMKL) &amp; F98 &amp; "/" &amp; D98</f>
+        <f t="shared" si="1"/>
         <v>http://www.geonovum.nl/imkl2015/1.0/def/OilGasChemicalsAppurtenanceIMKLTypeValue/Raaginrichting</v>
       </c>
     </row>
     <row r="99" spans="1:7" ht="15" thickBot="1">
       <c r="A99" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="B99" s="12" t="s">
         <v>206</v>
@@ -4477,13 +4491,13 @@
         <v>310</v>
       </c>
       <c r="G99" t="str">
-        <f>IF(B99="inspire",INSPIRE,IMKL) &amp; F99 &amp; "/" &amp; D99</f>
+        <f t="shared" si="1"/>
         <v>http://www.geonovum.nl/imkl2015/1.0/def/OilGasChemicalsAppurtenanceIMKLTypeValue/algemeenGasTransportOnderdeel</v>
       </c>
     </row>
     <row r="100" spans="1:7" ht="15" thickBot="1">
       <c r="A100" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="B100" s="12" t="s">
         <v>206</v>
@@ -4501,13 +4515,13 @@
         <v>311</v>
       </c>
       <c r="G100" t="str">
-        <f>IF(B100="inspire",INSPIRE,IMKL) &amp; F100 &amp; "/" &amp; D100</f>
+        <f t="shared" si="1"/>
         <v>http://www.geonovum.nl/imkl2015/1.0/def/OilGasChemicalsProductIMKLTypeValue/mud</v>
       </c>
     </row>
     <row r="101" spans="1:7" ht="15" thickBot="1">
       <c r="A101" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="B101" s="12" t="s">
         <v>206</v>
@@ -4525,13 +4539,13 @@
         <v>311</v>
       </c>
       <c r="G101" t="str">
-        <f>IF(B101="inspire",INSPIRE,IMKL) &amp; F101 &amp; "/" &amp; D101</f>
+        <f t="shared" si="1"/>
         <v>http://www.geonovum.nl/imkl2015/1.0/def/OilGasChemicalsProductIMKLTypeValue/methanol</v>
       </c>
     </row>
     <row r="102" spans="1:7">
       <c r="A102" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="B102" s="12" t="s">
         <v>206</v>
@@ -4549,13 +4563,13 @@
         <v>311</v>
       </c>
       <c r="G102" t="str">
-        <f>IF(B102="inspire",INSPIRE,IMKL) &amp; F102 &amp; "/" &amp; D102</f>
+        <f t="shared" si="1"/>
         <v>http://www.geonovum.nl/imkl2015/1.0/def/OilGasChemicalsProductIMKLTypeValue/emulsie</v>
       </c>
     </row>
     <row r="103" spans="1:7" ht="15" thickBot="1">
       <c r="A103" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="B103" s="12" t="s">
         <v>206</v>
@@ -4573,13 +4587,13 @@
         <v>311</v>
       </c>
       <c r="G103" t="str">
-        <f>IF(B103="inspire",INSPIRE,IMKL) &amp; F103 &amp; "/" &amp; D103</f>
+        <f t="shared" si="1"/>
         <v>http://www.geonovum.nl/imkl2015/1.0/def/OilGasChemicalsProductIMKLTypeValue/glycol</v>
       </c>
     </row>
     <row r="104" spans="1:7" ht="15" thickBot="1">
       <c r="A104" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="B104" s="12" t="s">
         <v>206</v>
@@ -4597,13 +4611,13 @@
         <v>310</v>
       </c>
       <c r="G104" t="str">
-        <f>IF(B104="inspire",INSPIRE,IMKL) &amp; F104 &amp; "/" &amp; D104</f>
+        <f t="shared" si="1"/>
         <v>http://www.geonovum.nl/imkl2015/1.0/def/OilGasChemicalsAppurtenanceIMKLTypeValue/hoogbouwkoppelpunt</v>
       </c>
     </row>
     <row r="105" spans="1:7" ht="15" thickBot="1">
       <c r="A105" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="B105" s="12" t="s">
         <v>206</v>
@@ -4621,13 +4635,13 @@
         <v>310</v>
       </c>
       <c r="G105" t="str">
-        <f>IF(B105="inspire",INSPIRE,IMKL) &amp; F105 &amp; "/" &amp; D105</f>
+        <f t="shared" si="1"/>
         <v>http://www.geonovum.nl/imkl2015/1.0/def/OilGasChemicalsAppurtenanceIMKLTypeValue/ontluchting</v>
       </c>
     </row>
     <row r="106" spans="1:7">
       <c r="A106" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="B106" s="12" t="s">
         <v>206</v>
@@ -4645,13 +4659,13 @@
         <v>310</v>
       </c>
       <c r="G106" t="str">
-        <f>IF(B106="inspire",INSPIRE,IMKL) &amp; F106 &amp; "/" &amp; D106</f>
+        <f t="shared" si="1"/>
         <v>http://www.geonovum.nl/imkl2015/1.0/def/OilGasChemicalsAppurtenanceIMKLTypeValue/aftakzadel</v>
       </c>
     </row>
     <row r="107" spans="1:7">
       <c r="A107" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="B107" s="12" t="s">
         <v>206</v>
@@ -4669,13 +4683,13 @@
         <v>310</v>
       </c>
       <c r="G107" t="str">
-        <f>IF(B107="inspire",INSPIRE,IMKL) &amp; F107 &amp; "/" &amp; D107</f>
+        <f t="shared" si="1"/>
         <v>http://www.geonovum.nl/imkl2015/1.0/def/OilGasChemicalsAppurtenanceIMKLTypeValue/overgangsstuk</v>
       </c>
     </row>
     <row r="108" spans="1:7">
       <c r="A108" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="B108" s="12" t="s">
         <v>206</v>
@@ -4693,13 +4707,13 @@
         <v>310</v>
       </c>
       <c r="G108" t="str">
-        <f>IF(B108="inspire",INSPIRE,IMKL) &amp; F108 &amp; "/" &amp; D108</f>
+        <f t="shared" si="1"/>
         <v>http://www.geonovum.nl/imkl2015/1.0/def/OilGasChemicalsAppurtenanceIMKLTypeValue/isolatiestuk</v>
       </c>
     </row>
     <row r="109" spans="1:7">
       <c r="A109" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="B109" s="12" t="s">
         <v>206</v>
@@ -4717,13 +4731,13 @@
         <v>310</v>
       </c>
       <c r="G109" t="str">
-        <f>IF(B109="inspire",INSPIRE,IMKL) &amp; F109 &amp; "/" &amp; D109</f>
+        <f t="shared" si="1"/>
         <v>http://www.geonovum.nl/imkl2015/1.0/def/OilGasChemicalsAppurtenanceIMKLTypeValue/ontspanningselement</v>
       </c>
     </row>
     <row r="110" spans="1:7">
       <c r="A110" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="B110" s="12" t="s">
         <v>206</v>
@@ -4741,13 +4755,13 @@
         <v>310</v>
       </c>
       <c r="G110" t="str">
-        <f>IF(B110="inspire",INSPIRE,IMKL) &amp; F110 &amp; "/" &amp; D110</f>
+        <f t="shared" si="1"/>
         <v>http://www.geonovum.nl/imkl2015/1.0/def/OilGasChemicalsAppurtenanceIMKLTypeValue/hoogteligging</v>
       </c>
     </row>
     <row r="111" spans="1:7">
       <c r="A111" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="B111" s="12" t="s">
         <v>206</v>
@@ -4765,13 +4779,13 @@
         <v>310</v>
       </c>
       <c r="G111" t="str">
-        <f>IF(B111="inspire",INSPIRE,IMKL) &amp; F111 &amp; "/" &amp; D111</f>
+        <f t="shared" si="1"/>
         <v>http://www.geonovum.nl/imkl2015/1.0/def/OilGasChemicalsAppurtenanceIMKLTypeValue/adrespunt</v>
       </c>
     </row>
     <row r="112" spans="1:7">
       <c r="A112" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="B112" s="12" t="s">
         <v>82</v>
@@ -4789,13 +4803,13 @@
         <v>310</v>
       </c>
       <c r="G112" t="str">
-        <f>IF(B112="inspire",INSPIRE,IMKL) &amp; F112 &amp; "/" &amp; D112</f>
+        <f t="shared" si="1"/>
         <v>http://www.geonovum.nl/imkl2015/1.0/def/OilGasChemicalsAppurtenanceIMKLTypeValue/eindkap</v>
       </c>
     </row>
     <row r="113" spans="1:7">
       <c r="A113" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="B113" s="12" t="s">
         <v>82</v>
@@ -4813,13 +4827,13 @@
         <v>310</v>
       </c>
       <c r="G113" t="str">
-        <f>IF(B113="inspire",INSPIRE,IMKL) &amp; F113 &amp; "/" &amp; D113</f>
+        <f t="shared" si="1"/>
         <v>http://www.geonovum.nl/imkl2015/1.0/def/OilGasChemicalsAppurtenanceIMKLTypeValue/verloopstuk</v>
       </c>
     </row>
     <row r="114" spans="1:7">
       <c r="A114" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="B114" s="12" t="s">
         <v>82</v>
@@ -4837,13 +4851,13 @@
         <v>310</v>
       </c>
       <c r="G114" t="str">
-        <f>IF(B114="inspire",INSPIRE,IMKL) &amp; F114 &amp; "/" &amp; D114</f>
+        <f t="shared" si="1"/>
         <v>http://www.geonovum.nl/imkl2015/1.0/def/OilGasChemicalsAppurtenanceIMKLTypeValue/afsluiter</v>
       </c>
     </row>
     <row r="115" spans="1:7">
       <c r="A115" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="B115" s="12" t="s">
         <v>82</v>
@@ -4861,13 +4875,13 @@
         <v>310</v>
       </c>
       <c r="G115" t="str">
-        <f>IF(B115="inspire",INSPIRE,IMKL) &amp; F115 &amp; "/" &amp; D115</f>
+        <f t="shared" si="1"/>
         <v>http://www.geonovum.nl/imkl2015/1.0/def/OilGasChemicalsAppurtenanceIMKLTypeValue/meetpunt</v>
       </c>
     </row>
     <row r="116" spans="1:7">
       <c r="A116" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="B116" s="12" t="s">
         <v>82</v>
@@ -4885,13 +4899,13 @@
         <v>310</v>
       </c>
       <c r="G116" t="str">
-        <f>IF(B116="inspire",INSPIRE,IMKL) &amp; F116 &amp; "/" &amp; D116</f>
+        <f t="shared" si="1"/>
         <v>http://www.geonovum.nl/imkl2015/1.0/def/OilGasChemicalsAppurtenanceIMKLTypeValue/sifon</v>
       </c>
     </row>
     <row r="117" spans="1:7">
       <c r="A117" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="B117" s="12" t="s">
         <v>82</v>
@@ -4909,13 +4923,13 @@
         <v>310</v>
       </c>
       <c r="G117" t="str">
-        <f>IF(B117="inspire",INSPIRE,IMKL) &amp; F117 &amp; "/" &amp; D117</f>
+        <f t="shared" si="1"/>
         <v>http://www.geonovum.nl/imkl2015/1.0/def/OilGasChemicalsAppurtenanceIMKLTypeValue/blaasgat</v>
       </c>
     </row>
     <row r="118" spans="1:7">
       <c r="A118" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="B118" s="12" t="s">
         <v>82</v>
@@ -4933,13 +4947,13 @@
         <v>310</v>
       </c>
       <c r="G118" t="str">
-        <f>IF(B118="inspire",INSPIRE,IMKL) &amp; F118 &amp; "/" &amp; D118</f>
+        <f t="shared" si="1"/>
         <v>http://www.geonovum.nl/imkl2015/1.0/def/OilGasChemicalsAppurtenanceIMKLTypeValue/kbMeetpunt</v>
       </c>
     </row>
     <row r="119" spans="1:7">
       <c r="A119" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="B119" s="12" t="s">
         <v>28</v>
@@ -4957,13 +4971,13 @@
         <v>309</v>
       </c>
       <c r="G119" t="str">
-        <f>IF(B119="inspire",INSPIRE,IMKL) &amp; F119 &amp; "/" &amp; D119</f>
+        <f t="shared" si="1"/>
         <v>http://inspire.ec.europa.eu/codelist/OilGasChemicalsAppurtenanceTypeValue/gasStation</v>
       </c>
     </row>
     <row r="120" spans="1:7">
       <c r="A120" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="B120" s="12" t="s">
         <v>28</v>
@@ -4972,7 +4986,7 @@
         <v>348</v>
       </c>
       <c r="D120" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="E120" s="18" t="s">
         <v>50</v>
@@ -4981,13 +4995,13 @@
         <v>309</v>
       </c>
       <c r="G120" t="str">
-        <f>IF(B120="inspire",INSPIRE,IMKL) &amp; F120 &amp; "/" &amp; D120</f>
+        <f t="shared" si="1"/>
         <v>http://inspire.ec.europa.eu/codelist/OilGasChemicalsAppurtenanceTypeValue/oilGasChemicalsNode</v>
       </c>
     </row>
     <row r="121" spans="1:7">
       <c r="A121" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="B121" s="12" t="s">
         <v>28</v>
@@ -5005,13 +5019,13 @@
         <v>309</v>
       </c>
       <c r="G121" t="str">
-        <f>IF(B121="inspire",INSPIRE,IMKL) &amp; F121 &amp; "/" &amp; D121</f>
+        <f t="shared" si="1"/>
         <v>http://inspire.ec.europa.eu/codelist/OilGasChemicalsAppurtenanceTypeValue/marker</v>
       </c>
     </row>
     <row r="122" spans="1:7">
       <c r="A122" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="B122" s="12" t="s">
         <v>28</v>
@@ -5029,13 +5043,13 @@
         <v>309</v>
       </c>
       <c r="G122" t="str">
-        <f>IF(B122="inspire",INSPIRE,IMKL) &amp; F122 &amp; "/" &amp; D122</f>
+        <f t="shared" si="1"/>
         <v>http://inspire.ec.europa.eu/codelist/OilGasChemicalsAppurtenanceTypeValue/deliveryPoint</v>
       </c>
     </row>
     <row r="123" spans="1:7">
       <c r="A123" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="B123" s="12" t="s">
         <v>28</v>
@@ -5053,13 +5067,13 @@
         <v>309</v>
       </c>
       <c r="G123" t="str">
-        <f>IF(B123="inspire",INSPIRE,IMKL) &amp; F123 &amp; "/" &amp; D123</f>
+        <f t="shared" si="1"/>
         <v>http://inspire.ec.europa.eu/codelist/OilGasChemicalsAppurtenanceTypeValue/terminal</v>
       </c>
     </row>
     <row r="124" spans="1:7">
       <c r="A124" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="B124" s="12" t="s">
         <v>28</v>
@@ -5077,13 +5091,13 @@
         <v>309</v>
       </c>
       <c r="G124" t="str">
-        <f>IF(B124="inspire",INSPIRE,IMKL) &amp; F124 &amp; "/" &amp; D124</f>
+        <f t="shared" si="1"/>
         <v>http://inspire.ec.europa.eu/codelist/OilGasChemicalsAppurtenanceTypeValue/pump</v>
       </c>
     </row>
     <row r="125" spans="1:7">
       <c r="A125" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="B125" s="12" t="s">
         <v>28</v>
@@ -5101,13 +5115,13 @@
         <v>309</v>
       </c>
       <c r="G125" t="str">
-        <f>IF(B125="inspire",INSPIRE,IMKL) &amp; F125 &amp; "/" &amp; D125</f>
+        <f t="shared" si="1"/>
         <v>http://inspire.ec.europa.eu/codelist/OilGasChemicalsAppurtenanceTypeValue/pumpingStation</v>
       </c>
     </row>
     <row r="126" spans="1:7">
       <c r="A126" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="B126" s="12" t="s">
         <v>28</v>
@@ -5125,13 +5139,13 @@
         <v>309</v>
       </c>
       <c r="G126" t="str">
-        <f>IF(B126="inspire",INSPIRE,IMKL) &amp; F126 &amp; "/" &amp; D126</f>
+        <f t="shared" si="1"/>
         <v>http://inspire.ec.europa.eu/codelist/OilGasChemicalsAppurtenanceTypeValue/productionRegion</v>
       </c>
     </row>
     <row r="127" spans="1:7">
       <c r="A127" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="B127" s="12" t="s">
         <v>28</v>
@@ -5149,13 +5163,13 @@
         <v>309</v>
       </c>
       <c r="G127" t="str">
-        <f>IF(B127="inspire",INSPIRE,IMKL) &amp; F127 &amp; "/" &amp; D127</f>
+        <f t="shared" si="1"/>
         <v>http://inspire.ec.europa.eu/codelist/OilGasChemicalsAppurtenanceTypeValue/storage</v>
       </c>
     </row>
     <row r="128" spans="1:7">
       <c r="A128" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="B128" s="12" t="s">
         <v>28</v>
@@ -5173,13 +5187,13 @@
         <v>260</v>
       </c>
       <c r="G128" t="str">
-        <f>IF(B128="inspire",INSPIRE,IMKL) &amp; F128 &amp; "/" &amp; D128</f>
+        <f t="shared" si="1"/>
         <v>http://inspire.ec.europa.eu/codelist/OilGasChemicalsProductTypeValue/naturalGas</v>
       </c>
     </row>
     <row r="129" spans="1:7">
       <c r="A129" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="B129" s="12" t="s">
         <v>82</v>
@@ -5197,13 +5211,13 @@
         <v>311</v>
       </c>
       <c r="G129" t="str">
-        <f>IF(B129="inspire",INSPIRE,IMKL) &amp; F129 &amp; "/" &amp; D129</f>
+        <f t="shared" si="1"/>
         <v>http://www.geonovum.nl/imkl2015/1.0/def/OilGasChemicalsProductIMKLTypeValue/bioGas</v>
       </c>
     </row>
     <row r="130" spans="1:7">
       <c r="A130" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="B130" s="1" t="s">
         <v>82</v>
@@ -5221,13 +5235,13 @@
         <v>260</v>
       </c>
       <c r="G130" t="str">
-        <f>IF(B130="inspire",INSPIRE,IMKL) &amp; F130 &amp; "/" &amp; D130</f>
+        <f t="shared" ref="G130:G193" si="2">IF(B130="inspire",INSPIRE,IMKL) &amp; F130 &amp; "/" &amp; D130</f>
         <v>http://www.geonovum.nl/imkl2015/1.0/def/OilGasChemicalsProductTypeValue/accetone</v>
       </c>
     </row>
     <row r="131" spans="1:7">
       <c r="A131" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="B131" s="1" t="s">
         <v>82</v>
@@ -5245,13 +5259,13 @@
         <v>260</v>
       </c>
       <c r="G131" t="str">
-        <f>IF(B131="inspire",INSPIRE,IMKL) &amp; F131 &amp; "/" &amp; D131</f>
+        <f t="shared" si="2"/>
         <v>http://www.geonovum.nl/imkl2015/1.0/def/OilGasChemicalsProductTypeValue/air</v>
       </c>
     </row>
     <row r="132" spans="1:7">
       <c r="A132" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="B132" s="1" t="s">
         <v>82</v>
@@ -5269,13 +5283,13 @@
         <v>260</v>
       </c>
       <c r="G132" t="str">
-        <f>IF(B132="inspire",INSPIRE,IMKL) &amp; F132 &amp; "/" &amp; D132</f>
+        <f t="shared" si="2"/>
         <v>http://www.geonovum.nl/imkl2015/1.0/def/OilGasChemicalsProductTypeValue/argon</v>
       </c>
     </row>
     <row r="133" spans="1:7">
       <c r="A133" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="B133" s="1" t="s">
         <v>82</v>
@@ -5293,13 +5307,13 @@
         <v>260</v>
       </c>
       <c r="G133" t="str">
-        <f>IF(B133="inspire",INSPIRE,IMKL) &amp; F133 &amp; "/" &amp; D133</f>
+        <f t="shared" si="2"/>
         <v>http://www.geonovum.nl/imkl2015/1.0/def/OilGasChemicalsProductTypeValue/butadiene1.2</v>
       </c>
     </row>
     <row r="134" spans="1:7">
       <c r="A134" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="B134" s="1" t="s">
         <v>82</v>
@@ -5317,13 +5331,13 @@
         <v>260</v>
       </c>
       <c r="G134" t="str">
-        <f>IF(B134="inspire",INSPIRE,IMKL) &amp; F134 &amp; "/" &amp; D134</f>
+        <f t="shared" si="2"/>
         <v>http://www.geonovum.nl/imkl2015/1.0/def/OilGasChemicalsProductTypeValue/butadiene1.3</v>
       </c>
     </row>
     <row r="135" spans="1:7">
       <c r="A135" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="B135" s="1" t="s">
         <v>82</v>
@@ -5341,13 +5355,13 @@
         <v>260</v>
       </c>
       <c r="G135" t="str">
-        <f>IF(B135="inspire",INSPIRE,IMKL) &amp; F135 &amp; "/" &amp; D135</f>
+        <f t="shared" si="2"/>
         <v>http://www.geonovum.nl/imkl2015/1.0/def/OilGasChemicalsProductTypeValue/butane</v>
       </c>
     </row>
     <row r="136" spans="1:7">
       <c r="A136" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="B136" s="1" t="s">
         <v>82</v>
@@ -5365,13 +5379,13 @@
         <v>260</v>
       </c>
       <c r="G136" t="str">
-        <f>IF(B136="inspire",INSPIRE,IMKL) &amp; F136 &amp; "/" &amp; D136</f>
+        <f t="shared" si="2"/>
         <v>http://www.geonovum.nl/imkl2015/1.0/def/OilGasChemicalsProductTypeValue/carbonMonoxide</v>
       </c>
     </row>
     <row r="137" spans="1:7">
       <c r="A137" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="B137" s="1" t="s">
         <v>82</v>
@@ -5389,13 +5403,13 @@
         <v>260</v>
       </c>
       <c r="G137" t="str">
-        <f>IF(B137="inspire",INSPIRE,IMKL) &amp; F137 &amp; "/" &amp; D137</f>
+        <f t="shared" si="2"/>
         <v>http://www.geonovum.nl/imkl2015/1.0/def/OilGasChemicalsProductTypeValue/chlorine</v>
       </c>
     </row>
     <row r="138" spans="1:7">
       <c r="A138" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="B138" s="1" t="s">
         <v>82</v>
@@ -5413,13 +5427,13 @@
         <v>260</v>
       </c>
       <c r="G138" t="str">
-        <f>IF(B138="inspire",INSPIRE,IMKL) &amp; F138 &amp; "/" &amp; D138</f>
+        <f t="shared" si="2"/>
         <v>http://www.geonovum.nl/imkl2015/1.0/def/OilGasChemicalsProductTypeValue/concrete</v>
       </c>
     </row>
     <row r="139" spans="1:7">
       <c r="A139" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="B139" s="1" t="s">
         <v>82</v>
@@ -5437,13 +5451,13 @@
         <v>260</v>
       </c>
       <c r="G139" t="str">
-        <f>IF(B139="inspire",INSPIRE,IMKL) &amp; F139 &amp; "/" &amp; D139</f>
+        <f t="shared" si="2"/>
         <v>http://www.geonovum.nl/imkl2015/1.0/def/OilGasChemicalsProductTypeValue/crude</v>
       </c>
     </row>
     <row r="140" spans="1:7">
       <c r="A140" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="B140" s="1" t="s">
         <v>82</v>
@@ -5461,13 +5475,13 @@
         <v>260</v>
       </c>
       <c r="G140" t="str">
-        <f>IF(B140="inspire",INSPIRE,IMKL) &amp; F140 &amp; "/" &amp; D140</f>
+        <f t="shared" si="2"/>
         <v>http://www.geonovum.nl/imkl2015/1.0/def/OilGasChemicalsProductTypeValue/dichloroethane</v>
       </c>
     </row>
     <row r="141" spans="1:7">
       <c r="A141" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="B141" s="1" t="s">
         <v>82</v>
@@ -5485,13 +5499,13 @@
         <v>260</v>
       </c>
       <c r="G141" t="str">
-        <f>IF(B141="inspire",INSPIRE,IMKL) &amp; F141 &amp; "/" &amp; D141</f>
+        <f t="shared" si="2"/>
         <v>http://www.geonovum.nl/imkl2015/1.0/def/OilGasChemicalsProductTypeValue/diesel</v>
       </c>
     </row>
     <row r="142" spans="1:7">
       <c r="A142" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="B142" s="1" t="s">
         <v>82</v>
@@ -5509,13 +5523,13 @@
         <v>260</v>
       </c>
       <c r="G142" t="str">
-        <f>IF(B142="inspire",INSPIRE,IMKL) &amp; F142 &amp; "/" &amp; D142</f>
+        <f t="shared" si="2"/>
         <v>http://www.geonovum.nl/imkl2015/1.0/def/OilGasChemicalsProductTypeValue/ethylene</v>
       </c>
     </row>
     <row r="143" spans="1:7">
       <c r="A143" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="B143" s="1" t="s">
         <v>82</v>
@@ -5533,13 +5547,13 @@
         <v>260</v>
       </c>
       <c r="G143" t="str">
-        <f>IF(B143="inspire",INSPIRE,IMKL) &amp; F143 &amp; "/" &amp; D143</f>
+        <f t="shared" si="2"/>
         <v>http://www.geonovum.nl/imkl2015/1.0/def/OilGasChemicalsProductTypeValue/gasFabricationOfCocs</v>
       </c>
     </row>
     <row r="144" spans="1:7">
       <c r="A144" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="B144" s="1" t="s">
         <v>82</v>
@@ -5557,13 +5571,13 @@
         <v>260</v>
       </c>
       <c r="G144" t="str">
-        <f>IF(B144="inspire",INSPIRE,IMKL) &amp; F144 &amp; "/" &amp; D144</f>
+        <f t="shared" si="2"/>
         <v>http://www.geonovum.nl/imkl2015/1.0/def/OilGasChemicalsProductTypeValue/gasHFx</v>
       </c>
     </row>
     <row r="145" spans="1:7">
       <c r="A145" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="B145" s="1" t="s">
         <v>82</v>
@@ -5581,13 +5595,13 @@
         <v>260</v>
       </c>
       <c r="G145" t="str">
-        <f>IF(B145="inspire",INSPIRE,IMKL) &amp; F145 &amp; "/" &amp; D145</f>
+        <f t="shared" si="2"/>
         <v>http://www.geonovum.nl/imkl2015/1.0/def/OilGasChemicalsProductTypeValue/gasoil</v>
       </c>
     </row>
     <row r="146" spans="1:7">
       <c r="A146" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="B146" s="1" t="s">
         <v>82</v>
@@ -5605,13 +5619,13 @@
         <v>260</v>
       </c>
       <c r="G146" t="str">
-        <f>IF(B146="inspire",INSPIRE,IMKL) &amp; F146 &amp; "/" &amp; D146</f>
+        <f t="shared" si="2"/>
         <v>http://www.geonovum.nl/imkl2015/1.0/def/OilGasChemicalsProductTypeValue/hydrogen</v>
       </c>
     </row>
     <row r="147" spans="1:7">
       <c r="A147" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="B147" s="1" t="s">
         <v>82</v>
@@ -5629,13 +5643,13 @@
         <v>260</v>
       </c>
       <c r="G147" t="str">
-        <f>IF(B147="inspire",INSPIRE,IMKL) &amp; F147 &amp; "/" &amp; D147</f>
+        <f t="shared" si="2"/>
         <v>http://www.geonovum.nl/imkl2015/1.0/def/OilGasChemicalsProductTypeValue/isobutane</v>
       </c>
     </row>
     <row r="148" spans="1:7">
       <c r="A148" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="B148" s="1" t="s">
         <v>82</v>
@@ -5653,13 +5667,13 @@
         <v>260</v>
       </c>
       <c r="G148" t="str">
-        <f>IF(B148="inspire",INSPIRE,IMKL) &amp; F148 &amp; "/" &amp; D148</f>
+        <f t="shared" si="2"/>
         <v>http://www.geonovum.nl/imkl2015/1.0/def/OilGasChemicalsProductTypeValue/JET-A1</v>
       </c>
     </row>
     <row r="149" spans="1:7">
       <c r="A149" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="B149" s="1" t="s">
         <v>82</v>
@@ -5677,13 +5691,13 @@
         <v>260</v>
       </c>
       <c r="G149" t="str">
-        <f>IF(B149="inspire",INSPIRE,IMKL) &amp; F149 &amp; "/" &amp; D149</f>
+        <f t="shared" si="2"/>
         <v>http://www.geonovum.nl/imkl2015/1.0/def/OilGasChemicalsProductTypeValue/kerosene</v>
       </c>
     </row>
     <row r="150" spans="1:7">
       <c r="A150" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="B150" s="1" t="s">
         <v>82</v>
@@ -5701,13 +5715,13 @@
         <v>260</v>
       </c>
       <c r="G150" t="str">
-        <f>IF(B150="inspire",INSPIRE,IMKL) &amp; F150 &amp; "/" &amp; D150</f>
+        <f t="shared" si="2"/>
         <v>http://www.geonovum.nl/imkl2015/1.0/def/OilGasChemicalsProductTypeValue/liquidAmmonia</v>
       </c>
     </row>
     <row r="151" spans="1:7">
       <c r="A151" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="B151" s="1" t="s">
         <v>82</v>
@@ -5725,13 +5739,13 @@
         <v>260</v>
       </c>
       <c r="G151" t="str">
-        <f>IF(B151="inspire",INSPIRE,IMKL) &amp; F151 &amp; "/" &amp; D151</f>
+        <f t="shared" si="2"/>
         <v>http://www.geonovum.nl/imkl2015/1.0/def/OilGasChemicalsProductTypeValue/liquidHydrocarbon</v>
       </c>
     </row>
     <row r="152" spans="1:7">
       <c r="A152" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="B152" s="1" t="s">
         <v>82</v>
@@ -5749,13 +5763,13 @@
         <v>260</v>
       </c>
       <c r="G152" t="str">
-        <f>IF(B152="inspire",INSPIRE,IMKL) &amp; F152 &amp; "/" &amp; D152</f>
+        <f t="shared" si="2"/>
         <v>http://www.geonovum.nl/imkl2015/1.0/def/OilGasChemicalsProductTypeValue/multiProduct</v>
       </c>
     </row>
     <row r="153" spans="1:7">
       <c r="A153" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="B153" s="1" t="s">
         <v>82</v>
@@ -5773,13 +5787,13 @@
         <v>260</v>
       </c>
       <c r="G153" t="str">
-        <f>IF(B153="inspire",INSPIRE,IMKL) &amp; F153 &amp; "/" &amp; D153</f>
+        <f t="shared" si="2"/>
         <v>http://www.geonovum.nl/imkl2015/1.0/def/OilGasChemicalsProductTypeValue/MVC</v>
       </c>
     </row>
     <row r="154" spans="1:7">
       <c r="A154" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="B154" s="1" t="s">
         <v>82</v>
@@ -5797,13 +5811,13 @@
         <v>260</v>
       </c>
       <c r="G154" t="str">
-        <f>IF(B154="inspire",INSPIRE,IMKL) &amp; F154 &amp; "/" &amp; D154</f>
+        <f t="shared" si="2"/>
         <v>http://www.geonovum.nl/imkl2015/1.0/def/OilGasChemicalsProductTypeValue/nitrogen</v>
       </c>
     </row>
     <row r="155" spans="1:7">
       <c r="A155" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="B155" s="1" t="s">
         <v>82</v>
@@ -5821,13 +5835,13 @@
         <v>260</v>
       </c>
       <c r="G155" t="str">
-        <f>IF(B155="inspire",INSPIRE,IMKL) &amp; F155 &amp; "/" &amp; D155</f>
+        <f t="shared" si="2"/>
         <v>http://www.geonovum.nl/imkl2015/1.0/def/OilGasChemicalsProductTypeValue/oxygen</v>
       </c>
     </row>
     <row r="156" spans="1:7">
       <c r="A156" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="B156" s="1" t="s">
         <v>82</v>
@@ -5845,13 +5859,13 @@
         <v>260</v>
       </c>
       <c r="G156" t="str">
-        <f>IF(B156="inspire",INSPIRE,IMKL) &amp; F156 &amp; "/" &amp; D156</f>
+        <f t="shared" si="2"/>
         <v>http://www.geonovum.nl/imkl2015/1.0/def/OilGasChemicalsProductTypeValue/phenol</v>
       </c>
     </row>
     <row r="157" spans="1:7">
       <c r="A157" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="B157" s="1" t="s">
         <v>82</v>
@@ -5869,13 +5883,13 @@
         <v>260</v>
       </c>
       <c r="G157" t="str">
-        <f>IF(B157="inspire",INSPIRE,IMKL) &amp; F157 &amp; "/" &amp; D157</f>
+        <f t="shared" si="2"/>
         <v>http://www.geonovum.nl/imkl2015/1.0/def/OilGasChemicalsProductTypeValue/propane</v>
       </c>
     </row>
     <row r="158" spans="1:7">
       <c r="A158" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="B158" s="1" t="s">
         <v>82</v>
@@ -5893,13 +5907,13 @@
         <v>260</v>
       </c>
       <c r="G158" t="str">
-        <f>IF(B158="inspire",INSPIRE,IMKL) &amp; F158 &amp; "/" &amp; D158</f>
+        <f t="shared" si="2"/>
         <v>http://www.geonovum.nl/imkl2015/1.0/def/OilGasChemicalsProductTypeValue/propylene</v>
       </c>
     </row>
     <row r="159" spans="1:7">
       <c r="A159" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="B159" s="1" t="s">
         <v>82</v>
@@ -5917,13 +5931,13 @@
         <v>260</v>
       </c>
       <c r="G159" t="str">
-        <f>IF(B159="inspire",INSPIRE,IMKL) &amp; F159 &amp; "/" &amp; D159</f>
+        <f t="shared" si="2"/>
         <v>http://www.geonovum.nl/imkl2015/1.0/def/OilGasChemicalsProductTypeValue/saltWater</v>
       </c>
     </row>
     <row r="160" spans="1:7">
       <c r="A160" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="B160" s="1" t="s">
         <v>82</v>
@@ -5941,13 +5955,13 @@
         <v>260</v>
       </c>
       <c r="G160" t="str">
-        <f>IF(B160="inspire",INSPIRE,IMKL) &amp; F160 &amp; "/" &amp; D160</f>
+        <f t="shared" si="2"/>
         <v>http://www.geonovum.nl/imkl2015/1.0/def/OilGasChemicalsProductTypeValue/saumur</v>
       </c>
     </row>
     <row r="161" spans="1:7">
       <c r="A161" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="B161" s="1" t="s">
         <v>82</v>
@@ -5965,13 +5979,13 @@
         <v>260</v>
       </c>
       <c r="G161" t="str">
-        <f>IF(B161="inspire",INSPIRE,IMKL) &amp; F161 &amp; "/" &amp; D161</f>
+        <f t="shared" si="2"/>
         <v>http://www.geonovum.nl/imkl2015/1.0/def/OilGasChemicalsProductTypeValue/sand</v>
       </c>
     </row>
     <row r="162" spans="1:7">
       <c r="A162" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="B162" s="1" t="s">
         <v>82</v>
@@ -5989,13 +6003,13 @@
         <v>260</v>
       </c>
       <c r="G162" t="str">
-        <f>IF(B162="inspire",INSPIRE,IMKL) &amp; F162 &amp; "/" &amp; D162</f>
+        <f t="shared" si="2"/>
         <v>http://www.geonovum.nl/imkl2015/1.0/def/OilGasChemicalsProductTypeValue/tetrachloroide</v>
       </c>
     </row>
     <row r="163" spans="1:7">
       <c r="A163" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="B163" s="1" t="s">
         <v>82</v>
@@ -6013,13 +6027,13 @@
         <v>260</v>
       </c>
       <c r="G163" t="str">
-        <f>IF(B163="inspire",INSPIRE,IMKL) &amp; F163 &amp; "/" &amp; D163</f>
+        <f t="shared" si="2"/>
         <v>http://www.geonovum.nl/imkl2015/1.0/def/OilGasChemicalsProductTypeValue/unknown</v>
       </c>
     </row>
     <row r="164" spans="1:7">
       <c r="A164" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="B164" s="1" t="s">
         <v>82</v>
@@ -6037,13 +6051,13 @@
         <v>260</v>
       </c>
       <c r="G164" t="str">
-        <f>IF(B164="inspire",INSPIRE,IMKL) &amp; F164 &amp; "/" &amp; D164</f>
+        <f t="shared" si="2"/>
         <v>http://www.geonovum.nl/imkl2015/1.0/def/OilGasChemicalsProductTypeValue/water</v>
       </c>
     </row>
     <row r="165" spans="1:7" ht="15" thickBot="1">
       <c r="A165" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="B165" s="1" t="s">
         <v>82</v>
@@ -6061,7 +6075,7 @@
         <v>260</v>
       </c>
       <c r="G165" t="str">
-        <f>IF(B165="inspire",INSPIRE,IMKL) &amp; F165 &amp; "/" &amp; D165</f>
+        <f t="shared" si="2"/>
         <v>http://www.geonovum.nl/imkl2015/1.0/def/OilGasChemicalsProductTypeValue/empty</v>
       </c>
     </row>
@@ -6085,7 +6099,7 @@
         <v>261</v>
       </c>
       <c r="G166" t="str">
-        <f>IF(B166="inspire",INSPIRE,IMKL) &amp; F166 &amp; "/" &amp; D166</f>
+        <f t="shared" si="2"/>
         <v>http://www.geonovum.nl/imkl2015/1.0/def/WaterAppurtenanceTypeIMKLValue/afsluiter</v>
       </c>
     </row>
@@ -6109,7 +6123,7 @@
         <v>261</v>
       </c>
       <c r="G167" t="str">
-        <f>IF(B167="inspire",INSPIRE,IMKL) &amp; F167 &amp; "/" &amp; D167</f>
+        <f t="shared" si="2"/>
         <v>http://www.geonovum.nl/imkl2015/1.0/def/WaterAppurtenanceTypeIMKLValue/diameterovergang</v>
       </c>
     </row>
@@ -6133,7 +6147,7 @@
         <v>261</v>
       </c>
       <c r="G168" t="str">
-        <f>IF(B168="inspire",INSPIRE,IMKL) &amp; F168 &amp; "/" &amp; D168</f>
+        <f t="shared" si="2"/>
         <v>http://www.geonovum.nl/imkl2015/1.0/def/WaterAppurtenanceTypeIMKLValue/materiaalovergang</v>
       </c>
     </row>
@@ -6157,7 +6171,7 @@
         <v>261</v>
       </c>
       <c r="G169" t="str">
-        <f>IF(B169="inspire",INSPIRE,IMKL) &amp; F169 &amp; "/" &amp; D169</f>
+        <f t="shared" si="2"/>
         <v>http://www.geonovum.nl/imkl2015/1.0/def/WaterAppurtenanceTypeIMKLValue/eindpunt</v>
       </c>
     </row>
@@ -6181,7 +6195,7 @@
         <v>261</v>
       </c>
       <c r="G170" t="str">
-        <f>IF(B170="inspire",INSPIRE,IMKL) &amp; F170 &amp; "/" &amp; D170</f>
+        <f t="shared" si="2"/>
         <v>http://www.geonovum.nl/imkl2015/1.0/def/WaterAppurtenanceTypeIMKLValue/blindflens</v>
       </c>
     </row>
@@ -6205,7 +6219,7 @@
         <v>306</v>
       </c>
       <c r="G171" t="str">
-        <f>IF(B171="inspire",INSPIRE,IMKL) &amp; F171 &amp; "/" &amp; D171</f>
+        <f t="shared" si="2"/>
         <v>http://inspire.ec.europa.eu/codelist/WaterAppurtenanceTypeValue/checkValve</v>
       </c>
     </row>
@@ -6229,7 +6243,7 @@
         <v>306</v>
       </c>
       <c r="G172" t="str">
-        <f>IF(B172="inspire",INSPIRE,IMKL) &amp; F172 &amp; "/" &amp; D172</f>
+        <f t="shared" si="2"/>
         <v>http://inspire.ec.europa.eu/codelist/WaterAppurtenanceTypeValue/waterExhaustPoint</v>
       </c>
     </row>
@@ -6253,7 +6267,7 @@
         <v>306</v>
       </c>
       <c r="G173" t="str">
-        <f>IF(B173="inspire",INSPIRE,IMKL) &amp; F173 &amp; "/" &amp; D173</f>
+        <f t="shared" si="2"/>
         <v>http://inspire.ec.europa.eu/codelist/WaterAppurtenanceTypeValue/waterDischargePoint</v>
       </c>
     </row>
@@ -6277,7 +6291,7 @@
         <v>306</v>
       </c>
       <c r="G174" t="str">
-        <f>IF(B174="inspire",INSPIRE,IMKL) &amp; F174 &amp; "/" &amp; D174</f>
+        <f t="shared" si="2"/>
         <v>http://inspire.ec.europa.eu/codelist/WaterAppurtenanceTypeValue/anode</v>
       </c>
     </row>
@@ -6301,7 +6315,7 @@
         <v>306</v>
       </c>
       <c r="G175" t="str">
-        <f>IF(B175="inspire",INSPIRE,IMKL) &amp; F175 &amp; "/" &amp; D175</f>
+        <f t="shared" si="2"/>
         <v>http://inspire.ec.europa.eu/codelist/WaterAppurtenanceTypeValue/fireHydrant</v>
       </c>
     </row>
@@ -6325,7 +6339,7 @@
         <v>306</v>
       </c>
       <c r="G176" t="str">
-        <f>IF(B176="inspire",INSPIRE,IMKL) &amp; F176 &amp; "/" &amp; D176</f>
+        <f t="shared" si="2"/>
         <v>http://inspire.ec.europa.eu/codelist/WaterAppurtenanceTypeValue/well</v>
       </c>
     </row>
@@ -6349,7 +6363,7 @@
         <v>306</v>
       </c>
       <c r="G177" t="str">
-        <f>IF(B177="inspire",INSPIRE,IMKL) &amp; F177 &amp; "/" &amp; D177</f>
+        <f t="shared" si="2"/>
         <v>http://inspire.ec.europa.eu/codelist/WaterAppurtenanceTypeValue/controlValve</v>
       </c>
     </row>
@@ -6373,7 +6387,7 @@
         <v>306</v>
       </c>
       <c r="G178" t="str">
-        <f>IF(B178="inspire",INSPIRE,IMKL) &amp; F178 &amp; "/" &amp; D178</f>
+        <f t="shared" si="2"/>
         <v>http://inspire.ec.europa.eu/codelist/WaterAppurtenanceTypeValue/pressureController</v>
       </c>
     </row>
@@ -6397,7 +6411,7 @@
         <v>306</v>
       </c>
       <c r="G179" t="str">
-        <f>IF(B179="inspire",INSPIRE,IMKL) &amp; F179 &amp; "/" &amp; D179</f>
+        <f t="shared" si="2"/>
         <v>http://inspire.ec.europa.eu/codelist/WaterAppurtenanceTypeValue/junction</v>
       </c>
     </row>
@@ -6421,7 +6435,7 @@
         <v>306</v>
       </c>
       <c r="G180" t="str">
-        <f>IF(B180="inspire",INSPIRE,IMKL) &amp; F180 &amp; "/" &amp; D180</f>
+        <f t="shared" si="2"/>
         <v>http://inspire.ec.europa.eu/codelist/WaterAppurtenanceTypeValue/lateralPoint</v>
       </c>
     </row>
@@ -6445,7 +6459,7 @@
         <v>306</v>
       </c>
       <c r="G181" t="str">
-        <f>IF(B181="inspire",INSPIRE,IMKL) &amp; F181 &amp; "/" &amp; D181</f>
+        <f t="shared" si="2"/>
         <v>http://inspire.ec.europa.eu/codelist/WaterAppurtenanceTypeValue/samplingStation</v>
       </c>
     </row>
@@ -6469,7 +6483,7 @@
         <v>306</v>
       </c>
       <c r="G182" t="str">
-        <f>IF(B182="inspire",INSPIRE,IMKL) &amp; F182 &amp; "/" &amp; D182</f>
+        <f t="shared" si="2"/>
         <v>http://inspire.ec.europa.eu/codelist/WaterAppurtenanceTypeValue/meter</v>
       </c>
     </row>
@@ -6493,7 +6507,7 @@
         <v>306</v>
       </c>
       <c r="G183" t="str">
-        <f>IF(B183="inspire",INSPIRE,IMKL) &amp; F183 &amp; "/" &amp; D183</f>
+        <f t="shared" si="2"/>
         <v>http://inspire.ec.europa.eu/codelist/WaterAppurtenanceTypeValue/airRelieveValve</v>
       </c>
     </row>
@@ -6517,7 +6531,7 @@
         <v>306</v>
       </c>
       <c r="G184" t="str">
-        <f>IF(B184="inspire",INSPIRE,IMKL) &amp; F184 &amp; "/" &amp; D184</f>
+        <f t="shared" si="2"/>
         <v>http://inspire.ec.europa.eu/codelist/WaterAppurtenanceTypeValue/storageFacility</v>
       </c>
     </row>
@@ -6532,7 +6546,7 @@
         <v>348</v>
       </c>
       <c r="D185" s="15" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="E185" s="16" t="s">
         <v>56</v>
@@ -6541,7 +6555,7 @@
         <v>306</v>
       </c>
       <c r="G185" t="str">
-        <f>IF(B185="inspire",INSPIRE,IMKL) &amp; F185 &amp; "/" &amp; D185</f>
+        <f t="shared" si="2"/>
         <v>http://inspire.ec.europa.eu/codelist/WaterAppurtenanceTypeValue/pumpStation</v>
       </c>
     </row>
@@ -6565,7 +6579,7 @@
         <v>306</v>
       </c>
       <c r="G186" t="str">
-        <f>IF(B186="inspire",INSPIRE,IMKL) &amp; F186 &amp; "/" &amp; D186</f>
+        <f t="shared" si="2"/>
         <v>http://inspire.ec.europa.eu/codelist/WaterAppurtenanceTypeValue/waterServicePoint</v>
       </c>
     </row>
@@ -6589,7 +6603,7 @@
         <v>306</v>
       </c>
       <c r="G187" t="str">
-        <f>IF(B187="inspire",INSPIRE,IMKL) &amp; F187 &amp; "/" &amp; D187</f>
+        <f t="shared" si="2"/>
         <v>http://inspire.ec.europa.eu/codelist/WaterAppurtenanceTypeValue/treatmentPlant</v>
       </c>
     </row>
@@ -6613,7 +6627,7 @@
         <v>262</v>
       </c>
       <c r="G188" t="str">
-        <f>IF(B188="inspire",INSPIRE,IMKL) &amp; F188 &amp; "/" &amp; D188</f>
+        <f t="shared" si="2"/>
         <v>http://www.geonovum.nl/imkl2015/1.0/def/WaterTypeValue/industrial</v>
       </c>
     </row>
@@ -6637,7 +6651,7 @@
         <v>262</v>
       </c>
       <c r="G189" t="str">
-        <f>IF(B189="inspire",INSPIRE,IMKL) &amp; F189 &amp; "/" &amp; D189</f>
+        <f t="shared" si="2"/>
         <v>http://www.geonovum.nl/imkl2015/1.0/def/WaterTypeValue/waste</v>
       </c>
     </row>
@@ -6661,7 +6675,7 @@
         <v>262</v>
       </c>
       <c r="G190" t="str">
-        <f>IF(B190="inspire",INSPIRE,IMKL) &amp; F190 &amp; "/" &amp; D190</f>
+        <f t="shared" si="2"/>
         <v>http://inspire.ec.europa.eu/codelist/WaterTypeValue/potable</v>
       </c>
     </row>
@@ -6685,7 +6699,7 @@
         <v>262</v>
       </c>
       <c r="G191" t="str">
-        <f>IF(B191="inspire",INSPIRE,IMKL) &amp; F191 &amp; "/" &amp; D191</f>
+        <f t="shared" si="2"/>
         <v>http://inspire.ec.europa.eu/codelist/WaterTypeValue/raw</v>
       </c>
     </row>
@@ -6709,7 +6723,7 @@
         <v>262</v>
       </c>
       <c r="G192" t="str">
-        <f>IF(B192="inspire",INSPIRE,IMKL) &amp; F192 &amp; "/" &amp; D192</f>
+        <f t="shared" si="2"/>
         <v>http://inspire.ec.europa.eu/codelist/WaterTypeValue/salt</v>
       </c>
     </row>
@@ -6733,7 +6747,7 @@
         <v>262</v>
       </c>
       <c r="G193" t="str">
-        <f>IF(B193="inspire",INSPIRE,IMKL) &amp; F193 &amp; "/" &amp; D193</f>
+        <f t="shared" si="2"/>
         <v>http://inspire.ec.europa.eu/codelist/WaterTypeValue/treated</v>
       </c>
     </row>
@@ -6753,13 +6767,13 @@
         <v>312</v>
       </c>
       <c r="G194" t="str">
-        <f>IF(B194="inspire",INSPIRE,IMKL) &amp; F194 &amp; "/" &amp; D194</f>
+        <f t="shared" ref="G194:G227" si="3">IF(B194="inspire",INSPIRE,IMKL) &amp; F194 &amp; "/" &amp; D194</f>
         <v>http://www.geonovum.nl/imkl2015/1.0/def/WaterAppurtenanceIMKLTypeValue/puntVanLevering</v>
       </c>
     </row>
     <row r="195" spans="1:7" ht="15" thickBot="1">
       <c r="A195" s="4" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="B195" s="21" t="s">
         <v>206</v>
@@ -6777,13 +6791,13 @@
         <v>263</v>
       </c>
       <c r="G195" t="str">
-        <f>IF(B195="inspire",INSPIRE,IMKL) &amp; F195 &amp; "/" &amp; D195</f>
+        <f t="shared" si="3"/>
         <v>http://www.geonovum.nl/imkl2015/1.0/def/SewerAppurtenanceTypeIMKLValue/gemaal</v>
       </c>
     </row>
     <row r="196" spans="1:7" ht="29" thickBot="1">
       <c r="A196" s="4" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="B196" s="21" t="s">
         <v>206</v>
@@ -6801,13 +6815,13 @@
         <v>263</v>
       </c>
       <c r="G196" t="str">
-        <f>IF(B196="inspire",INSPIRE,IMKL) &amp; F196 &amp; "/" &amp; D196</f>
+        <f t="shared" si="3"/>
         <v>http://www.geonovum.nl/imkl2015/1.0/def/SewerAppurtenanceTypeIMKLValue/infiltratievoorziening</v>
       </c>
     </row>
     <row r="197" spans="1:7" ht="15" thickBot="1">
       <c r="A197" s="4" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="B197" s="21" t="s">
         <v>206</v>
@@ -6825,13 +6839,13 @@
         <v>263</v>
       </c>
       <c r="G197" t="str">
-        <f>IF(B197="inspire",INSPIRE,IMKL) &amp; F197 &amp; "/" &amp; D197</f>
+        <f t="shared" si="3"/>
         <v>http://www.geonovum.nl/imkl2015/1.0/def/SewerAppurtenanceTypeIMKLValue/kolk</v>
       </c>
     </row>
     <row r="198" spans="1:7" ht="15" thickBot="1">
       <c r="A198" s="4" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="B198" s="21" t="s">
         <v>206</v>
@@ -6849,13 +6863,13 @@
         <v>263</v>
       </c>
       <c r="G198" t="str">
-        <f>IF(B198="inspire",INSPIRE,IMKL) &amp; F198 &amp; "/" &amp; D198</f>
+        <f t="shared" si="3"/>
         <v>http://www.geonovum.nl/imkl2015/1.0/def/SewerAppurtenanceTypeIMKLValue/kunstwerk</v>
       </c>
     </row>
     <row r="199" spans="1:7">
       <c r="A199" s="4" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="B199" s="21" t="s">
         <v>206</v>
@@ -6873,13 +6887,13 @@
         <v>263</v>
       </c>
       <c r="G199" t="str">
-        <f>IF(B199="inspire",INSPIRE,IMKL) &amp; F199 &amp; "/" &amp; D199</f>
+        <f t="shared" si="3"/>
         <v>http://www.geonovum.nl/imkl2015/1.0/def/SewerAppurtenanceTypeIMKLValue/reservoir</v>
       </c>
     </row>
     <row r="200" spans="1:7">
       <c r="A200" s="4" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="B200" s="21" t="s">
         <v>206</v>
@@ -6897,13 +6911,13 @@
         <v>263</v>
       </c>
       <c r="G200" t="str">
-        <f>IF(B200="inspire",INSPIRE,IMKL) &amp; F200 &amp; "/" &amp; D200</f>
+        <f t="shared" si="3"/>
         <v>http://www.geonovum.nl/imkl2015/1.0/def/SewerAppurtenanceTypeIMKLValue/uitlaatconstructie</v>
       </c>
     </row>
     <row r="201" spans="1:7" ht="15" thickBot="1">
       <c r="A201" s="4" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="B201" s="12" t="s">
         <v>28</v>
@@ -6921,13 +6935,13 @@
         <v>307</v>
       </c>
       <c r="G201" t="str">
-        <f>IF(B201="inspire",INSPIRE,IMKL) &amp; F201 &amp; "/" &amp; D201</f>
+        <f t="shared" si="3"/>
         <v>http://inspire.ec.europa.eu/codelist/SewerAppurtenanceTypeValue/connection</v>
       </c>
     </row>
     <row r="202" spans="1:7" ht="15" thickBot="1">
       <c r="A202" s="4" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="B202" s="12" t="s">
         <v>28</v>
@@ -6945,13 +6959,13 @@
         <v>307</v>
       </c>
       <c r="G202" t="str">
-        <f>IF(B202="inspire",INSPIRE,IMKL) &amp; F202 &amp; "/" &amp; D202</f>
+        <f t="shared" si="3"/>
         <v>http://inspire.ec.europa.eu/codelist/SewerAppurtenanceTypeValue/cleanOut</v>
       </c>
     </row>
     <row r="203" spans="1:7" ht="15" thickBot="1">
       <c r="A203" s="4" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="B203" s="12" t="s">
         <v>28</v>
@@ -6969,13 +6983,13 @@
         <v>307</v>
       </c>
       <c r="G203" t="str">
-        <f>IF(B203="inspire",INSPIRE,IMKL) &amp; F203 &amp; "/" &amp; D203</f>
+        <f t="shared" si="3"/>
         <v>http://inspire.ec.europa.eu/codelist/SewerAppurtenanceTypeValue/barrel</v>
       </c>
     </row>
     <row r="204" spans="1:7" ht="15" thickBot="1">
       <c r="A204" s="4" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="B204" s="12" t="s">
         <v>28</v>
@@ -6993,13 +7007,13 @@
         <v>307</v>
       </c>
       <c r="G204" t="str">
-        <f>IF(B204="inspire",INSPIRE,IMKL) &amp; F204 &amp; "/" &amp; D204</f>
+        <f t="shared" si="3"/>
         <v>http://inspire.ec.europa.eu/codelist/SewerAppurtenanceTypeValue/catchBasin</v>
       </c>
     </row>
     <row r="205" spans="1:7" ht="15" thickBot="1">
       <c r="A205" s="4" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="B205" s="12" t="s">
         <v>28</v>
@@ -7017,13 +7031,13 @@
         <v>307</v>
       </c>
       <c r="G205" t="str">
-        <f>IF(B205="inspire",INSPIRE,IMKL) &amp; F205 &amp; "/" &amp; D205</f>
+        <f t="shared" si="3"/>
         <v>http://inspire.ec.europa.eu/codelist/SewerAppurtenanceTypeValue/watertankOrChamber</v>
       </c>
     </row>
     <row r="206" spans="1:7" ht="15" thickBot="1">
       <c r="A206" s="4" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="B206" s="12" t="s">
         <v>28</v>
@@ -7041,13 +7055,13 @@
         <v>307</v>
       </c>
       <c r="G206" t="str">
-        <f>IF(B206="inspire",INSPIRE,IMKL) &amp; F206 &amp; "/" &amp; D206</f>
+        <f t="shared" si="3"/>
         <v>http://inspire.ec.europa.eu/codelist/SewerAppurtenanceTypeValue/specificStructure</v>
       </c>
     </row>
     <row r="207" spans="1:7">
       <c r="A207" s="4" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="B207" s="2" t="s">
         <v>82</v>
@@ -7065,13 +7079,13 @@
         <v>263</v>
       </c>
       <c r="G207" t="str">
-        <f>IF(B207="inspire",INSPIRE,IMKL) &amp; F207 &amp; "/" &amp; D207</f>
+        <f t="shared" si="3"/>
         <v>http://www.geonovum.nl/imkl2015/1.0/def/SewerAppurtenanceTypeIMKLValue/overstort</v>
       </c>
     </row>
     <row r="208" spans="1:7">
       <c r="A208" s="4" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="B208" s="1" t="s">
         <v>28</v>
@@ -7089,13 +7103,13 @@
         <v>307</v>
       </c>
       <c r="G208" t="str">
-        <f>IF(B208="inspire",INSPIRE,IMKL) &amp; F208 &amp; "/" &amp; D208</f>
+        <f t="shared" si="3"/>
         <v>http://inspire.ec.europa.eu/codelist/SewerAppurtenanceTypeValue/thrustProtection</v>
       </c>
     </row>
     <row r="209" spans="1:7">
       <c r="A209" s="4" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="B209" s="1" t="s">
         <v>28</v>
@@ -7113,13 +7127,13 @@
         <v>307</v>
       </c>
       <c r="G209" t="str">
-        <f>IF(B209="inspire",INSPIRE,IMKL) &amp; F209 &amp; "/" &amp; D209</f>
+        <f t="shared" si="3"/>
         <v>http://inspire.ec.europa.eu/codelist/SewerAppurtenanceTypeValue/tideGate</v>
       </c>
     </row>
     <row r="210" spans="1:7">
       <c r="A210" s="4" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="B210" s="1" t="s">
         <v>28</v>
@@ -7137,13 +7151,13 @@
         <v>307</v>
       </c>
       <c r="G210" t="str">
-        <f>IF(B210="inspire",INSPIRE,IMKL) &amp; F210 &amp; "/" &amp; D210</f>
+        <f t="shared" si="3"/>
         <v>http://inspire.ec.europa.eu/codelist/SewerAppurtenanceTypeValue/dischargeStructure</v>
       </c>
     </row>
     <row r="211" spans="1:7" ht="15" thickBot="1">
       <c r="A211" s="4" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="B211" s="12" t="s">
         <v>28</v>
@@ -7161,13 +7175,13 @@
         <v>264</v>
       </c>
       <c r="G211" t="str">
-        <f>IF(B211="inspire",INSPIRE,IMKL) &amp; F211 &amp; "/" &amp; D211</f>
+        <f t="shared" si="3"/>
         <v>http://inspire.ec.europa.eu/codelist/SewerWaterTypeValue/combined</v>
       </c>
     </row>
     <row r="212" spans="1:7" ht="15" thickBot="1">
       <c r="A212" s="4" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="B212" s="12" t="s">
         <v>28</v>
@@ -7185,13 +7199,13 @@
         <v>264</v>
       </c>
       <c r="G212" t="str">
-        <f>IF(B212="inspire",INSPIRE,IMKL) &amp; F212 &amp; "/" &amp; D212</f>
+        <f t="shared" si="3"/>
         <v>http://inspire.ec.europa.eu/codelist/SewerWaterTypeValue/reclaimed</v>
       </c>
     </row>
     <row r="213" spans="1:7" ht="15" thickBot="1">
       <c r="A213" s="4" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="B213" s="12" t="s">
         <v>28</v>
@@ -7209,13 +7223,13 @@
         <v>264</v>
       </c>
       <c r="G213" t="str">
-        <f>IF(B213="inspire",INSPIRE,IMKL) &amp; F213 &amp; "/" &amp; D213</f>
+        <f t="shared" si="3"/>
         <v>http://inspire.ec.europa.eu/codelist/SewerWaterTypeValue/sanitary</v>
       </c>
     </row>
     <row r="214" spans="1:7" ht="15" thickBot="1">
       <c r="A214" s="4" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="B214" s="12" t="s">
         <v>28</v>
@@ -7233,13 +7247,13 @@
         <v>264</v>
       </c>
       <c r="G214" t="str">
-        <f>IF(B214="inspire",INSPIRE,IMKL) &amp; F214 &amp; "/" &amp; D214</f>
+        <f t="shared" si="3"/>
         <v>http://inspire.ec.europa.eu/codelist/SewerWaterTypeValue/storm</v>
       </c>
     </row>
     <row r="215" spans="1:7">
       <c r="A215" s="4" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="C215" s="36" t="s">
         <v>348</v>
@@ -7254,7 +7268,7 @@
         <v>263</v>
       </c>
       <c r="G215" t="str">
-        <f>IF(B215="inspire",INSPIRE,IMKL) &amp; F215 &amp; "/" &amp; D215</f>
+        <f t="shared" si="3"/>
         <v>http://www.geonovum.nl/imkl2015/1.0/def/SewerAppurtenanceTypeIMKLValue/puntVanLevering</v>
       </c>
     </row>
@@ -7278,7 +7292,7 @@
         <v>263</v>
       </c>
       <c r="G216" t="str">
-        <f>IF(B216="inspire",INSPIRE,IMKL) &amp; F216 &amp; "/" &amp; D216</f>
+        <f t="shared" si="3"/>
         <v>http://www.geonovum.nl/imkl2015/1.0/def/SewerAppurtenanceTypeIMKLValue/compensator</v>
       </c>
     </row>
@@ -7302,7 +7316,7 @@
         <v>263</v>
       </c>
       <c r="G217" t="str">
-        <f>IF(B217="inspire",INSPIRE,IMKL) &amp; F217 &amp; "/" &amp; D217</f>
+        <f t="shared" si="3"/>
         <v>http://www.geonovum.nl/imkl2015/1.0/def/SewerAppurtenanceTypeIMKLValue/lekdetectiemeetpunt</v>
       </c>
     </row>
@@ -7326,7 +7340,7 @@
         <v>263</v>
       </c>
       <c r="G218" t="str">
-        <f>IF(B218="inspire",INSPIRE,IMKL) &amp; F218 &amp; "/" &amp; D218</f>
+        <f t="shared" si="3"/>
         <v>http://www.geonovum.nl/imkl2015/1.0/def/SewerAppurtenanceTypeIMKLValue/putten</v>
       </c>
     </row>
@@ -7350,7 +7364,7 @@
         <v>263</v>
       </c>
       <c r="G219" t="str">
-        <f>IF(B219="inspire",INSPIRE,IMKL) &amp; F219 &amp; "/" &amp; D219</f>
+        <f t="shared" si="3"/>
         <v>http://www.geonovum.nl/imkl2015/1.0/def/SewerAppurtenanceTypeIMKLValue/pompstation</v>
       </c>
     </row>
@@ -7374,7 +7388,7 @@
         <v>263</v>
       </c>
       <c r="G220" t="str">
-        <f>IF(B220="inspire",INSPIRE,IMKL) &amp; F220 &amp; "/" &amp; D220</f>
+        <f t="shared" si="3"/>
         <v>http://www.geonovum.nl/imkl2015/1.0/def/SewerAppurtenanceTypeIMKLValue/overdrachtsstation</v>
       </c>
     </row>
@@ -7389,7 +7403,7 @@
         <v>263</v>
       </c>
       <c r="G221" t="str">
-        <f>IF(B221="inspire",INSPIRE,IMKL) &amp; F221 &amp; "/" &amp; D221</f>
+        <f t="shared" si="3"/>
         <v>http://www.geonovum.nl/imkl2015/1.0/def/SewerAppurtenanceTypeIMKLValue/</v>
       </c>
     </row>
@@ -7413,7 +7427,7 @@
         <v>263</v>
       </c>
       <c r="G222" t="str">
-        <f>IF(B222="inspire",INSPIRE,IMKL) &amp; F222 &amp; "/" &amp; D222</f>
+        <f t="shared" si="3"/>
         <v>http://www.geonovum.nl/imkl2015/1.0/def/SewerAppurtenanceTypeIMKLValue/mantelbuis</v>
       </c>
     </row>
@@ -7437,7 +7451,7 @@
         <v>263</v>
       </c>
       <c r="G223" t="str">
-        <f>IF(B223="inspire",INSPIRE,IMKL) &amp; F223 &amp; "/" &amp; D223</f>
+        <f t="shared" si="3"/>
         <v>http://www.geonovum.nl/imkl2015/1.0/def/SewerAppurtenanceTypeIMKLValue/zinker</v>
       </c>
     </row>
@@ -7461,7 +7475,7 @@
         <v>263</v>
       </c>
       <c r="G224" t="str">
-        <f>IF(B224="inspire",INSPIRE,IMKL) &amp; F224 &amp; "/" &amp; D224</f>
+        <f t="shared" si="3"/>
         <v>http://www.geonovum.nl/imkl2015/1.0/def/SewerAppurtenanceTypeIMKLValue/inEnUittredepuntBoringen</v>
       </c>
     </row>
@@ -7485,7 +7499,7 @@
         <v>263</v>
       </c>
       <c r="G225" t="str">
-        <f>IF(B225="inspire",INSPIRE,IMKL) &amp; F225 &amp; "/" &amp; D225</f>
+        <f t="shared" si="3"/>
         <v>http://www.geonovum.nl/imkl2015/1.0/def/SewerAppurtenanceTypeIMKLValue/gestuurdeBoring</v>
       </c>
     </row>
@@ -7500,7 +7514,7 @@
         <v>263</v>
       </c>
       <c r="G226" t="str">
-        <f>IF(B226="inspire",INSPIRE,IMKL) &amp; F226 &amp; "/" &amp; D226</f>
+        <f t="shared" si="3"/>
         <v>http://www.geonovum.nl/imkl2015/1.0/def/SewerAppurtenanceTypeIMKLValue/</v>
       </c>
     </row>
@@ -7521,11 +7535,12 @@
         <v>263</v>
       </c>
       <c r="G227" t="str">
-        <f>IF(B227="inspire",INSPIRE,IMKL) &amp; F227 &amp; "/" &amp; D227</f>
+        <f t="shared" si="3"/>
         <v>http://www.geonovum.nl/imkl2015/1.0/def/SewerAppurtenanceTypeIMKLValue/puntVanLevering</v>
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:G227"/>
   <sortState ref="B2:F62">
     <sortCondition ref="C2:C62"/>
     <sortCondition ref="B2:B62"/>

</xml_diff>

<commit_message>
Nog twee fouten uit de lijst gehaald
En nog twee fouten gemarkeerd om op te lossen door Paul.
</commit_message>
<xml_diff>
--- a/3. waardelijsten/IMKL2015 - 0.9 waardelijsten.xlsx
+++ b/3. waardelijsten/IMKL2015 - 0.9 waardelijsten.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="26024"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="37560" yWindow="1240" windowWidth="28620" windowHeight="19480" tabRatio="645" activeTab="1"/>
+    <workbookView xWindow="38420" yWindow="720" windowWidth="25600" windowHeight="16060" tabRatio="645" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Toelichting" sheetId="8" r:id="rId1"/>
@@ -27,6 +27,64 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>Wilko Quak</author>
+  </authors>
+  <commentList>
+    <comment ref="D54" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t>Wilko Quak:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+CrossTheme is not known in INSPIRE</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F86" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t>Wilko Quak:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+This whole codelists seems to have dissappeared from INSPIRE. What now?</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1863" uniqueCount="383">
   <si>
@@ -1318,7 +1376,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="15" x14ac:knownFonts="1">
+  <fonts count="17" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1420,6 +1478,19 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -2231,11 +2302,12 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr filterMode="1" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:G227"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G91" sqref="G91"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="G238" sqref="G238"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -2271,7 +2343,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="2" spans="1:7" s="1" customFormat="1">
+    <row r="2" spans="1:7" s="1" customFormat="1" hidden="1">
       <c r="A2" s="1" t="s">
         <v>369</v>
       </c>
@@ -2295,7 +2367,7 @@
         <v>http://www.geonovum.nl/imkl2015/1.0/def/AnnotatieTypeValue/annotatiePijl</v>
       </c>
     </row>
-    <row r="3" spans="1:7" s="1" customFormat="1">
+    <row r="3" spans="1:7" s="1" customFormat="1" hidden="1">
       <c r="A3" s="1" t="s">
         <v>369</v>
       </c>
@@ -2316,7 +2388,7 @@
         <v>http://www.geonovum.nl/imkl2015/1.0/def/AnnotatieTypeValue/annotatieLijn</v>
       </c>
     </row>
-    <row r="4" spans="1:7" s="1" customFormat="1">
+    <row r="4" spans="1:7" s="1" customFormat="1" hidden="1">
       <c r="A4" s="1" t="s">
         <v>369</v>
       </c>
@@ -2337,7 +2409,7 @@
         <v>http://www.geonovum.nl/imkl2015/1.0/def/AnnotatieTypeValue/annotatieLabel</v>
       </c>
     </row>
-    <row r="5" spans="1:7" s="1" customFormat="1">
+    <row r="5" spans="1:7" s="1" customFormat="1" hidden="1">
       <c r="A5" s="1" t="s">
         <v>369</v>
       </c>
@@ -2358,7 +2430,7 @@
         <v>http://www.geonovum.nl/imkl2015/1.0/def/BestandMediaTypeValue/PNG</v>
       </c>
     </row>
-    <row r="6" spans="1:7" s="1" customFormat="1">
+    <row r="6" spans="1:7" s="1" customFormat="1" hidden="1">
       <c r="A6" s="1" t="s">
         <v>369</v>
       </c>
@@ -2379,7 +2451,7 @@
         <v>http://www.geonovum.nl/imkl2015/1.0/def/BestandMediaTypeValue/PDF</v>
       </c>
     </row>
-    <row r="7" spans="1:7" s="1" customFormat="1">
+    <row r="7" spans="1:7" s="1" customFormat="1" hidden="1">
       <c r="A7" s="1" t="s">
         <v>369</v>
       </c>
@@ -2400,7 +2472,7 @@
         <v>http://www.geonovum.nl/imkl2015/1.0/def/BestandMediaTypeValue/JPEG</v>
       </c>
     </row>
-    <row r="8" spans="1:7" s="1" customFormat="1">
+    <row r="8" spans="1:7" s="1" customFormat="1" hidden="1">
       <c r="A8" s="1" t="s">
         <v>369</v>
       </c>
@@ -2421,7 +2493,7 @@
         <v>http://www.geonovum.nl/imkl2015/1.0/def/BestandMediaTypeValue/TIFF</v>
       </c>
     </row>
-    <row r="9" spans="1:7" s="1" customFormat="1">
+    <row r="9" spans="1:7" s="1" customFormat="1" hidden="1">
       <c r="A9" s="1" t="s">
         <v>369</v>
       </c>
@@ -2443,7 +2515,7 @@
         <v>http://inspire.ec.europa.eu/codelist/ConditionOfFacilityValue/functional</v>
       </c>
     </row>
-    <row r="10" spans="1:7" s="1" customFormat="1">
+    <row r="10" spans="1:7" s="1" customFormat="1" hidden="1">
       <c r="A10" s="1" t="s">
         <v>369</v>
       </c>
@@ -2465,7 +2537,7 @@
         <v>http://inspire.ec.europa.eu/codelist/ConditionOfFacilityValue/projected</v>
       </c>
     </row>
-    <row r="11" spans="1:7" s="1" customFormat="1">
+    <row r="11" spans="1:7" s="1" customFormat="1" hidden="1">
       <c r="A11" s="1" t="s">
         <v>369</v>
       </c>
@@ -2487,7 +2559,7 @@
         <v>http://inspire.ec.europa.eu/codelist/ConditionOfFacilityValue/disused</v>
       </c>
     </row>
-    <row r="12" spans="1:7" s="1" customFormat="1" ht="15" customHeight="1">
+    <row r="12" spans="1:7" s="1" customFormat="1" ht="15" hidden="1" customHeight="1">
       <c r="A12" s="1" t="s">
         <v>369</v>
       </c>
@@ -2508,7 +2580,7 @@
         <v>http://www.geonovum.nl/imkl2015/1.0/def/NauwkeurigheidDiepteValue/tot30cm</v>
       </c>
     </row>
-    <row r="13" spans="1:7" s="1" customFormat="1" ht="15.75" customHeight="1">
+    <row r="13" spans="1:7" s="1" customFormat="1" ht="15.75" hidden="1" customHeight="1">
       <c r="A13" s="1" t="s">
         <v>369</v>
       </c>
@@ -2529,7 +2601,7 @@
         <v>http://www.geonovum.nl/imkl2015/1.0/def/NauwkeurigheidDiepteValue/tot50cm</v>
       </c>
     </row>
-    <row r="14" spans="1:7" s="1" customFormat="1" ht="15.75" customHeight="1">
+    <row r="14" spans="1:7" s="1" customFormat="1" ht="15.75" hidden="1" customHeight="1">
       <c r="A14" s="1" t="s">
         <v>369</v>
       </c>
@@ -2550,7 +2622,7 @@
         <v>http://www.geonovum.nl/imkl2015/1.0/def/NauwkeurigheidDiepteValue/tot100cm</v>
       </c>
     </row>
-    <row r="15" spans="1:7" s="1" customFormat="1" ht="14.25" customHeight="1">
+    <row r="15" spans="1:7" s="1" customFormat="1" ht="14.25" hidden="1" customHeight="1">
       <c r="A15" s="1" t="s">
         <v>369</v>
       </c>
@@ -2571,7 +2643,7 @@
         <v>http://www.geonovum.nl/imkl2015/1.0/def/NauwkeurigheidDiepteValue/onbekend</v>
       </c>
     </row>
-    <row r="16" spans="1:7" s="1" customFormat="1">
+    <row r="16" spans="1:7" s="1" customFormat="1" hidden="1">
       <c r="A16" s="1" t="s">
         <v>369</v>
       </c>
@@ -2592,7 +2664,7 @@
         <v>http://www.geonovum.nl/imkl2015/1.0/def/ExtraDetailInfoTypeValue/huisaansluiting</v>
       </c>
     </row>
-    <row r="17" spans="1:7" s="1" customFormat="1">
+    <row r="17" spans="1:7" s="1" customFormat="1" hidden="1">
       <c r="A17" s="1" t="s">
         <v>369</v>
       </c>
@@ -2613,7 +2685,7 @@
         <v>http://www.geonovum.nl/imkl2015/1.0/def/ExtraDetailInfoTypeValue/lengteprofiel</v>
       </c>
     </row>
-    <row r="18" spans="1:7" s="1" customFormat="1">
+    <row r="18" spans="1:7" s="1" customFormat="1" hidden="1">
       <c r="A18" s="1" t="s">
         <v>369</v>
       </c>
@@ -2634,7 +2706,7 @@
         <v>http://www.geonovum.nl/imkl2015/1.0/def/ExtraDetailInfoTypeValue/gestuurdeBoring</v>
       </c>
     </row>
-    <row r="19" spans="1:7" s="1" customFormat="1">
+    <row r="19" spans="1:7" s="1" customFormat="1" hidden="1">
       <c r="A19" s="1" t="s">
         <v>369</v>
       </c>
@@ -2655,7 +2727,7 @@
         <v>http://www.geonovum.nl/imkl2015/1.0/def/ExtraDetailInfoTypeValue/dwarsprofiel</v>
       </c>
     </row>
-    <row r="20" spans="1:7" s="1" customFormat="1" ht="12.75" customHeight="1">
+    <row r="20" spans="1:7" s="1" customFormat="1" ht="12.75" hidden="1" customHeight="1">
       <c r="A20" s="1" t="s">
         <v>369</v>
       </c>
@@ -2676,7 +2748,7 @@
         <v>http://www.geonovum.nl/imkl2015/1.0/def/ExtraTopografieTypeValue/eigen</v>
       </c>
     </row>
-    <row r="21" spans="1:7" s="1" customFormat="1">
+    <row r="21" spans="1:7" s="1" customFormat="1" hidden="1">
       <c r="A21" s="1" t="s">
         <v>369</v>
       </c>
@@ -2697,7 +2769,7 @@
         <v>http://www.geonovum.nl/imkl2015/1.0/def/ExtraTopografieTypeValue/ontwerp</v>
       </c>
     </row>
-    <row r="22" spans="1:7" s="1" customFormat="1" ht="14.25" customHeight="1">
+    <row r="22" spans="1:7" s="1" customFormat="1" ht="14.25" hidden="1" customHeight="1">
       <c r="A22" s="1" t="s">
         <v>369</v>
       </c>
@@ -2718,7 +2790,7 @@
         <v>http://www.geonovum.nl/imkl2015/1.0/def/NauwkeurigheidXYvalue/tot30cm</v>
       </c>
     </row>
-    <row r="23" spans="1:7" s="1" customFormat="1" ht="14.25" customHeight="1">
+    <row r="23" spans="1:7" s="1" customFormat="1" ht="14.25" hidden="1" customHeight="1">
       <c r="A23" s="1" t="s">
         <v>369</v>
       </c>
@@ -2739,7 +2811,7 @@
         <v>http://www.geonovum.nl/imkl2015/1.0/def/NauwkeurigheidXYvalue/tot50cm</v>
       </c>
     </row>
-    <row r="24" spans="1:7" s="1" customFormat="1">
+    <row r="24" spans="1:7" s="1" customFormat="1" hidden="1">
       <c r="A24" s="1" t="s">
         <v>369</v>
       </c>
@@ -2760,7 +2832,7 @@
         <v>http://www.geonovum.nl/imkl2015/1.0/def/NauwkeurigheidXYvalue/tot100cm</v>
       </c>
     </row>
-    <row r="25" spans="1:7" s="1" customFormat="1">
+    <row r="25" spans="1:7" s="1" customFormat="1" hidden="1">
       <c r="A25" s="1" t="s">
         <v>369</v>
       </c>
@@ -2781,7 +2853,7 @@
         <v>http://www.geonovum.nl/imkl2015/1.0/def/MaatvoeringsTypeValue/maatvoeringshulplijn</v>
       </c>
     </row>
-    <row r="26" spans="1:7" s="1" customFormat="1">
+    <row r="26" spans="1:7" s="1" customFormat="1" hidden="1">
       <c r="A26" s="1" t="s">
         <v>369</v>
       </c>
@@ -2802,7 +2874,7 @@
         <v>http://www.geonovum.nl/imkl2015/1.0/def/MaatvoeringsTypeValue/maatvoeringslijn</v>
       </c>
     </row>
-    <row r="27" spans="1:7" s="1" customFormat="1">
+    <row r="27" spans="1:7" s="1" customFormat="1" hidden="1">
       <c r="A27" s="1" t="s">
         <v>369</v>
       </c>
@@ -2823,7 +2895,7 @@
         <v>http://www.geonovum.nl/imkl2015/1.0/def/MaatvoeringsTypeValue/maatvoeringspijl</v>
       </c>
     </row>
-    <row r="28" spans="1:7">
+    <row r="28" spans="1:7" hidden="1">
       <c r="A28" s="1" t="s">
         <v>369</v>
       </c>
@@ -2845,7 +2917,7 @@
         <v>http://www.geonovum.nl/imkl2015/1.0/def/MaatvoeringsTypeValue/maatvoeringslabel</v>
       </c>
     </row>
-    <row r="29" spans="1:7">
+    <row r="29" spans="1:7" hidden="1">
       <c r="A29" s="1" t="s">
         <v>369</v>
       </c>
@@ -2869,7 +2941,7 @@
         <v>http://www.geonovum.nl/imkl2015/1.0/def/Thema/buisleidingGevaarlijkeInhoud</v>
       </c>
     </row>
-    <row r="30" spans="1:7">
+    <row r="30" spans="1:7" hidden="1">
       <c r="A30" s="1" t="s">
         <v>369</v>
       </c>
@@ -2890,7 +2962,7 @@
         <v>http://www.geonovum.nl/imkl2015/1.0/def/Thema/datatransport</v>
       </c>
     </row>
-    <row r="31" spans="1:7">
+    <row r="31" spans="1:7" hidden="1">
       <c r="A31" s="1" t="s">
         <v>369</v>
       </c>
@@ -2914,7 +2986,7 @@
         <v>http://www.geonovum.nl/imkl2015/1.0/def/Thema/gasLageDruk</v>
       </c>
     </row>
-    <row r="32" spans="1:7">
+    <row r="32" spans="1:7" hidden="1">
       <c r="A32" s="1" t="s">
         <v>369</v>
       </c>
@@ -2938,7 +3010,7 @@
         <v>http://www.geonovum.nl/imkl2015/1.0/def/Thema/gasHogeDruk</v>
       </c>
     </row>
-    <row r="33" spans="1:7">
+    <row r="33" spans="1:7" hidden="1">
       <c r="A33" s="1" t="s">
         <v>369</v>
       </c>
@@ -2962,7 +3034,7 @@
         <v>http://www.geonovum.nl/imkl2015/1.0/def/Thema/petrochemie</v>
       </c>
     </row>
-    <row r="34" spans="1:7">
+    <row r="34" spans="1:7" hidden="1">
       <c r="A34" s="1" t="s">
         <v>369</v>
       </c>
@@ -2986,7 +3058,7 @@
         <v>http://www.geonovum.nl/imkl2015/1.0/def/Thema/landelijkHoogspanningsnet</v>
       </c>
     </row>
-    <row r="35" spans="1:7">
+    <row r="35" spans="1:7" hidden="1">
       <c r="A35" s="1" t="s">
         <v>369</v>
       </c>
@@ -3010,7 +3082,7 @@
         <v>http://www.geonovum.nl/imkl2015/1.0/def/Thema/hoogspanning</v>
       </c>
     </row>
-    <row r="36" spans="1:7">
+    <row r="36" spans="1:7" hidden="1">
       <c r="A36" s="1" t="s">
         <v>369</v>
       </c>
@@ -3034,7 +3106,7 @@
         <v>http://www.geonovum.nl/imkl2015/1.0/def/Thema/laagspanning</v>
       </c>
     </row>
-    <row r="37" spans="1:7">
+    <row r="37" spans="1:7" hidden="1">
       <c r="A37" s="1" t="s">
         <v>369</v>
       </c>
@@ -3058,7 +3130,7 @@
         <v>http://www.geonovum.nl/imkl2015/1.0/def/Thema/middenspanning</v>
       </c>
     </row>
-    <row r="38" spans="1:7">
+    <row r="38" spans="1:7" hidden="1">
       <c r="A38" s="1" t="s">
         <v>369</v>
       </c>
@@ -3082,7 +3154,7 @@
         <v>http://www.geonovum.nl/imkl2015/1.0/def/Thema/rioolVrijverval</v>
       </c>
     </row>
-    <row r="39" spans="1:7">
+    <row r="39" spans="1:7" hidden="1">
       <c r="A39" s="1" t="s">
         <v>369</v>
       </c>
@@ -3106,7 +3178,7 @@
         <v>http://www.geonovum.nl/imkl2015/1.0/def/Thema/rioolOnderDruk</v>
       </c>
     </row>
-    <row r="40" spans="1:7">
+    <row r="40" spans="1:7" hidden="1">
       <c r="A40" s="1" t="s">
         <v>369</v>
       </c>
@@ -3130,7 +3202,7 @@
         <v>http://www.geonovum.nl/imkl2015/1.0/def/Thema/warmte</v>
       </c>
     </row>
-    <row r="41" spans="1:7">
+    <row r="41" spans="1:7" hidden="1">
       <c r="A41" s="1" t="s">
         <v>369</v>
       </c>
@@ -3154,7 +3226,7 @@
         <v>http://www.geonovum.nl/imkl2015/1.0/def/Thema/water</v>
       </c>
     </row>
-    <row r="42" spans="1:7">
+    <row r="42" spans="1:7" hidden="1">
       <c r="A42" s="1" t="s">
         <v>369</v>
       </c>
@@ -3178,7 +3250,7 @@
         <v>http://www.geonovum.nl/imkl2015/1.0/def/Thema/wees</v>
       </c>
     </row>
-    <row r="43" spans="1:7">
+    <row r="43" spans="1:7" hidden="1">
       <c r="A43" s="1" t="s">
         <v>369</v>
       </c>
@@ -3202,7 +3274,7 @@
         <v>http://www.geonovum.nl/imkl2015/1.0/def/Thema/overig</v>
       </c>
     </row>
-    <row r="44" spans="1:7">
+    <row r="44" spans="1:7" hidden="1">
       <c r="A44" s="1" t="s">
         <v>369</v>
       </c>
@@ -3223,7 +3295,7 @@
         <v>http://inspire.ec.europa.eu/codelist/UtilityDeliveryTypeValue/collection</v>
       </c>
     </row>
-    <row r="45" spans="1:7">
+    <row r="45" spans="1:7" hidden="1">
       <c r="A45" s="1" t="s">
         <v>369</v>
       </c>
@@ -3244,7 +3316,7 @@
         <v>http://inspire.ec.europa.eu/codelist/UtilityDeliveryTypeValue/distribution</v>
       </c>
     </row>
-    <row r="46" spans="1:7">
+    <row r="46" spans="1:7" hidden="1">
       <c r="A46" s="1" t="s">
         <v>369</v>
       </c>
@@ -3265,7 +3337,7 @@
         <v>http://inspire.ec.europa.eu/codelist/UtilityDeliveryTypeValue/private</v>
       </c>
     </row>
-    <row r="47" spans="1:7">
+    <row r="47" spans="1:7" hidden="1">
       <c r="A47" s="1" t="s">
         <v>369</v>
       </c>
@@ -3433,7 +3505,7 @@
         <v>http://inspire.ec.europa.eu/codelist/UtilityNetworkTypeValue/crossTheme</v>
       </c>
     </row>
-    <row r="55" spans="1:7">
+    <row r="55" spans="1:7" hidden="1">
       <c r="A55" s="1" t="s">
         <v>369</v>
       </c>
@@ -3454,7 +3526,7 @@
         <v>http://inspire.ec.europa.eu/codelist/WarningTypeValue/net</v>
       </c>
     </row>
-    <row r="56" spans="1:7">
+    <row r="56" spans="1:7" hidden="1">
       <c r="A56" s="1" t="s">
         <v>369</v>
       </c>
@@ -3475,7 +3547,7 @@
         <v>http://inspire.ec.europa.eu/codelist/WarningTypeValue/tape</v>
       </c>
     </row>
-    <row r="57" spans="1:7" ht="15" thickBot="1">
+    <row r="57" spans="1:7" hidden="1">
       <c r="A57" s="1" t="s">
         <v>369</v>
       </c>
@@ -3496,7 +3568,7 @@
         <v>http://inspire.ec.europa.eu/codelist/WarningTypeValue/concretePaving</v>
       </c>
     </row>
-    <row r="58" spans="1:7" ht="15" thickBot="1">
+    <row r="58" spans="1:7" ht="15" hidden="1" thickBot="1">
       <c r="A58" t="s">
         <v>370</v>
       </c>
@@ -3520,7 +3592,7 @@
         <v>http://www.geonovum.nl/imkl2015/1.0/def/ElectricityAppurtenanceTypeIMKLValue/aarding</v>
       </c>
     </row>
-    <row r="59" spans="1:7" ht="15" thickBot="1">
+    <row r="59" spans="1:7" ht="15" hidden="1" thickBot="1">
       <c r="A59" t="s">
         <v>370</v>
       </c>
@@ -3544,7 +3616,7 @@
         <v>http://www.geonovum.nl/imkl2015/1.0/def/ElectricityAppurtenanceTypeIMKLValue/mof</v>
       </c>
     </row>
-    <row r="60" spans="1:7" ht="15" thickBot="1">
+    <row r="60" spans="1:7" ht="15" hidden="1" thickBot="1">
       <c r="A60" t="s">
         <v>370</v>
       </c>
@@ -3568,7 +3640,7 @@
         <v>http://www.geonovum.nl/imkl2015/1.0/def/ElectricityAppurtenanceTypeIMKLValue/hoogteligging</v>
       </c>
     </row>
-    <row r="61" spans="1:7" ht="15" thickBot="1">
+    <row r="61" spans="1:7" ht="15" hidden="1" thickBot="1">
       <c r="A61" t="s">
         <v>370</v>
       </c>
@@ -3592,7 +3664,7 @@
         <v>http://www.geonovum.nl/imkl2015/1.0/def/ElectricityAppurtenanceTypeIMKLValue/Adrespunt</v>
       </c>
     </row>
-    <row r="62" spans="1:7" ht="15" thickBot="1">
+    <row r="62" spans="1:7" ht="15" hidden="1" thickBot="1">
       <c r="A62" t="s">
         <v>370</v>
       </c>
@@ -3616,7 +3688,7 @@
         <v>http://inspire.ec.europa.eu/codelist/ElectricityAppurtenanceTypeValue/connectionBox</v>
       </c>
     </row>
-    <row r="63" spans="1:7" ht="15" thickBot="1">
+    <row r="63" spans="1:7" ht="15" hidden="1" thickBot="1">
       <c r="A63" t="s">
         <v>370</v>
       </c>
@@ -3640,7 +3712,7 @@
         <v>http://inspire.ec.europa.eu/codelist/ElectricityAppurtenanceTypeValue/mainStation</v>
       </c>
     </row>
-    <row r="64" spans="1:7" ht="15" thickBot="1">
+    <row r="64" spans="1:7" ht="15" hidden="1" thickBot="1">
       <c r="A64" t="s">
         <v>370</v>
       </c>
@@ -3664,7 +3736,7 @@
         <v>http://inspire.ec.europa.eu/codelist/ElectricityAppurtenanceTypeValue/generator</v>
       </c>
     </row>
-    <row r="65" spans="1:7" ht="15" thickBot="1">
+    <row r="65" spans="1:7" ht="15" hidden="1" thickBot="1">
       <c r="A65" t="s">
         <v>370</v>
       </c>
@@ -3688,7 +3760,7 @@
         <v>http://inspire.ec.europa.eu/codelist/ElectricityAppurtenanceTypeValue/netStation</v>
       </c>
     </row>
-    <row r="66" spans="1:7" ht="15" thickBot="1">
+    <row r="66" spans="1:7" ht="15" hidden="1" thickBot="1">
       <c r="A66" t="s">
         <v>370</v>
       </c>
@@ -3712,7 +3784,7 @@
         <v>http://inspire.ec.europa.eu/codelist/ElectricityAppurtenanceTypeValue/subStation</v>
       </c>
     </row>
-    <row r="67" spans="1:7" ht="15" thickBot="1">
+    <row r="67" spans="1:7" ht="15" hidden="1" thickBot="1">
       <c r="A67" t="s">
         <v>370</v>
       </c>
@@ -3736,7 +3808,7 @@
         <v>http://inspire.ec.europa.eu/codelist/ElectricityAppurtenanceTypeValue/deliveryPoint</v>
       </c>
     </row>
-    <row r="68" spans="1:7" ht="15" thickBot="1">
+    <row r="68" spans="1:7" ht="15" hidden="1" thickBot="1">
       <c r="A68" t="s">
         <v>370</v>
       </c>
@@ -3760,7 +3832,7 @@
         <v>http://inspire.ec.europa.eu/codelist/ElectricityAppurtenanceTypeValue/streetLight</v>
       </c>
     </row>
-    <row r="69" spans="1:7" ht="15" thickBot="1">
+    <row r="69" spans="1:7" ht="15" hidden="1" thickBot="1">
       <c r="A69" t="s">
         <v>370</v>
       </c>
@@ -3781,7 +3853,7 @@
         <v>http://www.geonovum.nl/imkl2015/1.0/def/ElectricityAppurtenanceTypeIMKLValue/puntVanLevering</v>
       </c>
     </row>
-    <row r="70" spans="1:7" ht="15" thickBot="1">
+    <row r="70" spans="1:7" ht="15" hidden="1" thickBot="1">
       <c r="A70" t="s">
         <v>370</v>
       </c>
@@ -3802,7 +3874,7 @@
         <v>http://www.geonovum.nl/imkl2015/1.0/def/ElectricityAppurtenanceTypeIMKLValue/geulmof</v>
       </c>
     </row>
-    <row r="71" spans="1:7">
+    <row r="71" spans="1:7" hidden="1">
       <c r="A71" t="s">
         <v>370</v>
       </c>
@@ -3826,7 +3898,7 @@
         <v>http://www.geonovum.nl/imkl2015/1.0/def/ElectricityAppurtenanceTypeIMKLValue/kbMeetpunt</v>
       </c>
     </row>
-    <row r="72" spans="1:7">
+    <row r="72" spans="1:7" hidden="1">
       <c r="A72" t="s">
         <v>370</v>
       </c>
@@ -3850,7 +3922,7 @@
         <v>http://www.geonovum.nl/imkl2015/1.0/def/ElectricityAppurtenanceTypeIMKLValue/kbInstallatie</v>
       </c>
     </row>
-    <row r="73" spans="1:7">
+    <row r="73" spans="1:7" hidden="1">
       <c r="A73" t="s">
         <v>370</v>
       </c>
@@ -3874,7 +3946,7 @@
         <v>http://www.geonovum.nl/imkl2015/1.0/def/ElectricityAppurtenanceTypeIMKLValue/kbEindpunt</v>
       </c>
     </row>
-    <row r="74" spans="1:7">
+    <row r="74" spans="1:7" hidden="1">
       <c r="A74" t="s">
         <v>370</v>
       </c>
@@ -3898,7 +3970,7 @@
         <v>http://www.geonovum.nl/imkl2015/1.0/def/ElectricityAppurtenanceTypeIMKLValue/kbContact</v>
       </c>
     </row>
-    <row r="75" spans="1:7" ht="15" thickBot="1">
+    <row r="75" spans="1:7" ht="15" hidden="1" thickBot="1">
       <c r="A75" t="s">
         <v>370</v>
       </c>
@@ -3927,7 +3999,7 @@
         <v>371</v>
       </c>
       <c r="B76" s="13" t="s">
-        <v>28</v>
+        <v>206</v>
       </c>
       <c r="C76" s="13" t="s">
         <v>348</v>
@@ -3943,7 +4015,7 @@
       </c>
       <c r="G76" t="str">
         <f t="shared" si="1"/>
-        <v>http://inspire.ec.europa.eu/codelist/TelecommunicationsAppurtenanceIMKLTypeValue/antenna</v>
+        <v>http://www.geonovum.nl/imkl2015/1.0/def/TelecommunicationsAppurtenanceIMKLTypeValue/antenna</v>
       </c>
     </row>
     <row r="77" spans="1:7">
@@ -3951,7 +4023,7 @@
         <v>371</v>
       </c>
       <c r="B77" s="13" t="s">
-        <v>28</v>
+        <v>206</v>
       </c>
       <c r="C77" s="13" t="s">
         <v>348</v>
@@ -3967,7 +4039,7 @@
       </c>
       <c r="G77" t="str">
         <f t="shared" si="1"/>
-        <v>http://inspire.ec.europa.eu/codelist/TelecommunicationsAppurtenanceIMKLTypeValue/termination</v>
+        <v>http://www.geonovum.nl/imkl2015/1.0/def/TelecommunicationsAppurtenanceIMKLTypeValue/termination</v>
       </c>
     </row>
     <row r="78" spans="1:7">
@@ -4255,7 +4327,7 @@
         <v>http://www.geonovum.nl/imkl2015/1.0/def/TelecommunicationsAppurtenanceIMKLTypeValue/puntVanLevering</v>
       </c>
     </row>
-    <row r="90" spans="1:7" ht="15" thickBot="1">
+    <row r="90" spans="1:7" ht="15" hidden="1" thickBot="1">
       <c r="A90" t="s">
         <v>372</v>
       </c>
@@ -4279,7 +4351,7 @@
         <v>http://www.geonovum.nl/imkl2015/1.0/def/OilGasChemicalsAppurtenanceIMKLTypeValue/buis</v>
       </c>
     </row>
-    <row r="91" spans="1:7" ht="15" thickBot="1">
+    <row r="91" spans="1:7" ht="15" hidden="1" thickBot="1">
       <c r="A91" t="s">
         <v>372</v>
       </c>
@@ -4303,7 +4375,7 @@
         <v>http://www.geonovum.nl/imkl2015/1.0/def/OilGasChemicalsAppurtenanceIMKLTypeValue/bocht</v>
       </c>
     </row>
-    <row r="92" spans="1:7" ht="15" thickBot="1">
+    <row r="92" spans="1:7" ht="15" hidden="1" thickBot="1">
       <c r="A92" t="s">
         <v>372</v>
       </c>
@@ -4327,7 +4399,7 @@
         <v>http://www.geonovum.nl/imkl2015/1.0/def/OilGasChemicalsAppurtenanceIMKLTypeValue/tstuk</v>
       </c>
     </row>
-    <row r="93" spans="1:7" ht="15" thickBot="1">
+    <row r="93" spans="1:7" ht="15" hidden="1" thickBot="1">
       <c r="A93" t="s">
         <v>372</v>
       </c>
@@ -4351,7 +4423,7 @@
         <v>http://www.geonovum.nl/imkl2015/1.0/def/OilGasChemicalsAppurtenanceIMKLTypeValue/bodem</v>
       </c>
     </row>
-    <row r="94" spans="1:7" ht="15" thickBot="1">
+    <row r="94" spans="1:7" ht="15" hidden="1" thickBot="1">
       <c r="A94" t="s">
         <v>372</v>
       </c>
@@ -4375,7 +4447,7 @@
         <v>http://www.geonovum.nl/imkl2015/1.0/def/OilGasChemicalsAppurtenanceIMKLTypeValue/lasnok</v>
       </c>
     </row>
-    <row r="95" spans="1:7" ht="15" thickBot="1">
+    <row r="95" spans="1:7" ht="15" hidden="1" thickBot="1">
       <c r="A95" t="s">
         <v>372</v>
       </c>
@@ -4399,7 +4471,7 @@
         <v>http://www.geonovum.nl/imkl2015/1.0/def/OilGasChemicalsAppurtenanceIMKLTypeValue/expansiestuk</v>
       </c>
     </row>
-    <row r="96" spans="1:7" ht="15" thickBot="1">
+    <row r="96" spans="1:7" ht="15" hidden="1" thickBot="1">
       <c r="A96" t="s">
         <v>372</v>
       </c>
@@ -4423,7 +4495,7 @@
         <v>http://www.geonovum.nl/imkl2015/1.0/def/OilGasChemicalsAppurtenanceIMKLTypeValue/isolatieKoppeling</v>
       </c>
     </row>
-    <row r="97" spans="1:7" ht="15" thickBot="1">
+    <row r="97" spans="1:7" ht="15" hidden="1" thickBot="1">
       <c r="A97" t="s">
         <v>372</v>
       </c>
@@ -4447,7 +4519,7 @@
         <v>http://www.geonovum.nl/imkl2015/1.0/def/OilGasChemicalsAppurtenanceIMKLTypeValue/vloeistofvanger</v>
       </c>
     </row>
-    <row r="98" spans="1:7" ht="15" thickBot="1">
+    <row r="98" spans="1:7" ht="15" hidden="1" thickBot="1">
       <c r="A98" t="s">
         <v>372</v>
       </c>
@@ -4471,7 +4543,7 @@
         <v>http://www.geonovum.nl/imkl2015/1.0/def/OilGasChemicalsAppurtenanceIMKLTypeValue/Raaginrichting</v>
       </c>
     </row>
-    <row r="99" spans="1:7" ht="15" thickBot="1">
+    <row r="99" spans="1:7" ht="15" hidden="1" thickBot="1">
       <c r="A99" t="s">
         <v>372</v>
       </c>
@@ -4495,7 +4567,7 @@
         <v>http://www.geonovum.nl/imkl2015/1.0/def/OilGasChemicalsAppurtenanceIMKLTypeValue/algemeenGasTransportOnderdeel</v>
       </c>
     </row>
-    <row r="100" spans="1:7" ht="15" thickBot="1">
+    <row r="100" spans="1:7" ht="15" hidden="1" thickBot="1">
       <c r="A100" t="s">
         <v>372</v>
       </c>
@@ -4519,7 +4591,7 @@
         <v>http://www.geonovum.nl/imkl2015/1.0/def/OilGasChemicalsProductIMKLTypeValue/mud</v>
       </c>
     </row>
-    <row r="101" spans="1:7" ht="15" thickBot="1">
+    <row r="101" spans="1:7" ht="15" hidden="1" thickBot="1">
       <c r="A101" t="s">
         <v>372</v>
       </c>
@@ -4543,7 +4615,7 @@
         <v>http://www.geonovum.nl/imkl2015/1.0/def/OilGasChemicalsProductIMKLTypeValue/methanol</v>
       </c>
     </row>
-    <row r="102" spans="1:7">
+    <row r="102" spans="1:7" hidden="1">
       <c r="A102" t="s">
         <v>372</v>
       </c>
@@ -4567,7 +4639,7 @@
         <v>http://www.geonovum.nl/imkl2015/1.0/def/OilGasChemicalsProductIMKLTypeValue/emulsie</v>
       </c>
     </row>
-    <row r="103" spans="1:7" ht="15" thickBot="1">
+    <row r="103" spans="1:7" hidden="1">
       <c r="A103" t="s">
         <v>372</v>
       </c>
@@ -4591,7 +4663,7 @@
         <v>http://www.geonovum.nl/imkl2015/1.0/def/OilGasChemicalsProductIMKLTypeValue/glycol</v>
       </c>
     </row>
-    <row r="104" spans="1:7" ht="15" thickBot="1">
+    <row r="104" spans="1:7" ht="15" hidden="1" thickBot="1">
       <c r="A104" t="s">
         <v>372</v>
       </c>
@@ -4615,7 +4687,7 @@
         <v>http://www.geonovum.nl/imkl2015/1.0/def/OilGasChemicalsAppurtenanceIMKLTypeValue/hoogbouwkoppelpunt</v>
       </c>
     </row>
-    <row r="105" spans="1:7" ht="15" thickBot="1">
+    <row r="105" spans="1:7" ht="15" hidden="1" thickBot="1">
       <c r="A105" t="s">
         <v>372</v>
       </c>
@@ -4639,7 +4711,7 @@
         <v>http://www.geonovum.nl/imkl2015/1.0/def/OilGasChemicalsAppurtenanceIMKLTypeValue/ontluchting</v>
       </c>
     </row>
-    <row r="106" spans="1:7">
+    <row r="106" spans="1:7" hidden="1">
       <c r="A106" t="s">
         <v>372</v>
       </c>
@@ -4663,7 +4735,7 @@
         <v>http://www.geonovum.nl/imkl2015/1.0/def/OilGasChemicalsAppurtenanceIMKLTypeValue/aftakzadel</v>
       </c>
     </row>
-    <row r="107" spans="1:7">
+    <row r="107" spans="1:7" hidden="1">
       <c r="A107" t="s">
         <v>372</v>
       </c>
@@ -4687,7 +4759,7 @@
         <v>http://www.geonovum.nl/imkl2015/1.0/def/OilGasChemicalsAppurtenanceIMKLTypeValue/overgangsstuk</v>
       </c>
     </row>
-    <row r="108" spans="1:7">
+    <row r="108" spans="1:7" hidden="1">
       <c r="A108" t="s">
         <v>372</v>
       </c>
@@ -4711,7 +4783,7 @@
         <v>http://www.geonovum.nl/imkl2015/1.0/def/OilGasChemicalsAppurtenanceIMKLTypeValue/isolatiestuk</v>
       </c>
     </row>
-    <row r="109" spans="1:7">
+    <row r="109" spans="1:7" hidden="1">
       <c r="A109" t="s">
         <v>372</v>
       </c>
@@ -4735,7 +4807,7 @@
         <v>http://www.geonovum.nl/imkl2015/1.0/def/OilGasChemicalsAppurtenanceIMKLTypeValue/ontspanningselement</v>
       </c>
     </row>
-    <row r="110" spans="1:7">
+    <row r="110" spans="1:7" hidden="1">
       <c r="A110" t="s">
         <v>372</v>
       </c>
@@ -4759,7 +4831,7 @@
         <v>http://www.geonovum.nl/imkl2015/1.0/def/OilGasChemicalsAppurtenanceIMKLTypeValue/hoogteligging</v>
       </c>
     </row>
-    <row r="111" spans="1:7">
+    <row r="111" spans="1:7" hidden="1">
       <c r="A111" t="s">
         <v>372</v>
       </c>
@@ -4783,7 +4855,7 @@
         <v>http://www.geonovum.nl/imkl2015/1.0/def/OilGasChemicalsAppurtenanceIMKLTypeValue/adrespunt</v>
       </c>
     </row>
-    <row r="112" spans="1:7">
+    <row r="112" spans="1:7" hidden="1">
       <c r="A112" t="s">
         <v>372</v>
       </c>
@@ -4807,7 +4879,7 @@
         <v>http://www.geonovum.nl/imkl2015/1.0/def/OilGasChemicalsAppurtenanceIMKLTypeValue/eindkap</v>
       </c>
     </row>
-    <row r="113" spans="1:7">
+    <row r="113" spans="1:7" hidden="1">
       <c r="A113" t="s">
         <v>372</v>
       </c>
@@ -4831,7 +4903,7 @@
         <v>http://www.geonovum.nl/imkl2015/1.0/def/OilGasChemicalsAppurtenanceIMKLTypeValue/verloopstuk</v>
       </c>
     </row>
-    <row r="114" spans="1:7">
+    <row r="114" spans="1:7" hidden="1">
       <c r="A114" t="s">
         <v>372</v>
       </c>
@@ -4855,7 +4927,7 @@
         <v>http://www.geonovum.nl/imkl2015/1.0/def/OilGasChemicalsAppurtenanceIMKLTypeValue/afsluiter</v>
       </c>
     </row>
-    <row r="115" spans="1:7">
+    <row r="115" spans="1:7" hidden="1">
       <c r="A115" t="s">
         <v>372</v>
       </c>
@@ -4879,7 +4951,7 @@
         <v>http://www.geonovum.nl/imkl2015/1.0/def/OilGasChemicalsAppurtenanceIMKLTypeValue/meetpunt</v>
       </c>
     </row>
-    <row r="116" spans="1:7">
+    <row r="116" spans="1:7" hidden="1">
       <c r="A116" t="s">
         <v>372</v>
       </c>
@@ -4903,7 +4975,7 @@
         <v>http://www.geonovum.nl/imkl2015/1.0/def/OilGasChemicalsAppurtenanceIMKLTypeValue/sifon</v>
       </c>
     </row>
-    <row r="117" spans="1:7">
+    <row r="117" spans="1:7" hidden="1">
       <c r="A117" t="s">
         <v>372</v>
       </c>
@@ -4927,7 +4999,7 @@
         <v>http://www.geonovum.nl/imkl2015/1.0/def/OilGasChemicalsAppurtenanceIMKLTypeValue/blaasgat</v>
       </c>
     </row>
-    <row r="118" spans="1:7">
+    <row r="118" spans="1:7" hidden="1">
       <c r="A118" t="s">
         <v>372</v>
       </c>
@@ -4951,7 +5023,7 @@
         <v>http://www.geonovum.nl/imkl2015/1.0/def/OilGasChemicalsAppurtenanceIMKLTypeValue/kbMeetpunt</v>
       </c>
     </row>
-    <row r="119" spans="1:7">
+    <row r="119" spans="1:7" hidden="1">
       <c r="A119" t="s">
         <v>372</v>
       </c>
@@ -4975,7 +5047,7 @@
         <v>http://inspire.ec.europa.eu/codelist/OilGasChemicalsAppurtenanceTypeValue/gasStation</v>
       </c>
     </row>
-    <row r="120" spans="1:7">
+    <row r="120" spans="1:7" hidden="1">
       <c r="A120" t="s">
         <v>372</v>
       </c>
@@ -4999,7 +5071,7 @@
         <v>http://inspire.ec.europa.eu/codelist/OilGasChemicalsAppurtenanceTypeValue/oilGasChemicalsNode</v>
       </c>
     </row>
-    <row r="121" spans="1:7">
+    <row r="121" spans="1:7" hidden="1">
       <c r="A121" t="s">
         <v>372</v>
       </c>
@@ -5023,7 +5095,7 @@
         <v>http://inspire.ec.europa.eu/codelist/OilGasChemicalsAppurtenanceTypeValue/marker</v>
       </c>
     </row>
-    <row r="122" spans="1:7">
+    <row r="122" spans="1:7" hidden="1">
       <c r="A122" t="s">
         <v>372</v>
       </c>
@@ -5047,7 +5119,7 @@
         <v>http://inspire.ec.europa.eu/codelist/OilGasChemicalsAppurtenanceTypeValue/deliveryPoint</v>
       </c>
     </row>
-    <row r="123" spans="1:7">
+    <row r="123" spans="1:7" hidden="1">
       <c r="A123" t="s">
         <v>372</v>
       </c>
@@ -5071,7 +5143,7 @@
         <v>http://inspire.ec.europa.eu/codelist/OilGasChemicalsAppurtenanceTypeValue/terminal</v>
       </c>
     </row>
-    <row r="124" spans="1:7">
+    <row r="124" spans="1:7" hidden="1">
       <c r="A124" t="s">
         <v>372</v>
       </c>
@@ -5095,7 +5167,7 @@
         <v>http://inspire.ec.europa.eu/codelist/OilGasChemicalsAppurtenanceTypeValue/pump</v>
       </c>
     </row>
-    <row r="125" spans="1:7">
+    <row r="125" spans="1:7" hidden="1">
       <c r="A125" t="s">
         <v>372</v>
       </c>
@@ -5119,7 +5191,7 @@
         <v>http://inspire.ec.europa.eu/codelist/OilGasChemicalsAppurtenanceTypeValue/pumpingStation</v>
       </c>
     </row>
-    <row r="126" spans="1:7">
+    <row r="126" spans="1:7" hidden="1">
       <c r="A126" t="s">
         <v>372</v>
       </c>
@@ -5143,7 +5215,7 @@
         <v>http://inspire.ec.europa.eu/codelist/OilGasChemicalsAppurtenanceTypeValue/productionRegion</v>
       </c>
     </row>
-    <row r="127" spans="1:7">
+    <row r="127" spans="1:7" hidden="1">
       <c r="A127" t="s">
         <v>372</v>
       </c>
@@ -5167,7 +5239,7 @@
         <v>http://inspire.ec.europa.eu/codelist/OilGasChemicalsAppurtenanceTypeValue/storage</v>
       </c>
     </row>
-    <row r="128" spans="1:7">
+    <row r="128" spans="1:7" hidden="1">
       <c r="A128" t="s">
         <v>372</v>
       </c>
@@ -5191,7 +5263,7 @@
         <v>http://inspire.ec.europa.eu/codelist/OilGasChemicalsProductTypeValue/naturalGas</v>
       </c>
     </row>
-    <row r="129" spans="1:7">
+    <row r="129" spans="1:7" hidden="1">
       <c r="A129" t="s">
         <v>372</v>
       </c>
@@ -5215,7 +5287,7 @@
         <v>http://www.geonovum.nl/imkl2015/1.0/def/OilGasChemicalsProductIMKLTypeValue/bioGas</v>
       </c>
     </row>
-    <row r="130" spans="1:7">
+    <row r="130" spans="1:7" hidden="1">
       <c r="A130" t="s">
         <v>372</v>
       </c>
@@ -5239,7 +5311,7 @@
         <v>http://www.geonovum.nl/imkl2015/1.0/def/OilGasChemicalsProductTypeValue/accetone</v>
       </c>
     </row>
-    <row r="131" spans="1:7">
+    <row r="131" spans="1:7" hidden="1">
       <c r="A131" t="s">
         <v>372</v>
       </c>
@@ -5263,7 +5335,7 @@
         <v>http://www.geonovum.nl/imkl2015/1.0/def/OilGasChemicalsProductTypeValue/air</v>
       </c>
     </row>
-    <row r="132" spans="1:7">
+    <row r="132" spans="1:7" hidden="1">
       <c r="A132" t="s">
         <v>372</v>
       </c>
@@ -5287,7 +5359,7 @@
         <v>http://www.geonovum.nl/imkl2015/1.0/def/OilGasChemicalsProductTypeValue/argon</v>
       </c>
     </row>
-    <row r="133" spans="1:7">
+    <row r="133" spans="1:7" hidden="1">
       <c r="A133" t="s">
         <v>372</v>
       </c>
@@ -5311,7 +5383,7 @@
         <v>http://www.geonovum.nl/imkl2015/1.0/def/OilGasChemicalsProductTypeValue/butadiene1.2</v>
       </c>
     </row>
-    <row r="134" spans="1:7">
+    <row r="134" spans="1:7" hidden="1">
       <c r="A134" t="s">
         <v>372</v>
       </c>
@@ -5335,7 +5407,7 @@
         <v>http://www.geonovum.nl/imkl2015/1.0/def/OilGasChemicalsProductTypeValue/butadiene1.3</v>
       </c>
     </row>
-    <row r="135" spans="1:7">
+    <row r="135" spans="1:7" hidden="1">
       <c r="A135" t="s">
         <v>372</v>
       </c>
@@ -5359,7 +5431,7 @@
         <v>http://www.geonovum.nl/imkl2015/1.0/def/OilGasChemicalsProductTypeValue/butane</v>
       </c>
     </row>
-    <row r="136" spans="1:7">
+    <row r="136" spans="1:7" hidden="1">
       <c r="A136" t="s">
         <v>372</v>
       </c>
@@ -5383,7 +5455,7 @@
         <v>http://www.geonovum.nl/imkl2015/1.0/def/OilGasChemicalsProductTypeValue/carbonMonoxide</v>
       </c>
     </row>
-    <row r="137" spans="1:7">
+    <row r="137" spans="1:7" hidden="1">
       <c r="A137" t="s">
         <v>372</v>
       </c>
@@ -5407,7 +5479,7 @@
         <v>http://www.geonovum.nl/imkl2015/1.0/def/OilGasChemicalsProductTypeValue/chlorine</v>
       </c>
     </row>
-    <row r="138" spans="1:7">
+    <row r="138" spans="1:7" hidden="1">
       <c r="A138" t="s">
         <v>372</v>
       </c>
@@ -5431,7 +5503,7 @@
         <v>http://www.geonovum.nl/imkl2015/1.0/def/OilGasChemicalsProductTypeValue/concrete</v>
       </c>
     </row>
-    <row r="139" spans="1:7">
+    <row r="139" spans="1:7" hidden="1">
       <c r="A139" t="s">
         <v>372</v>
       </c>
@@ -5455,7 +5527,7 @@
         <v>http://www.geonovum.nl/imkl2015/1.0/def/OilGasChemicalsProductTypeValue/crude</v>
       </c>
     </row>
-    <row r="140" spans="1:7">
+    <row r="140" spans="1:7" hidden="1">
       <c r="A140" t="s">
         <v>372</v>
       </c>
@@ -5479,7 +5551,7 @@
         <v>http://www.geonovum.nl/imkl2015/1.0/def/OilGasChemicalsProductTypeValue/dichloroethane</v>
       </c>
     </row>
-    <row r="141" spans="1:7">
+    <row r="141" spans="1:7" hidden="1">
       <c r="A141" t="s">
         <v>372</v>
       </c>
@@ -5503,7 +5575,7 @@
         <v>http://www.geonovum.nl/imkl2015/1.0/def/OilGasChemicalsProductTypeValue/diesel</v>
       </c>
     </row>
-    <row r="142" spans="1:7">
+    <row r="142" spans="1:7" hidden="1">
       <c r="A142" t="s">
         <v>372</v>
       </c>
@@ -5527,7 +5599,7 @@
         <v>http://www.geonovum.nl/imkl2015/1.0/def/OilGasChemicalsProductTypeValue/ethylene</v>
       </c>
     </row>
-    <row r="143" spans="1:7">
+    <row r="143" spans="1:7" hidden="1">
       <c r="A143" t="s">
         <v>372</v>
       </c>
@@ -5551,7 +5623,7 @@
         <v>http://www.geonovum.nl/imkl2015/1.0/def/OilGasChemicalsProductTypeValue/gasFabricationOfCocs</v>
       </c>
     </row>
-    <row r="144" spans="1:7">
+    <row r="144" spans="1:7" hidden="1">
       <c r="A144" t="s">
         <v>372</v>
       </c>
@@ -5575,7 +5647,7 @@
         <v>http://www.geonovum.nl/imkl2015/1.0/def/OilGasChemicalsProductTypeValue/gasHFx</v>
       </c>
     </row>
-    <row r="145" spans="1:7">
+    <row r="145" spans="1:7" hidden="1">
       <c r="A145" t="s">
         <v>372</v>
       </c>
@@ -5599,7 +5671,7 @@
         <v>http://www.geonovum.nl/imkl2015/1.0/def/OilGasChemicalsProductTypeValue/gasoil</v>
       </c>
     </row>
-    <row r="146" spans="1:7">
+    <row r="146" spans="1:7" hidden="1">
       <c r="A146" t="s">
         <v>372</v>
       </c>
@@ -5623,7 +5695,7 @@
         <v>http://www.geonovum.nl/imkl2015/1.0/def/OilGasChemicalsProductTypeValue/hydrogen</v>
       </c>
     </row>
-    <row r="147" spans="1:7">
+    <row r="147" spans="1:7" hidden="1">
       <c r="A147" t="s">
         <v>372</v>
       </c>
@@ -5647,7 +5719,7 @@
         <v>http://www.geonovum.nl/imkl2015/1.0/def/OilGasChemicalsProductTypeValue/isobutane</v>
       </c>
     </row>
-    <row r="148" spans="1:7">
+    <row r="148" spans="1:7" hidden="1">
       <c r="A148" t="s">
         <v>372</v>
       </c>
@@ -5671,7 +5743,7 @@
         <v>http://www.geonovum.nl/imkl2015/1.0/def/OilGasChemicalsProductTypeValue/JET-A1</v>
       </c>
     </row>
-    <row r="149" spans="1:7">
+    <row r="149" spans="1:7" hidden="1">
       <c r="A149" t="s">
         <v>372</v>
       </c>
@@ -5695,7 +5767,7 @@
         <v>http://www.geonovum.nl/imkl2015/1.0/def/OilGasChemicalsProductTypeValue/kerosene</v>
       </c>
     </row>
-    <row r="150" spans="1:7">
+    <row r="150" spans="1:7" hidden="1">
       <c r="A150" t="s">
         <v>372</v>
       </c>
@@ -5719,7 +5791,7 @@
         <v>http://www.geonovum.nl/imkl2015/1.0/def/OilGasChemicalsProductTypeValue/liquidAmmonia</v>
       </c>
     </row>
-    <row r="151" spans="1:7">
+    <row r="151" spans="1:7" hidden="1">
       <c r="A151" t="s">
         <v>372</v>
       </c>
@@ -5743,7 +5815,7 @@
         <v>http://www.geonovum.nl/imkl2015/1.0/def/OilGasChemicalsProductTypeValue/liquidHydrocarbon</v>
       </c>
     </row>
-    <row r="152" spans="1:7">
+    <row r="152" spans="1:7" hidden="1">
       <c r="A152" t="s">
         <v>372</v>
       </c>
@@ -5767,7 +5839,7 @@
         <v>http://www.geonovum.nl/imkl2015/1.0/def/OilGasChemicalsProductTypeValue/multiProduct</v>
       </c>
     </row>
-    <row r="153" spans="1:7">
+    <row r="153" spans="1:7" hidden="1">
       <c r="A153" t="s">
         <v>372</v>
       </c>
@@ -5791,7 +5863,7 @@
         <v>http://www.geonovum.nl/imkl2015/1.0/def/OilGasChemicalsProductTypeValue/MVC</v>
       </c>
     </row>
-    <row r="154" spans="1:7">
+    <row r="154" spans="1:7" hidden="1">
       <c r="A154" t="s">
         <v>372</v>
       </c>
@@ -5815,7 +5887,7 @@
         <v>http://www.geonovum.nl/imkl2015/1.0/def/OilGasChemicalsProductTypeValue/nitrogen</v>
       </c>
     </row>
-    <row r="155" spans="1:7">
+    <row r="155" spans="1:7" hidden="1">
       <c r="A155" t="s">
         <v>372</v>
       </c>
@@ -5839,7 +5911,7 @@
         <v>http://www.geonovum.nl/imkl2015/1.0/def/OilGasChemicalsProductTypeValue/oxygen</v>
       </c>
     </row>
-    <row r="156" spans="1:7">
+    <row r="156" spans="1:7" hidden="1">
       <c r="A156" t="s">
         <v>372</v>
       </c>
@@ -5863,7 +5935,7 @@
         <v>http://www.geonovum.nl/imkl2015/1.0/def/OilGasChemicalsProductTypeValue/phenol</v>
       </c>
     </row>
-    <row r="157" spans="1:7">
+    <row r="157" spans="1:7" hidden="1">
       <c r="A157" t="s">
         <v>372</v>
       </c>
@@ -5887,7 +5959,7 @@
         <v>http://www.geonovum.nl/imkl2015/1.0/def/OilGasChemicalsProductTypeValue/propane</v>
       </c>
     </row>
-    <row r="158" spans="1:7">
+    <row r="158" spans="1:7" hidden="1">
       <c r="A158" t="s">
         <v>372</v>
       </c>
@@ -5911,7 +5983,7 @@
         <v>http://www.geonovum.nl/imkl2015/1.0/def/OilGasChemicalsProductTypeValue/propylene</v>
       </c>
     </row>
-    <row r="159" spans="1:7">
+    <row r="159" spans="1:7" hidden="1">
       <c r="A159" t="s">
         <v>372</v>
       </c>
@@ -5935,7 +6007,7 @@
         <v>http://www.geonovum.nl/imkl2015/1.0/def/OilGasChemicalsProductTypeValue/saltWater</v>
       </c>
     </row>
-    <row r="160" spans="1:7">
+    <row r="160" spans="1:7" hidden="1">
       <c r="A160" t="s">
         <v>372</v>
       </c>
@@ -5959,7 +6031,7 @@
         <v>http://www.geonovum.nl/imkl2015/1.0/def/OilGasChemicalsProductTypeValue/saumur</v>
       </c>
     </row>
-    <row r="161" spans="1:7">
+    <row r="161" spans="1:7" hidden="1">
       <c r="A161" t="s">
         <v>372</v>
       </c>
@@ -5983,7 +6055,7 @@
         <v>http://www.geonovum.nl/imkl2015/1.0/def/OilGasChemicalsProductTypeValue/sand</v>
       </c>
     </row>
-    <row r="162" spans="1:7">
+    <row r="162" spans="1:7" hidden="1">
       <c r="A162" t="s">
         <v>372</v>
       </c>
@@ -6007,7 +6079,7 @@
         <v>http://www.geonovum.nl/imkl2015/1.0/def/OilGasChemicalsProductTypeValue/tetrachloroide</v>
       </c>
     </row>
-    <row r="163" spans="1:7">
+    <row r="163" spans="1:7" hidden="1">
       <c r="A163" t="s">
         <v>372</v>
       </c>
@@ -6031,7 +6103,7 @@
         <v>http://www.geonovum.nl/imkl2015/1.0/def/OilGasChemicalsProductTypeValue/unknown</v>
       </c>
     </row>
-    <row r="164" spans="1:7">
+    <row r="164" spans="1:7" hidden="1">
       <c r="A164" t="s">
         <v>372</v>
       </c>
@@ -6055,7 +6127,7 @@
         <v>http://www.geonovum.nl/imkl2015/1.0/def/OilGasChemicalsProductTypeValue/water</v>
       </c>
     </row>
-    <row r="165" spans="1:7" ht="15" thickBot="1">
+    <row r="165" spans="1:7" hidden="1">
       <c r="A165" t="s">
         <v>372</v>
       </c>
@@ -6079,7 +6151,7 @@
         <v>http://www.geonovum.nl/imkl2015/1.0/def/OilGasChemicalsProductTypeValue/empty</v>
       </c>
     </row>
-    <row r="166" spans="1:7" ht="15" thickBot="1">
+    <row r="166" spans="1:7" ht="15" hidden="1" thickBot="1">
       <c r="A166" s="4" t="s">
         <v>114</v>
       </c>
@@ -6103,7 +6175,7 @@
         <v>http://www.geonovum.nl/imkl2015/1.0/def/WaterAppurtenanceTypeIMKLValue/afsluiter</v>
       </c>
     </row>
-    <row r="167" spans="1:7" ht="15" thickBot="1">
+    <row r="167" spans="1:7" ht="15" hidden="1" thickBot="1">
       <c r="A167" s="4" t="s">
         <v>114</v>
       </c>
@@ -6127,7 +6199,7 @@
         <v>http://www.geonovum.nl/imkl2015/1.0/def/WaterAppurtenanceTypeIMKLValue/diameterovergang</v>
       </c>
     </row>
-    <row r="168" spans="1:7" ht="15" thickBot="1">
+    <row r="168" spans="1:7" ht="15" hidden="1" thickBot="1">
       <c r="A168" s="4" t="s">
         <v>114</v>
       </c>
@@ -6151,7 +6223,7 @@
         <v>http://www.geonovum.nl/imkl2015/1.0/def/WaterAppurtenanceTypeIMKLValue/materiaalovergang</v>
       </c>
     </row>
-    <row r="169" spans="1:7" ht="15" thickBot="1">
+    <row r="169" spans="1:7" ht="15" hidden="1" thickBot="1">
       <c r="A169" s="4" t="s">
         <v>114</v>
       </c>
@@ -6175,7 +6247,7 @@
         <v>http://www.geonovum.nl/imkl2015/1.0/def/WaterAppurtenanceTypeIMKLValue/eindpunt</v>
       </c>
     </row>
-    <row r="170" spans="1:7" ht="15" thickBot="1">
+    <row r="170" spans="1:7" ht="15" hidden="1" thickBot="1">
       <c r="A170" s="4" t="s">
         <v>114</v>
       </c>
@@ -6199,7 +6271,7 @@
         <v>http://www.geonovum.nl/imkl2015/1.0/def/WaterAppurtenanceTypeIMKLValue/blindflens</v>
       </c>
     </row>
-    <row r="171" spans="1:7" ht="15" thickBot="1">
+    <row r="171" spans="1:7" ht="15" hidden="1" thickBot="1">
       <c r="A171" s="4" t="s">
         <v>114</v>
       </c>
@@ -6223,7 +6295,7 @@
         <v>http://inspire.ec.europa.eu/codelist/WaterAppurtenanceTypeValue/checkValve</v>
       </c>
     </row>
-    <row r="172" spans="1:7" ht="15" thickBot="1">
+    <row r="172" spans="1:7" ht="15" hidden="1" thickBot="1">
       <c r="A172" s="4" t="s">
         <v>114</v>
       </c>
@@ -6247,7 +6319,7 @@
         <v>http://inspire.ec.europa.eu/codelist/WaterAppurtenanceTypeValue/waterExhaustPoint</v>
       </c>
     </row>
-    <row r="173" spans="1:7" ht="15" thickBot="1">
+    <row r="173" spans="1:7" ht="15" hidden="1" thickBot="1">
       <c r="A173" s="4" t="s">
         <v>114</v>
       </c>
@@ -6271,7 +6343,7 @@
         <v>http://inspire.ec.europa.eu/codelist/WaterAppurtenanceTypeValue/waterDischargePoint</v>
       </c>
     </row>
-    <row r="174" spans="1:7" ht="15" thickBot="1">
+    <row r="174" spans="1:7" ht="15" hidden="1" thickBot="1">
       <c r="A174" s="4" t="s">
         <v>114</v>
       </c>
@@ -6295,7 +6367,7 @@
         <v>http://inspire.ec.europa.eu/codelist/WaterAppurtenanceTypeValue/anode</v>
       </c>
     </row>
-    <row r="175" spans="1:7" ht="15" thickBot="1">
+    <row r="175" spans="1:7" ht="15" hidden="1" thickBot="1">
       <c r="A175" s="4" t="s">
         <v>114</v>
       </c>
@@ -6319,7 +6391,7 @@
         <v>http://inspire.ec.europa.eu/codelist/WaterAppurtenanceTypeValue/fireHydrant</v>
       </c>
     </row>
-    <row r="176" spans="1:7" ht="15" thickBot="1">
+    <row r="176" spans="1:7" ht="15" hidden="1" thickBot="1">
       <c r="A176" s="4" t="s">
         <v>114</v>
       </c>
@@ -6343,7 +6415,7 @@
         <v>http://inspire.ec.europa.eu/codelist/WaterAppurtenanceTypeValue/well</v>
       </c>
     </row>
-    <row r="177" spans="1:7" ht="15" thickBot="1">
+    <row r="177" spans="1:7" ht="15" hidden="1" thickBot="1">
       <c r="A177" s="4" t="s">
         <v>114</v>
       </c>
@@ -6367,7 +6439,7 @@
         <v>http://inspire.ec.europa.eu/codelist/WaterAppurtenanceTypeValue/controlValve</v>
       </c>
     </row>
-    <row r="178" spans="1:7" ht="15" thickBot="1">
+    <row r="178" spans="1:7" ht="15" hidden="1" thickBot="1">
       <c r="A178" s="4" t="s">
         <v>114</v>
       </c>
@@ -6391,7 +6463,7 @@
         <v>http://inspire.ec.europa.eu/codelist/WaterAppurtenanceTypeValue/pressureController</v>
       </c>
     </row>
-    <row r="179" spans="1:7" ht="15" thickBot="1">
+    <row r="179" spans="1:7" ht="15" hidden="1" thickBot="1">
       <c r="A179" s="4" t="s">
         <v>114</v>
       </c>
@@ -6415,7 +6487,7 @@
         <v>http://inspire.ec.europa.eu/codelist/WaterAppurtenanceTypeValue/junction</v>
       </c>
     </row>
-    <row r="180" spans="1:7" ht="15" thickBot="1">
+    <row r="180" spans="1:7" ht="15" hidden="1" thickBot="1">
       <c r="A180" s="4" t="s">
         <v>114</v>
       </c>
@@ -6439,7 +6511,7 @@
         <v>http://inspire.ec.europa.eu/codelist/WaterAppurtenanceTypeValue/lateralPoint</v>
       </c>
     </row>
-    <row r="181" spans="1:7" ht="15" thickBot="1">
+    <row r="181" spans="1:7" ht="15" hidden="1" thickBot="1">
       <c r="A181" s="4" t="s">
         <v>114</v>
       </c>
@@ -6463,7 +6535,7 @@
         <v>http://inspire.ec.europa.eu/codelist/WaterAppurtenanceTypeValue/samplingStation</v>
       </c>
     </row>
-    <row r="182" spans="1:7" ht="15" thickBot="1">
+    <row r="182" spans="1:7" ht="15" hidden="1" thickBot="1">
       <c r="A182" s="4" t="s">
         <v>114</v>
       </c>
@@ -6487,7 +6559,7 @@
         <v>http://inspire.ec.europa.eu/codelist/WaterAppurtenanceTypeValue/meter</v>
       </c>
     </row>
-    <row r="183" spans="1:7" ht="15" thickBot="1">
+    <row r="183" spans="1:7" ht="15" hidden="1" thickBot="1">
       <c r="A183" s="4" t="s">
         <v>114</v>
       </c>
@@ -6511,7 +6583,7 @@
         <v>http://inspire.ec.europa.eu/codelist/WaterAppurtenanceTypeValue/airRelieveValve</v>
       </c>
     </row>
-    <row r="184" spans="1:7" ht="15" thickBot="1">
+    <row r="184" spans="1:7" ht="15" hidden="1" thickBot="1">
       <c r="A184" s="4" t="s">
         <v>114</v>
       </c>
@@ -6535,7 +6607,7 @@
         <v>http://inspire.ec.europa.eu/codelist/WaterAppurtenanceTypeValue/storageFacility</v>
       </c>
     </row>
-    <row r="185" spans="1:7" ht="15" thickBot="1">
+    <row r="185" spans="1:7" ht="15" hidden="1" thickBot="1">
       <c r="A185" s="4" t="s">
         <v>114</v>
       </c>
@@ -6559,7 +6631,7 @@
         <v>http://inspire.ec.europa.eu/codelist/WaterAppurtenanceTypeValue/pumpStation</v>
       </c>
     </row>
-    <row r="186" spans="1:7" ht="15" thickBot="1">
+    <row r="186" spans="1:7" ht="15" hidden="1" thickBot="1">
       <c r="A186" s="4" t="s">
         <v>114</v>
       </c>
@@ -6583,7 +6655,7 @@
         <v>http://inspire.ec.europa.eu/codelist/WaterAppurtenanceTypeValue/waterServicePoint</v>
       </c>
     </row>
-    <row r="187" spans="1:7" ht="15" thickBot="1">
+    <row r="187" spans="1:7" ht="15" hidden="1" thickBot="1">
       <c r="A187" s="4" t="s">
         <v>114</v>
       </c>
@@ -6607,7 +6679,7 @@
         <v>http://inspire.ec.europa.eu/codelist/WaterAppurtenanceTypeValue/treatmentPlant</v>
       </c>
     </row>
-    <row r="188" spans="1:7" ht="15" thickBot="1">
+    <row r="188" spans="1:7" ht="15" hidden="1" thickBot="1">
       <c r="A188" s="4" t="s">
         <v>114</v>
       </c>
@@ -6631,7 +6703,7 @@
         <v>http://www.geonovum.nl/imkl2015/1.0/def/WaterTypeValue/industrial</v>
       </c>
     </row>
-    <row r="189" spans="1:7" ht="15" thickBot="1">
+    <row r="189" spans="1:7" ht="15" hidden="1" thickBot="1">
       <c r="A189" s="4" t="s">
         <v>114</v>
       </c>
@@ -6655,7 +6727,7 @@
         <v>http://www.geonovum.nl/imkl2015/1.0/def/WaterTypeValue/waste</v>
       </c>
     </row>
-    <row r="190" spans="1:7" ht="15" thickBot="1">
+    <row r="190" spans="1:7" ht="15" hidden="1" thickBot="1">
       <c r="A190" s="4" t="s">
         <v>114</v>
       </c>
@@ -6679,7 +6751,7 @@
         <v>http://inspire.ec.europa.eu/codelist/WaterTypeValue/potable</v>
       </c>
     </row>
-    <row r="191" spans="1:7" ht="15" thickBot="1">
+    <row r="191" spans="1:7" ht="15" hidden="1" thickBot="1">
       <c r="A191" s="4" t="s">
         <v>114</v>
       </c>
@@ -6703,7 +6775,7 @@
         <v>http://inspire.ec.europa.eu/codelist/WaterTypeValue/raw</v>
       </c>
     </row>
-    <row r="192" spans="1:7" ht="15" thickBot="1">
+    <row r="192" spans="1:7" ht="15" hidden="1" thickBot="1">
       <c r="A192" s="4" t="s">
         <v>114</v>
       </c>
@@ -6727,7 +6799,7 @@
         <v>http://inspire.ec.europa.eu/codelist/WaterTypeValue/salt</v>
       </c>
     </row>
-    <row r="193" spans="1:7" ht="15" thickBot="1">
+    <row r="193" spans="1:7" ht="15" hidden="1" thickBot="1">
       <c r="A193" s="4" t="s">
         <v>114</v>
       </c>
@@ -6751,7 +6823,7 @@
         <v>http://inspire.ec.europa.eu/codelist/WaterTypeValue/treated</v>
       </c>
     </row>
-    <row r="194" spans="1:7" ht="15" thickBot="1">
+    <row r="194" spans="1:7" ht="15" hidden="1" thickBot="1">
       <c r="A194" s="4" t="s">
         <v>114</v>
       </c>
@@ -6771,7 +6843,7 @@
         <v>http://www.geonovum.nl/imkl2015/1.0/def/WaterAppurtenanceIMKLTypeValue/puntVanLevering</v>
       </c>
     </row>
-    <row r="195" spans="1:7" ht="15" thickBot="1">
+    <row r="195" spans="1:7" ht="15" hidden="1" thickBot="1">
       <c r="A195" s="4" t="s">
         <v>373</v>
       </c>
@@ -6795,7 +6867,7 @@
         <v>http://www.geonovum.nl/imkl2015/1.0/def/SewerAppurtenanceTypeIMKLValue/gemaal</v>
       </c>
     </row>
-    <row r="196" spans="1:7" ht="29" thickBot="1">
+    <row r="196" spans="1:7" ht="29" hidden="1" thickBot="1">
       <c r="A196" s="4" t="s">
         <v>373</v>
       </c>
@@ -6819,7 +6891,7 @@
         <v>http://www.geonovum.nl/imkl2015/1.0/def/SewerAppurtenanceTypeIMKLValue/infiltratievoorziening</v>
       </c>
     </row>
-    <row r="197" spans="1:7" ht="15" thickBot="1">
+    <row r="197" spans="1:7" ht="15" hidden="1" thickBot="1">
       <c r="A197" s="4" t="s">
         <v>373</v>
       </c>
@@ -6843,7 +6915,7 @@
         <v>http://www.geonovum.nl/imkl2015/1.0/def/SewerAppurtenanceTypeIMKLValue/kolk</v>
       </c>
     </row>
-    <row r="198" spans="1:7" ht="15" thickBot="1">
+    <row r="198" spans="1:7" ht="15" hidden="1" thickBot="1">
       <c r="A198" s="4" t="s">
         <v>373</v>
       </c>
@@ -6867,7 +6939,7 @@
         <v>http://www.geonovum.nl/imkl2015/1.0/def/SewerAppurtenanceTypeIMKLValue/kunstwerk</v>
       </c>
     </row>
-    <row r="199" spans="1:7">
+    <row r="199" spans="1:7" hidden="1">
       <c r="A199" s="4" t="s">
         <v>373</v>
       </c>
@@ -6891,7 +6963,7 @@
         <v>http://www.geonovum.nl/imkl2015/1.0/def/SewerAppurtenanceTypeIMKLValue/reservoir</v>
       </c>
     </row>
-    <row r="200" spans="1:7">
+    <row r="200" spans="1:7" hidden="1">
       <c r="A200" s="4" t="s">
         <v>373</v>
       </c>
@@ -6915,7 +6987,7 @@
         <v>http://www.geonovum.nl/imkl2015/1.0/def/SewerAppurtenanceTypeIMKLValue/uitlaatconstructie</v>
       </c>
     </row>
-    <row r="201" spans="1:7" ht="15" thickBot="1">
+    <row r="201" spans="1:7" ht="15" hidden="1" thickBot="1">
       <c r="A201" s="4" t="s">
         <v>373</v>
       </c>
@@ -6939,7 +7011,7 @@
         <v>http://inspire.ec.europa.eu/codelist/SewerAppurtenanceTypeValue/connection</v>
       </c>
     </row>
-    <row r="202" spans="1:7" ht="15" thickBot="1">
+    <row r="202" spans="1:7" ht="15" hidden="1" thickBot="1">
       <c r="A202" s="4" t="s">
         <v>373</v>
       </c>
@@ -6963,7 +7035,7 @@
         <v>http://inspire.ec.europa.eu/codelist/SewerAppurtenanceTypeValue/cleanOut</v>
       </c>
     </row>
-    <row r="203" spans="1:7" ht="15" thickBot="1">
+    <row r="203" spans="1:7" ht="15" hidden="1" thickBot="1">
       <c r="A203" s="4" t="s">
         <v>373</v>
       </c>
@@ -6987,7 +7059,7 @@
         <v>http://inspire.ec.europa.eu/codelist/SewerAppurtenanceTypeValue/barrel</v>
       </c>
     </row>
-    <row r="204" spans="1:7" ht="15" thickBot="1">
+    <row r="204" spans="1:7" ht="15" hidden="1" thickBot="1">
       <c r="A204" s="4" t="s">
         <v>373</v>
       </c>
@@ -7011,7 +7083,7 @@
         <v>http://inspire.ec.europa.eu/codelist/SewerAppurtenanceTypeValue/catchBasin</v>
       </c>
     </row>
-    <row r="205" spans="1:7" ht="15" thickBot="1">
+    <row r="205" spans="1:7" ht="15" hidden="1" thickBot="1">
       <c r="A205" s="4" t="s">
         <v>373</v>
       </c>
@@ -7035,7 +7107,7 @@
         <v>http://inspire.ec.europa.eu/codelist/SewerAppurtenanceTypeValue/watertankOrChamber</v>
       </c>
     </row>
-    <row r="206" spans="1:7" ht="15" thickBot="1">
+    <row r="206" spans="1:7" ht="15" hidden="1" thickBot="1">
       <c r="A206" s="4" t="s">
         <v>373</v>
       </c>
@@ -7059,7 +7131,7 @@
         <v>http://inspire.ec.europa.eu/codelist/SewerAppurtenanceTypeValue/specificStructure</v>
       </c>
     </row>
-    <row r="207" spans="1:7">
+    <row r="207" spans="1:7" hidden="1">
       <c r="A207" s="4" t="s">
         <v>373</v>
       </c>
@@ -7083,7 +7155,7 @@
         <v>http://www.geonovum.nl/imkl2015/1.0/def/SewerAppurtenanceTypeIMKLValue/overstort</v>
       </c>
     </row>
-    <row r="208" spans="1:7">
+    <row r="208" spans="1:7" hidden="1">
       <c r="A208" s="4" t="s">
         <v>373</v>
       </c>
@@ -7107,7 +7179,7 @@
         <v>http://inspire.ec.europa.eu/codelist/SewerAppurtenanceTypeValue/thrustProtection</v>
       </c>
     </row>
-    <row r="209" spans="1:7">
+    <row r="209" spans="1:7" hidden="1">
       <c r="A209" s="4" t="s">
         <v>373</v>
       </c>
@@ -7131,7 +7203,7 @@
         <v>http://inspire.ec.europa.eu/codelist/SewerAppurtenanceTypeValue/tideGate</v>
       </c>
     </row>
-    <row r="210" spans="1:7">
+    <row r="210" spans="1:7" hidden="1">
       <c r="A210" s="4" t="s">
         <v>373</v>
       </c>
@@ -7155,7 +7227,7 @@
         <v>http://inspire.ec.europa.eu/codelist/SewerAppurtenanceTypeValue/dischargeStructure</v>
       </c>
     </row>
-    <row r="211" spans="1:7" ht="15" thickBot="1">
+    <row r="211" spans="1:7" ht="15" hidden="1" thickBot="1">
       <c r="A211" s="4" t="s">
         <v>373</v>
       </c>
@@ -7179,7 +7251,7 @@
         <v>http://inspire.ec.europa.eu/codelist/SewerWaterTypeValue/combined</v>
       </c>
     </row>
-    <row r="212" spans="1:7" ht="15" thickBot="1">
+    <row r="212" spans="1:7" ht="15" hidden="1" thickBot="1">
       <c r="A212" s="4" t="s">
         <v>373</v>
       </c>
@@ -7203,7 +7275,7 @@
         <v>http://inspire.ec.europa.eu/codelist/SewerWaterTypeValue/reclaimed</v>
       </c>
     </row>
-    <row r="213" spans="1:7" ht="15" thickBot="1">
+    <row r="213" spans="1:7" ht="15" hidden="1" thickBot="1">
       <c r="A213" s="4" t="s">
         <v>373</v>
       </c>
@@ -7227,7 +7299,7 @@
         <v>http://inspire.ec.europa.eu/codelist/SewerWaterTypeValue/sanitary</v>
       </c>
     </row>
-    <row r="214" spans="1:7" ht="15" thickBot="1">
+    <row r="214" spans="1:7" ht="15" hidden="1" thickBot="1">
       <c r="A214" s="4" t="s">
         <v>373</v>
       </c>
@@ -7251,7 +7323,7 @@
         <v>http://inspire.ec.europa.eu/codelist/SewerWaterTypeValue/storm</v>
       </c>
     </row>
-    <row r="215" spans="1:7">
+    <row r="215" spans="1:7" hidden="1">
       <c r="A215" s="4" t="s">
         <v>373</v>
       </c>
@@ -7272,7 +7344,7 @@
         <v>http://www.geonovum.nl/imkl2015/1.0/def/SewerAppurtenanceTypeIMKLValue/puntVanLevering</v>
       </c>
     </row>
-    <row r="216" spans="1:7">
+    <row r="216" spans="1:7" hidden="1">
       <c r="A216" s="4" t="s">
         <v>131</v>
       </c>
@@ -7296,7 +7368,7 @@
         <v>http://www.geonovum.nl/imkl2015/1.0/def/SewerAppurtenanceTypeIMKLValue/compensator</v>
       </c>
     </row>
-    <row r="217" spans="1:7">
+    <row r="217" spans="1:7" hidden="1">
       <c r="A217" s="4" t="s">
         <v>131</v>
       </c>
@@ -7320,7 +7392,7 @@
         <v>http://www.geonovum.nl/imkl2015/1.0/def/SewerAppurtenanceTypeIMKLValue/lekdetectiemeetpunt</v>
       </c>
     </row>
-    <row r="218" spans="1:7">
+    <row r="218" spans="1:7" hidden="1">
       <c r="A218" s="4" t="s">
         <v>131</v>
       </c>
@@ -7344,7 +7416,7 @@
         <v>http://www.geonovum.nl/imkl2015/1.0/def/SewerAppurtenanceTypeIMKLValue/putten</v>
       </c>
     </row>
-    <row r="219" spans="1:7">
+    <row r="219" spans="1:7" hidden="1">
       <c r="A219" s="4" t="s">
         <v>131</v>
       </c>
@@ -7368,7 +7440,7 @@
         <v>http://www.geonovum.nl/imkl2015/1.0/def/SewerAppurtenanceTypeIMKLValue/pompstation</v>
       </c>
     </row>
-    <row r="220" spans="1:7">
+    <row r="220" spans="1:7" hidden="1">
       <c r="A220" s="4" t="s">
         <v>131</v>
       </c>
@@ -7392,7 +7464,7 @@
         <v>http://www.geonovum.nl/imkl2015/1.0/def/SewerAppurtenanceTypeIMKLValue/overdrachtsstation</v>
       </c>
     </row>
-    <row r="221" spans="1:7">
+    <row r="221" spans="1:7" hidden="1">
       <c r="A221" s="4" t="s">
         <v>131</v>
       </c>
@@ -7407,7 +7479,7 @@
         <v>http://www.geonovum.nl/imkl2015/1.0/def/SewerAppurtenanceTypeIMKLValue/</v>
       </c>
     </row>
-    <row r="222" spans="1:7">
+    <row r="222" spans="1:7" hidden="1">
       <c r="A222" s="4" t="s">
         <v>131</v>
       </c>
@@ -7431,7 +7503,7 @@
         <v>http://www.geonovum.nl/imkl2015/1.0/def/SewerAppurtenanceTypeIMKLValue/mantelbuis</v>
       </c>
     </row>
-    <row r="223" spans="1:7" ht="70">
+    <row r="223" spans="1:7" ht="70" hidden="1">
       <c r="A223" s="4" t="s">
         <v>131</v>
       </c>
@@ -7455,7 +7527,7 @@
         <v>http://www.geonovum.nl/imkl2015/1.0/def/SewerAppurtenanceTypeIMKLValue/zinker</v>
       </c>
     </row>
-    <row r="224" spans="1:7">
+    <row r="224" spans="1:7" hidden="1">
       <c r="A224" s="4" t="s">
         <v>131</v>
       </c>
@@ -7479,7 +7551,7 @@
         <v>http://www.geonovum.nl/imkl2015/1.0/def/SewerAppurtenanceTypeIMKLValue/inEnUittredepuntBoringen</v>
       </c>
     </row>
-    <row r="225" spans="1:7">
+    <row r="225" spans="1:7" hidden="1">
       <c r="A225" s="4" t="s">
         <v>131</v>
       </c>
@@ -7503,7 +7575,7 @@
         <v>http://www.geonovum.nl/imkl2015/1.0/def/SewerAppurtenanceTypeIMKLValue/gestuurdeBoring</v>
       </c>
     </row>
-    <row r="226" spans="1:7">
+    <row r="226" spans="1:7" hidden="1">
       <c r="A226" s="4" t="s">
         <v>131</v>
       </c>
@@ -7518,7 +7590,7 @@
         <v>http://www.geonovum.nl/imkl2015/1.0/def/SewerAppurtenanceTypeIMKLValue/</v>
       </c>
     </row>
-    <row r="227" spans="1:7">
+    <row r="227" spans="1:7" hidden="1">
       <c r="A227" s="4" t="s">
         <v>131</v>
       </c>
@@ -7540,7 +7612,15 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:G227"/>
+  <autoFilter ref="A1:G227">
+    <filterColumn colId="5">
+      <filters>
+        <filter val="TelecommunicationsAppurtenanceIMKLTypeValue"/>
+        <filter val="TelecommunicationsCableMaterialTypeValue"/>
+        <filter val="UtilityNetworkTypeValue"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <sortState ref="B2:F62">
     <sortCondition ref="C2:C62"/>
     <sortCondition ref="B2:B62"/>
@@ -7602,6 +7682,7 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <legacyDrawing r:id="rId54"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>

<commit_message>
Moved TelecommunicationsCableMaterialTypeValue to IMKL
Fixes #36
</commit_message>
<xml_diff>
--- a/3. waardelijsten/IMKL2015 - 0.9 waardelijsten.xlsx
+++ b/3. waardelijsten/IMKL2015 - 0.9 waardelijsten.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="26024"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="38420" yWindow="720" windowWidth="25600" windowHeight="16060" tabRatio="645" activeTab="1"/>
+    <workbookView xWindow="38415" yWindow="720" windowWidth="24240" windowHeight="13740" tabRatio="645" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Toelichting" sheetId="8" r:id="rId1"/>
@@ -18,7 +18,7 @@
     <definedName name="IMKL">Toelichting!$B$22</definedName>
     <definedName name="INSPIRE">Toelichting!$B$23</definedName>
   </definedNames>
-  <calcPr calcId="140001" concurrentCalc="0"/>
+  <calcPr calcId="145621" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -2265,12 +2265,12 @@
       <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="56" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="22" spans="2:3">
+    <row r="22" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B22" s="35" t="s">
         <v>380</v>
       </c>
@@ -2278,7 +2278,7 @@
         <v>279</v>
       </c>
     </row>
-    <row r="23" spans="2:3">
+    <row r="23" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
         <v>280</v>
       </c>
@@ -2303,24 +2303,23 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr filterMode="1" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:G227"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="G238" sqref="G238"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="B89" sqref="B89"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="12.6640625" customWidth="1"/>
+    <col min="2" max="2" width="12.7109375" customWidth="1"/>
     <col min="3" max="3" width="37" customWidth="1"/>
-    <col min="4" max="4" width="31.33203125" customWidth="1"/>
-    <col min="5" max="5" width="16.6640625" customWidth="1"/>
-    <col min="6" max="6" width="42.6640625" customWidth="1"/>
-    <col min="7" max="7" width="82.6640625" customWidth="1"/>
+    <col min="4" max="4" width="31.28515625" customWidth="1"/>
+    <col min="5" max="5" width="16.7109375" customWidth="1"/>
+    <col min="6" max="6" width="42.7109375" customWidth="1"/>
+    <col min="7" max="7" width="82.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="4" customFormat="1">
+    <row r="1" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>368</v>
       </c>
@@ -2343,7 +2342,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="2" spans="1:7" s="1" customFormat="1" hidden="1">
+    <row r="2" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>369</v>
       </c>
@@ -2367,7 +2366,7 @@
         <v>http://www.geonovum.nl/imkl2015/1.0/def/AnnotatieTypeValue/annotatiePijl</v>
       </c>
     </row>
-    <row r="3" spans="1:7" s="1" customFormat="1" hidden="1">
+    <row r="3" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>369</v>
       </c>
@@ -2388,7 +2387,7 @@
         <v>http://www.geonovum.nl/imkl2015/1.0/def/AnnotatieTypeValue/annotatieLijn</v>
       </c>
     </row>
-    <row r="4" spans="1:7" s="1" customFormat="1" hidden="1">
+    <row r="4" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>369</v>
       </c>
@@ -2409,7 +2408,7 @@
         <v>http://www.geonovum.nl/imkl2015/1.0/def/AnnotatieTypeValue/annotatieLabel</v>
       </c>
     </row>
-    <row r="5" spans="1:7" s="1" customFormat="1" hidden="1">
+    <row r="5" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>369</v>
       </c>
@@ -2430,7 +2429,7 @@
         <v>http://www.geonovum.nl/imkl2015/1.0/def/BestandMediaTypeValue/PNG</v>
       </c>
     </row>
-    <row r="6" spans="1:7" s="1" customFormat="1" hidden="1">
+    <row r="6" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>369</v>
       </c>
@@ -2451,7 +2450,7 @@
         <v>http://www.geonovum.nl/imkl2015/1.0/def/BestandMediaTypeValue/PDF</v>
       </c>
     </row>
-    <row r="7" spans="1:7" s="1" customFormat="1" hidden="1">
+    <row r="7" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>369</v>
       </c>
@@ -2472,7 +2471,7 @@
         <v>http://www.geonovum.nl/imkl2015/1.0/def/BestandMediaTypeValue/JPEG</v>
       </c>
     </row>
-    <row r="8" spans="1:7" s="1" customFormat="1" hidden="1">
+    <row r="8" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>369</v>
       </c>
@@ -2493,7 +2492,7 @@
         <v>http://www.geonovum.nl/imkl2015/1.0/def/BestandMediaTypeValue/TIFF</v>
       </c>
     </row>
-    <row r="9" spans="1:7" s="1" customFormat="1" hidden="1">
+    <row r="9" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>369</v>
       </c>
@@ -2515,7 +2514,7 @@
         <v>http://inspire.ec.europa.eu/codelist/ConditionOfFacilityValue/functional</v>
       </c>
     </row>
-    <row r="10" spans="1:7" s="1" customFormat="1" hidden="1">
+    <row r="10" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>369</v>
       </c>
@@ -2537,7 +2536,7 @@
         <v>http://inspire.ec.europa.eu/codelist/ConditionOfFacilityValue/projected</v>
       </c>
     </row>
-    <row r="11" spans="1:7" s="1" customFormat="1" hidden="1">
+    <row r="11" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>369</v>
       </c>
@@ -2559,7 +2558,7 @@
         <v>http://inspire.ec.europa.eu/codelist/ConditionOfFacilityValue/disused</v>
       </c>
     </row>
-    <row r="12" spans="1:7" s="1" customFormat="1" ht="15" hidden="1" customHeight="1">
+    <row r="12" spans="1:7" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>369</v>
       </c>
@@ -2580,7 +2579,7 @@
         <v>http://www.geonovum.nl/imkl2015/1.0/def/NauwkeurigheidDiepteValue/tot30cm</v>
       </c>
     </row>
-    <row r="13" spans="1:7" s="1" customFormat="1" ht="15.75" hidden="1" customHeight="1">
+    <row r="13" spans="1:7" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>369</v>
       </c>
@@ -2601,7 +2600,7 @@
         <v>http://www.geonovum.nl/imkl2015/1.0/def/NauwkeurigheidDiepteValue/tot50cm</v>
       </c>
     </row>
-    <row r="14" spans="1:7" s="1" customFormat="1" ht="15.75" hidden="1" customHeight="1">
+    <row r="14" spans="1:7" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>369</v>
       </c>
@@ -2622,7 +2621,7 @@
         <v>http://www.geonovum.nl/imkl2015/1.0/def/NauwkeurigheidDiepteValue/tot100cm</v>
       </c>
     </row>
-    <row r="15" spans="1:7" s="1" customFormat="1" ht="14.25" hidden="1" customHeight="1">
+    <row r="15" spans="1:7" s="1" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>369</v>
       </c>
@@ -2643,7 +2642,7 @@
         <v>http://www.geonovum.nl/imkl2015/1.0/def/NauwkeurigheidDiepteValue/onbekend</v>
       </c>
     </row>
-    <row r="16" spans="1:7" s="1" customFormat="1" hidden="1">
+    <row r="16" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>369</v>
       </c>
@@ -2664,7 +2663,7 @@
         <v>http://www.geonovum.nl/imkl2015/1.0/def/ExtraDetailInfoTypeValue/huisaansluiting</v>
       </c>
     </row>
-    <row r="17" spans="1:7" s="1" customFormat="1" hidden="1">
+    <row r="17" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>369</v>
       </c>
@@ -2685,7 +2684,7 @@
         <v>http://www.geonovum.nl/imkl2015/1.0/def/ExtraDetailInfoTypeValue/lengteprofiel</v>
       </c>
     </row>
-    <row r="18" spans="1:7" s="1" customFormat="1" hidden="1">
+    <row r="18" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>369</v>
       </c>
@@ -2706,7 +2705,7 @@
         <v>http://www.geonovum.nl/imkl2015/1.0/def/ExtraDetailInfoTypeValue/gestuurdeBoring</v>
       </c>
     </row>
-    <row r="19" spans="1:7" s="1" customFormat="1" hidden="1">
+    <row r="19" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>369</v>
       </c>
@@ -2727,7 +2726,7 @@
         <v>http://www.geonovum.nl/imkl2015/1.0/def/ExtraDetailInfoTypeValue/dwarsprofiel</v>
       </c>
     </row>
-    <row r="20" spans="1:7" s="1" customFormat="1" ht="12.75" hidden="1" customHeight="1">
+    <row r="20" spans="1:7" s="1" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>369</v>
       </c>
@@ -2748,7 +2747,7 @@
         <v>http://www.geonovum.nl/imkl2015/1.0/def/ExtraTopografieTypeValue/eigen</v>
       </c>
     </row>
-    <row r="21" spans="1:7" s="1" customFormat="1" hidden="1">
+    <row r="21" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>369</v>
       </c>
@@ -2769,7 +2768,7 @@
         <v>http://www.geonovum.nl/imkl2015/1.0/def/ExtraTopografieTypeValue/ontwerp</v>
       </c>
     </row>
-    <row r="22" spans="1:7" s="1" customFormat="1" ht="14.25" hidden="1" customHeight="1">
+    <row r="22" spans="1:7" s="1" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>369</v>
       </c>
@@ -2790,7 +2789,7 @@
         <v>http://www.geonovum.nl/imkl2015/1.0/def/NauwkeurigheidXYvalue/tot30cm</v>
       </c>
     </row>
-    <row r="23" spans="1:7" s="1" customFormat="1" ht="14.25" hidden="1" customHeight="1">
+    <row r="23" spans="1:7" s="1" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>369</v>
       </c>
@@ -2811,7 +2810,7 @@
         <v>http://www.geonovum.nl/imkl2015/1.0/def/NauwkeurigheidXYvalue/tot50cm</v>
       </c>
     </row>
-    <row r="24" spans="1:7" s="1" customFormat="1" hidden="1">
+    <row r="24" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>369</v>
       </c>
@@ -2832,7 +2831,7 @@
         <v>http://www.geonovum.nl/imkl2015/1.0/def/NauwkeurigheidXYvalue/tot100cm</v>
       </c>
     </row>
-    <row r="25" spans="1:7" s="1" customFormat="1" hidden="1">
+    <row r="25" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>369</v>
       </c>
@@ -2853,7 +2852,7 @@
         <v>http://www.geonovum.nl/imkl2015/1.0/def/MaatvoeringsTypeValue/maatvoeringshulplijn</v>
       </c>
     </row>
-    <row r="26" spans="1:7" s="1" customFormat="1" hidden="1">
+    <row r="26" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>369</v>
       </c>
@@ -2874,7 +2873,7 @@
         <v>http://www.geonovum.nl/imkl2015/1.0/def/MaatvoeringsTypeValue/maatvoeringslijn</v>
       </c>
     </row>
-    <row r="27" spans="1:7" s="1" customFormat="1" hidden="1">
+    <row r="27" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>369</v>
       </c>
@@ -2895,7 +2894,7 @@
         <v>http://www.geonovum.nl/imkl2015/1.0/def/MaatvoeringsTypeValue/maatvoeringspijl</v>
       </c>
     </row>
-    <row r="28" spans="1:7" hidden="1">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>369</v>
       </c>
@@ -2917,7 +2916,7 @@
         <v>http://www.geonovum.nl/imkl2015/1.0/def/MaatvoeringsTypeValue/maatvoeringslabel</v>
       </c>
     </row>
-    <row r="29" spans="1:7" hidden="1">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>369</v>
       </c>
@@ -2941,7 +2940,7 @@
         <v>http://www.geonovum.nl/imkl2015/1.0/def/Thema/buisleidingGevaarlijkeInhoud</v>
       </c>
     </row>
-    <row r="30" spans="1:7" hidden="1">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
         <v>369</v>
       </c>
@@ -2962,7 +2961,7 @@
         <v>http://www.geonovum.nl/imkl2015/1.0/def/Thema/datatransport</v>
       </c>
     </row>
-    <row r="31" spans="1:7" hidden="1">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
         <v>369</v>
       </c>
@@ -2986,7 +2985,7 @@
         <v>http://www.geonovum.nl/imkl2015/1.0/def/Thema/gasLageDruk</v>
       </c>
     </row>
-    <row r="32" spans="1:7" hidden="1">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
         <v>369</v>
       </c>
@@ -3010,7 +3009,7 @@
         <v>http://www.geonovum.nl/imkl2015/1.0/def/Thema/gasHogeDruk</v>
       </c>
     </row>
-    <row r="33" spans="1:7" hidden="1">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
         <v>369</v>
       </c>
@@ -3034,7 +3033,7 @@
         <v>http://www.geonovum.nl/imkl2015/1.0/def/Thema/petrochemie</v>
       </c>
     </row>
-    <row r="34" spans="1:7" hidden="1">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
         <v>369</v>
       </c>
@@ -3058,7 +3057,7 @@
         <v>http://www.geonovum.nl/imkl2015/1.0/def/Thema/landelijkHoogspanningsnet</v>
       </c>
     </row>
-    <row r="35" spans="1:7" hidden="1">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
         <v>369</v>
       </c>
@@ -3082,7 +3081,7 @@
         <v>http://www.geonovum.nl/imkl2015/1.0/def/Thema/hoogspanning</v>
       </c>
     </row>
-    <row r="36" spans="1:7" hidden="1">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
         <v>369</v>
       </c>
@@ -3106,7 +3105,7 @@
         <v>http://www.geonovum.nl/imkl2015/1.0/def/Thema/laagspanning</v>
       </c>
     </row>
-    <row r="37" spans="1:7" hidden="1">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
         <v>369</v>
       </c>
@@ -3130,7 +3129,7 @@
         <v>http://www.geonovum.nl/imkl2015/1.0/def/Thema/middenspanning</v>
       </c>
     </row>
-    <row r="38" spans="1:7" hidden="1">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
         <v>369</v>
       </c>
@@ -3154,7 +3153,7 @@
         <v>http://www.geonovum.nl/imkl2015/1.0/def/Thema/rioolVrijverval</v>
       </c>
     </row>
-    <row r="39" spans="1:7" hidden="1">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
         <v>369</v>
       </c>
@@ -3178,7 +3177,7 @@
         <v>http://www.geonovum.nl/imkl2015/1.0/def/Thema/rioolOnderDruk</v>
       </c>
     </row>
-    <row r="40" spans="1:7" hidden="1">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
         <v>369</v>
       </c>
@@ -3202,7 +3201,7 @@
         <v>http://www.geonovum.nl/imkl2015/1.0/def/Thema/warmte</v>
       </c>
     </row>
-    <row r="41" spans="1:7" hidden="1">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
         <v>369</v>
       </c>
@@ -3226,7 +3225,7 @@
         <v>http://www.geonovum.nl/imkl2015/1.0/def/Thema/water</v>
       </c>
     </row>
-    <row r="42" spans="1:7" hidden="1">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
         <v>369</v>
       </c>
@@ -3250,7 +3249,7 @@
         <v>http://www.geonovum.nl/imkl2015/1.0/def/Thema/wees</v>
       </c>
     </row>
-    <row r="43" spans="1:7" hidden="1">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
         <v>369</v>
       </c>
@@ -3274,7 +3273,7 @@
         <v>http://www.geonovum.nl/imkl2015/1.0/def/Thema/overig</v>
       </c>
     </row>
-    <row r="44" spans="1:7" hidden="1">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
         <v>369</v>
       </c>
@@ -3295,7 +3294,7 @@
         <v>http://inspire.ec.europa.eu/codelist/UtilityDeliveryTypeValue/collection</v>
       </c>
     </row>
-    <row r="45" spans="1:7" hidden="1">
+    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
         <v>369</v>
       </c>
@@ -3316,7 +3315,7 @@
         <v>http://inspire.ec.europa.eu/codelist/UtilityDeliveryTypeValue/distribution</v>
       </c>
     </row>
-    <row r="46" spans="1:7" hidden="1">
+    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
         <v>369</v>
       </c>
@@ -3337,7 +3336,7 @@
         <v>http://inspire.ec.europa.eu/codelist/UtilityDeliveryTypeValue/private</v>
       </c>
     </row>
-    <row r="47" spans="1:7" hidden="1">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
         <v>369</v>
       </c>
@@ -3358,7 +3357,7 @@
         <v>http://inspire.ec.europa.eu/codelist/UtilityDeliveryTypeValue/transport</v>
       </c>
     </row>
-    <row r="48" spans="1:7">
+    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
         <v>369</v>
       </c>
@@ -3379,7 +3378,7 @@
         <v>http://inspire.ec.europa.eu/codelist/UtilityNetworkTypeValue/electricity</v>
       </c>
     </row>
-    <row r="49" spans="1:7">
+    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
         <v>369</v>
       </c>
@@ -3400,7 +3399,7 @@
         <v>http://inspire.ec.europa.eu/codelist/UtilityNetworkTypeValue/oilGasChemical</v>
       </c>
     </row>
-    <row r="50" spans="1:7">
+    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
         <v>369</v>
       </c>
@@ -3421,7 +3420,7 @@
         <v>http://inspire.ec.europa.eu/codelist/UtilityNetworkTypeValue/sewer</v>
       </c>
     </row>
-    <row r="51" spans="1:7">
+    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
         <v>369</v>
       </c>
@@ -3442,7 +3441,7 @@
         <v>http://inspire.ec.europa.eu/codelist/UtilityNetworkTypeValue/water</v>
       </c>
     </row>
-    <row r="52" spans="1:7">
+    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
         <v>369</v>
       </c>
@@ -3463,7 +3462,7 @@
         <v>http://inspire.ec.europa.eu/codelist/UtilityNetworkTypeValue/thermal</v>
       </c>
     </row>
-    <row r="53" spans="1:7">
+    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
         <v>369</v>
       </c>
@@ -3484,7 +3483,7 @@
         <v>http://inspire.ec.europa.eu/codelist/UtilityNetworkTypeValue/telecommunications</v>
       </c>
     </row>
-    <row r="54" spans="1:7">
+    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
         <v>369</v>
       </c>
@@ -3505,7 +3504,7 @@
         <v>http://inspire.ec.europa.eu/codelist/UtilityNetworkTypeValue/crossTheme</v>
       </c>
     </row>
-    <row r="55" spans="1:7" hidden="1">
+    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
         <v>369</v>
       </c>
@@ -3526,7 +3525,7 @@
         <v>http://inspire.ec.europa.eu/codelist/WarningTypeValue/net</v>
       </c>
     </row>
-    <row r="56" spans="1:7" hidden="1">
+    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
         <v>369</v>
       </c>
@@ -3547,7 +3546,7 @@
         <v>http://inspire.ec.europa.eu/codelist/WarningTypeValue/tape</v>
       </c>
     </row>
-    <row r="57" spans="1:7" hidden="1">
+    <row r="57" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A57" s="1" t="s">
         <v>369</v>
       </c>
@@ -3568,7 +3567,7 @@
         <v>http://inspire.ec.europa.eu/codelist/WarningTypeValue/concretePaving</v>
       </c>
     </row>
-    <row r="58" spans="1:7" ht="15" hidden="1" thickBot="1">
+    <row r="58" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
         <v>370</v>
       </c>
@@ -3592,7 +3591,7 @@
         <v>http://www.geonovum.nl/imkl2015/1.0/def/ElectricityAppurtenanceTypeIMKLValue/aarding</v>
       </c>
     </row>
-    <row r="59" spans="1:7" ht="15" hidden="1" thickBot="1">
+    <row r="59" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
         <v>370</v>
       </c>
@@ -3616,7 +3615,7 @@
         <v>http://www.geonovum.nl/imkl2015/1.0/def/ElectricityAppurtenanceTypeIMKLValue/mof</v>
       </c>
     </row>
-    <row r="60" spans="1:7" ht="15" hidden="1" thickBot="1">
+    <row r="60" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
         <v>370</v>
       </c>
@@ -3640,7 +3639,7 @@
         <v>http://www.geonovum.nl/imkl2015/1.0/def/ElectricityAppurtenanceTypeIMKLValue/hoogteligging</v>
       </c>
     </row>
-    <row r="61" spans="1:7" ht="15" hidden="1" thickBot="1">
+    <row r="61" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
         <v>370</v>
       </c>
@@ -3664,7 +3663,7 @@
         <v>http://www.geonovum.nl/imkl2015/1.0/def/ElectricityAppurtenanceTypeIMKLValue/Adrespunt</v>
       </c>
     </row>
-    <row r="62" spans="1:7" ht="15" hidden="1" thickBot="1">
+    <row r="62" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
         <v>370</v>
       </c>
@@ -3688,7 +3687,7 @@
         <v>http://inspire.ec.europa.eu/codelist/ElectricityAppurtenanceTypeValue/connectionBox</v>
       </c>
     </row>
-    <row r="63" spans="1:7" ht="15" hidden="1" thickBot="1">
+    <row r="63" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
         <v>370</v>
       </c>
@@ -3712,7 +3711,7 @@
         <v>http://inspire.ec.europa.eu/codelist/ElectricityAppurtenanceTypeValue/mainStation</v>
       </c>
     </row>
-    <row r="64" spans="1:7" ht="15" hidden="1" thickBot="1">
+    <row r="64" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
         <v>370</v>
       </c>
@@ -3736,7 +3735,7 @@
         <v>http://inspire.ec.europa.eu/codelist/ElectricityAppurtenanceTypeValue/generator</v>
       </c>
     </row>
-    <row r="65" spans="1:7" ht="15" hidden="1" thickBot="1">
+    <row r="65" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
         <v>370</v>
       </c>
@@ -3760,7 +3759,7 @@
         <v>http://inspire.ec.europa.eu/codelist/ElectricityAppurtenanceTypeValue/netStation</v>
       </c>
     </row>
-    <row r="66" spans="1:7" ht="15" hidden="1" thickBot="1">
+    <row r="66" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
         <v>370</v>
       </c>
@@ -3784,7 +3783,7 @@
         <v>http://inspire.ec.europa.eu/codelist/ElectricityAppurtenanceTypeValue/subStation</v>
       </c>
     </row>
-    <row r="67" spans="1:7" ht="15" hidden="1" thickBot="1">
+    <row r="67" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
         <v>370</v>
       </c>
@@ -3808,7 +3807,7 @@
         <v>http://inspire.ec.europa.eu/codelist/ElectricityAppurtenanceTypeValue/deliveryPoint</v>
       </c>
     </row>
-    <row r="68" spans="1:7" ht="15" hidden="1" thickBot="1">
+    <row r="68" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
         <v>370</v>
       </c>
@@ -3832,7 +3831,7 @@
         <v>http://inspire.ec.europa.eu/codelist/ElectricityAppurtenanceTypeValue/streetLight</v>
       </c>
     </row>
-    <row r="69" spans="1:7" ht="15" hidden="1" thickBot="1">
+    <row r="69" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
         <v>370</v>
       </c>
@@ -3853,7 +3852,7 @@
         <v>http://www.geonovum.nl/imkl2015/1.0/def/ElectricityAppurtenanceTypeIMKLValue/puntVanLevering</v>
       </c>
     </row>
-    <row r="70" spans="1:7" ht="15" hidden="1" thickBot="1">
+    <row r="70" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
         <v>370</v>
       </c>
@@ -3874,7 +3873,7 @@
         <v>http://www.geonovum.nl/imkl2015/1.0/def/ElectricityAppurtenanceTypeIMKLValue/geulmof</v>
       </c>
     </row>
-    <row r="71" spans="1:7" hidden="1">
+    <row r="71" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>370</v>
       </c>
@@ -3898,7 +3897,7 @@
         <v>http://www.geonovum.nl/imkl2015/1.0/def/ElectricityAppurtenanceTypeIMKLValue/kbMeetpunt</v>
       </c>
     </row>
-    <row r="72" spans="1:7" hidden="1">
+    <row r="72" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>370</v>
       </c>
@@ -3922,7 +3921,7 @@
         <v>http://www.geonovum.nl/imkl2015/1.0/def/ElectricityAppurtenanceTypeIMKLValue/kbInstallatie</v>
       </c>
     </row>
-    <row r="73" spans="1:7" hidden="1">
+    <row r="73" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>370</v>
       </c>
@@ -3946,7 +3945,7 @@
         <v>http://www.geonovum.nl/imkl2015/1.0/def/ElectricityAppurtenanceTypeIMKLValue/kbEindpunt</v>
       </c>
     </row>
-    <row r="74" spans="1:7" hidden="1">
+    <row r="74" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>370</v>
       </c>
@@ -3970,7 +3969,7 @@
         <v>http://www.geonovum.nl/imkl2015/1.0/def/ElectricityAppurtenanceTypeIMKLValue/kbContact</v>
       </c>
     </row>
-    <row r="75" spans="1:7" ht="15" hidden="1" thickBot="1">
+    <row r="75" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
         <v>370</v>
       </c>
@@ -3994,7 +3993,7 @@
         <v>http://www.geonovum.nl/imkl2015/1.0/def/ElectricityAppurtenanceTypeIMKLValue/hoogbouwkoppelpunt</v>
       </c>
     </row>
-    <row r="76" spans="1:7">
+    <row r="76" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>371</v>
       </c>
@@ -4018,7 +4017,7 @@
         <v>http://www.geonovum.nl/imkl2015/1.0/def/TelecommunicationsAppurtenanceIMKLTypeValue/antenna</v>
       </c>
     </row>
-    <row r="77" spans="1:7">
+    <row r="77" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>371</v>
       </c>
@@ -4042,7 +4041,7 @@
         <v>http://www.geonovum.nl/imkl2015/1.0/def/TelecommunicationsAppurtenanceIMKLTypeValue/termination</v>
       </c>
     </row>
-    <row r="78" spans="1:7">
+    <row r="78" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>371</v>
       </c>
@@ -4066,7 +4065,7 @@
         <v>http://www.geonovum.nl/imkl2015/1.0/def/TelecommunicationsAppurtenanceIMKLTypeValue/handhole</v>
       </c>
     </row>
-    <row r="79" spans="1:7">
+    <row r="79" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>371</v>
       </c>
@@ -4090,7 +4089,7 @@
         <v>http://www.geonovum.nl/imkl2015/1.0/def/TelecommunicationsAppurtenanceIMKLTypeValue/mof</v>
       </c>
     </row>
-    <row r="80" spans="1:7">
+    <row r="80" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>371</v>
       </c>
@@ -4114,7 +4113,7 @@
         <v>http://www.geonovum.nl/imkl2015/1.0/def/TelecommunicationsAppurtenanceIMKLTypeValue/verzameltermOndergrondseLeidingelementenOpnemen</v>
       </c>
     </row>
-    <row r="81" spans="1:7">
+    <row r="81" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>371</v>
       </c>
@@ -4138,7 +4137,7 @@
         <v>http://www.geonovum.nl/imkl2015/1.0/def/TelecommunicationsAppurtenanceIMKLTypeValue/kabelverdeler</v>
       </c>
     </row>
-    <row r="82" spans="1:7">
+    <row r="82" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>371</v>
       </c>
@@ -4162,7 +4161,7 @@
         <v>http://www.geonovum.nl/imkl2015/1.0/def/TelecommunicationsAppurtenanceIMKLTypeValue/Stijgleiding</v>
       </c>
     </row>
-    <row r="83" spans="1:7">
+    <row r="83" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>371</v>
       </c>
@@ -4186,7 +4185,7 @@
         <v>http://www.geonovum.nl/imkl2015/1.0/def/TelecommunicationsAppurtenanceIMKLTypeValue/GTWPOpnemen</v>
       </c>
     </row>
-    <row r="84" spans="1:7">
+    <row r="84" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>371</v>
       </c>
@@ -4210,7 +4209,7 @@
         <v>http://www.geonovum.nl/imkl2015/1.0/def/TelecommunicationsAppurtenanceIMKLTypeValue/afdekplaten</v>
       </c>
     </row>
-    <row r="85" spans="1:7">
+    <row r="85" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>371</v>
       </c>
@@ -4234,12 +4233,12 @@
         <v>http://www.geonovum.nl/imkl2015/1.0/def/TelecommunicationsAppurtenanceIMKLTypeValue/doorvoerramen</v>
       </c>
     </row>
-    <row r="86" spans="1:7">
+    <row r="86" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>371</v>
       </c>
       <c r="B86" s="17" t="s">
-        <v>28</v>
+        <v>206</v>
       </c>
       <c r="C86" s="17" t="s">
         <v>135</v>
@@ -4255,15 +4254,15 @@
       </c>
       <c r="G86" t="str">
         <f t="shared" si="1"/>
-        <v>http://inspire.ec.europa.eu/codelist/TelecommunicationsCableMaterialTypeValue/coaxial</v>
-      </c>
-    </row>
-    <row r="87" spans="1:7">
+        <v>http://www.geonovum.nl/imkl2015/1.0/def/TelecommunicationsCableMaterialTypeValue/coaxial</v>
+      </c>
+    </row>
+    <row r="87" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>371</v>
       </c>
       <c r="B87" s="17" t="s">
-        <v>28</v>
+        <v>206</v>
       </c>
       <c r="C87" s="17" t="s">
         <v>135</v>
@@ -4279,15 +4278,15 @@
       </c>
       <c r="G87" t="str">
         <f t="shared" si="1"/>
-        <v>http://inspire.ec.europa.eu/codelist/TelecommunicationsCableMaterialTypeValue/opticalFiber</v>
-      </c>
-    </row>
-    <row r="88" spans="1:7">
+        <v>http://www.geonovum.nl/imkl2015/1.0/def/TelecommunicationsCableMaterialTypeValue/opticalFiber</v>
+      </c>
+    </row>
+    <row r="88" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>371</v>
       </c>
       <c r="B88" s="17" t="s">
-        <v>28</v>
+        <v>206</v>
       </c>
       <c r="C88" s="17" t="s">
         <v>135</v>
@@ -4303,10 +4302,10 @@
       </c>
       <c r="G88" t="str">
         <f t="shared" si="1"/>
-        <v>http://inspire.ec.europa.eu/codelist/TelecommunicationsCableMaterialTypeValue/twistedPair</v>
-      </c>
-    </row>
-    <row r="89" spans="1:7" ht="15" thickBot="1">
+        <v>http://www.geonovum.nl/imkl2015/1.0/def/TelecommunicationsCableMaterialTypeValue/twistedPair</v>
+      </c>
+    </row>
+    <row r="89" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
         <v>371</v>
       </c>
@@ -4327,7 +4326,7 @@
         <v>http://www.geonovum.nl/imkl2015/1.0/def/TelecommunicationsAppurtenanceIMKLTypeValue/puntVanLevering</v>
       </c>
     </row>
-    <row r="90" spans="1:7" ht="15" hidden="1" thickBot="1">
+    <row r="90" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
         <v>372</v>
       </c>
@@ -4351,7 +4350,7 @@
         <v>http://www.geonovum.nl/imkl2015/1.0/def/OilGasChemicalsAppurtenanceIMKLTypeValue/buis</v>
       </c>
     </row>
-    <row r="91" spans="1:7" ht="15" hidden="1" thickBot="1">
+    <row r="91" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A91" t="s">
         <v>372</v>
       </c>
@@ -4375,7 +4374,7 @@
         <v>http://www.geonovum.nl/imkl2015/1.0/def/OilGasChemicalsAppurtenanceIMKLTypeValue/bocht</v>
       </c>
     </row>
-    <row r="92" spans="1:7" ht="15" hidden="1" thickBot="1">
+    <row r="92" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A92" t="s">
         <v>372</v>
       </c>
@@ -4399,7 +4398,7 @@
         <v>http://www.geonovum.nl/imkl2015/1.0/def/OilGasChemicalsAppurtenanceIMKLTypeValue/tstuk</v>
       </c>
     </row>
-    <row r="93" spans="1:7" ht="15" hidden="1" thickBot="1">
+    <row r="93" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A93" t="s">
         <v>372</v>
       </c>
@@ -4423,7 +4422,7 @@
         <v>http://www.geonovum.nl/imkl2015/1.0/def/OilGasChemicalsAppurtenanceIMKLTypeValue/bodem</v>
       </c>
     </row>
-    <row r="94" spans="1:7" ht="15" hidden="1" thickBot="1">
+    <row r="94" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A94" t="s">
         <v>372</v>
       </c>
@@ -4447,7 +4446,7 @@
         <v>http://www.geonovum.nl/imkl2015/1.0/def/OilGasChemicalsAppurtenanceIMKLTypeValue/lasnok</v>
       </c>
     </row>
-    <row r="95" spans="1:7" ht="15" hidden="1" thickBot="1">
+    <row r="95" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A95" t="s">
         <v>372</v>
       </c>
@@ -4471,7 +4470,7 @@
         <v>http://www.geonovum.nl/imkl2015/1.0/def/OilGasChemicalsAppurtenanceIMKLTypeValue/expansiestuk</v>
       </c>
     </row>
-    <row r="96" spans="1:7" ht="15" hidden="1" thickBot="1">
+    <row r="96" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A96" t="s">
         <v>372</v>
       </c>
@@ -4495,7 +4494,7 @@
         <v>http://www.geonovum.nl/imkl2015/1.0/def/OilGasChemicalsAppurtenanceIMKLTypeValue/isolatieKoppeling</v>
       </c>
     </row>
-    <row r="97" spans="1:7" ht="15" hidden="1" thickBot="1">
+    <row r="97" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A97" t="s">
         <v>372</v>
       </c>
@@ -4519,7 +4518,7 @@
         <v>http://www.geonovum.nl/imkl2015/1.0/def/OilGasChemicalsAppurtenanceIMKLTypeValue/vloeistofvanger</v>
       </c>
     </row>
-    <row r="98" spans="1:7" ht="15" hidden="1" thickBot="1">
+    <row r="98" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A98" t="s">
         <v>372</v>
       </c>
@@ -4543,7 +4542,7 @@
         <v>http://www.geonovum.nl/imkl2015/1.0/def/OilGasChemicalsAppurtenanceIMKLTypeValue/Raaginrichting</v>
       </c>
     </row>
-    <row r="99" spans="1:7" ht="15" hidden="1" thickBot="1">
+    <row r="99" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A99" t="s">
         <v>372</v>
       </c>
@@ -4567,7 +4566,7 @@
         <v>http://www.geonovum.nl/imkl2015/1.0/def/OilGasChemicalsAppurtenanceIMKLTypeValue/algemeenGasTransportOnderdeel</v>
       </c>
     </row>
-    <row r="100" spans="1:7" ht="15" hidden="1" thickBot="1">
+    <row r="100" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A100" t="s">
         <v>372</v>
       </c>
@@ -4591,7 +4590,7 @@
         <v>http://www.geonovum.nl/imkl2015/1.0/def/OilGasChemicalsProductIMKLTypeValue/mud</v>
       </c>
     </row>
-    <row r="101" spans="1:7" ht="15" hidden="1" thickBot="1">
+    <row r="101" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A101" t="s">
         <v>372</v>
       </c>
@@ -4615,7 +4614,7 @@
         <v>http://www.geonovum.nl/imkl2015/1.0/def/OilGasChemicalsProductIMKLTypeValue/methanol</v>
       </c>
     </row>
-    <row r="102" spans="1:7" hidden="1">
+    <row r="102" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
         <v>372</v>
       </c>
@@ -4639,7 +4638,7 @@
         <v>http://www.geonovum.nl/imkl2015/1.0/def/OilGasChemicalsProductIMKLTypeValue/emulsie</v>
       </c>
     </row>
-    <row r="103" spans="1:7" hidden="1">
+    <row r="103" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A103" t="s">
         <v>372</v>
       </c>
@@ -4663,7 +4662,7 @@
         <v>http://www.geonovum.nl/imkl2015/1.0/def/OilGasChemicalsProductIMKLTypeValue/glycol</v>
       </c>
     </row>
-    <row r="104" spans="1:7" ht="15" hidden="1" thickBot="1">
+    <row r="104" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A104" t="s">
         <v>372</v>
       </c>
@@ -4687,7 +4686,7 @@
         <v>http://www.geonovum.nl/imkl2015/1.0/def/OilGasChemicalsAppurtenanceIMKLTypeValue/hoogbouwkoppelpunt</v>
       </c>
     </row>
-    <row r="105" spans="1:7" ht="15" hidden="1" thickBot="1">
+    <row r="105" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A105" t="s">
         <v>372</v>
       </c>
@@ -4711,7 +4710,7 @@
         <v>http://www.geonovum.nl/imkl2015/1.0/def/OilGasChemicalsAppurtenanceIMKLTypeValue/ontluchting</v>
       </c>
     </row>
-    <row r="106" spans="1:7" hidden="1">
+    <row r="106" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
         <v>372</v>
       </c>
@@ -4735,7 +4734,7 @@
         <v>http://www.geonovum.nl/imkl2015/1.0/def/OilGasChemicalsAppurtenanceIMKLTypeValue/aftakzadel</v>
       </c>
     </row>
-    <row r="107" spans="1:7" hidden="1">
+    <row r="107" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
         <v>372</v>
       </c>
@@ -4759,7 +4758,7 @@
         <v>http://www.geonovum.nl/imkl2015/1.0/def/OilGasChemicalsAppurtenanceIMKLTypeValue/overgangsstuk</v>
       </c>
     </row>
-    <row r="108" spans="1:7" hidden="1">
+    <row r="108" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
         <v>372</v>
       </c>
@@ -4783,7 +4782,7 @@
         <v>http://www.geonovum.nl/imkl2015/1.0/def/OilGasChemicalsAppurtenanceIMKLTypeValue/isolatiestuk</v>
       </c>
     </row>
-    <row r="109" spans="1:7" hidden="1">
+    <row r="109" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
         <v>372</v>
       </c>
@@ -4807,7 +4806,7 @@
         <v>http://www.geonovum.nl/imkl2015/1.0/def/OilGasChemicalsAppurtenanceIMKLTypeValue/ontspanningselement</v>
       </c>
     </row>
-    <row r="110" spans="1:7" hidden="1">
+    <row r="110" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
         <v>372</v>
       </c>
@@ -4831,7 +4830,7 @@
         <v>http://www.geonovum.nl/imkl2015/1.0/def/OilGasChemicalsAppurtenanceIMKLTypeValue/hoogteligging</v>
       </c>
     </row>
-    <row r="111" spans="1:7" hidden="1">
+    <row r="111" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
         <v>372</v>
       </c>
@@ -4855,7 +4854,7 @@
         <v>http://www.geonovum.nl/imkl2015/1.0/def/OilGasChemicalsAppurtenanceIMKLTypeValue/adrespunt</v>
       </c>
     </row>
-    <row r="112" spans="1:7" hidden="1">
+    <row r="112" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
         <v>372</v>
       </c>
@@ -4879,7 +4878,7 @@
         <v>http://www.geonovum.nl/imkl2015/1.0/def/OilGasChemicalsAppurtenanceIMKLTypeValue/eindkap</v>
       </c>
     </row>
-    <row r="113" spans="1:7" hidden="1">
+    <row r="113" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
         <v>372</v>
       </c>
@@ -4903,7 +4902,7 @@
         <v>http://www.geonovum.nl/imkl2015/1.0/def/OilGasChemicalsAppurtenanceIMKLTypeValue/verloopstuk</v>
       </c>
     </row>
-    <row r="114" spans="1:7" hidden="1">
+    <row r="114" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
         <v>372</v>
       </c>
@@ -4927,7 +4926,7 @@
         <v>http://www.geonovum.nl/imkl2015/1.0/def/OilGasChemicalsAppurtenanceIMKLTypeValue/afsluiter</v>
       </c>
     </row>
-    <row r="115" spans="1:7" hidden="1">
+    <row r="115" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
         <v>372</v>
       </c>
@@ -4951,7 +4950,7 @@
         <v>http://www.geonovum.nl/imkl2015/1.0/def/OilGasChemicalsAppurtenanceIMKLTypeValue/meetpunt</v>
       </c>
     </row>
-    <row r="116" spans="1:7" hidden="1">
+    <row r="116" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
         <v>372</v>
       </c>
@@ -4975,7 +4974,7 @@
         <v>http://www.geonovum.nl/imkl2015/1.0/def/OilGasChemicalsAppurtenanceIMKLTypeValue/sifon</v>
       </c>
     </row>
-    <row r="117" spans="1:7" hidden="1">
+    <row r="117" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
         <v>372</v>
       </c>
@@ -4999,7 +4998,7 @@
         <v>http://www.geonovum.nl/imkl2015/1.0/def/OilGasChemicalsAppurtenanceIMKLTypeValue/blaasgat</v>
       </c>
     </row>
-    <row r="118" spans="1:7" hidden="1">
+    <row r="118" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
         <v>372</v>
       </c>
@@ -5023,7 +5022,7 @@
         <v>http://www.geonovum.nl/imkl2015/1.0/def/OilGasChemicalsAppurtenanceIMKLTypeValue/kbMeetpunt</v>
       </c>
     </row>
-    <row r="119" spans="1:7" hidden="1">
+    <row r="119" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
         <v>372</v>
       </c>
@@ -5047,7 +5046,7 @@
         <v>http://inspire.ec.europa.eu/codelist/OilGasChemicalsAppurtenanceTypeValue/gasStation</v>
       </c>
     </row>
-    <row r="120" spans="1:7" hidden="1">
+    <row r="120" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
         <v>372</v>
       </c>
@@ -5071,7 +5070,7 @@
         <v>http://inspire.ec.europa.eu/codelist/OilGasChemicalsAppurtenanceTypeValue/oilGasChemicalsNode</v>
       </c>
     </row>
-    <row r="121" spans="1:7" hidden="1">
+    <row r="121" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
         <v>372</v>
       </c>
@@ -5095,7 +5094,7 @@
         <v>http://inspire.ec.europa.eu/codelist/OilGasChemicalsAppurtenanceTypeValue/marker</v>
       </c>
     </row>
-    <row r="122" spans="1:7" hidden="1">
+    <row r="122" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
         <v>372</v>
       </c>
@@ -5119,7 +5118,7 @@
         <v>http://inspire.ec.europa.eu/codelist/OilGasChemicalsAppurtenanceTypeValue/deliveryPoint</v>
       </c>
     </row>
-    <row r="123" spans="1:7" hidden="1">
+    <row r="123" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
         <v>372</v>
       </c>
@@ -5143,7 +5142,7 @@
         <v>http://inspire.ec.europa.eu/codelist/OilGasChemicalsAppurtenanceTypeValue/terminal</v>
       </c>
     </row>
-    <row r="124" spans="1:7" hidden="1">
+    <row r="124" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
         <v>372</v>
       </c>
@@ -5167,7 +5166,7 @@
         <v>http://inspire.ec.europa.eu/codelist/OilGasChemicalsAppurtenanceTypeValue/pump</v>
       </c>
     </row>
-    <row r="125" spans="1:7" hidden="1">
+    <row r="125" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
         <v>372</v>
       </c>
@@ -5191,7 +5190,7 @@
         <v>http://inspire.ec.europa.eu/codelist/OilGasChemicalsAppurtenanceTypeValue/pumpingStation</v>
       </c>
     </row>
-    <row r="126" spans="1:7" hidden="1">
+    <row r="126" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
         <v>372</v>
       </c>
@@ -5215,7 +5214,7 @@
         <v>http://inspire.ec.europa.eu/codelist/OilGasChemicalsAppurtenanceTypeValue/productionRegion</v>
       </c>
     </row>
-    <row r="127" spans="1:7" hidden="1">
+    <row r="127" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
         <v>372</v>
       </c>
@@ -5239,7 +5238,7 @@
         <v>http://inspire.ec.europa.eu/codelist/OilGasChemicalsAppurtenanceTypeValue/storage</v>
       </c>
     </row>
-    <row r="128" spans="1:7" hidden="1">
+    <row r="128" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
         <v>372</v>
       </c>
@@ -5263,7 +5262,7 @@
         <v>http://inspire.ec.europa.eu/codelist/OilGasChemicalsProductTypeValue/naturalGas</v>
       </c>
     </row>
-    <row r="129" spans="1:7" hidden="1">
+    <row r="129" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
         <v>372</v>
       </c>
@@ -5287,7 +5286,7 @@
         <v>http://www.geonovum.nl/imkl2015/1.0/def/OilGasChemicalsProductIMKLTypeValue/bioGas</v>
       </c>
     </row>
-    <row r="130" spans="1:7" hidden="1">
+    <row r="130" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
         <v>372</v>
       </c>
@@ -5311,7 +5310,7 @@
         <v>http://www.geonovum.nl/imkl2015/1.0/def/OilGasChemicalsProductTypeValue/accetone</v>
       </c>
     </row>
-    <row r="131" spans="1:7" hidden="1">
+    <row r="131" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
         <v>372</v>
       </c>
@@ -5335,7 +5334,7 @@
         <v>http://www.geonovum.nl/imkl2015/1.0/def/OilGasChemicalsProductTypeValue/air</v>
       </c>
     </row>
-    <row r="132" spans="1:7" hidden="1">
+    <row r="132" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
         <v>372</v>
       </c>
@@ -5359,7 +5358,7 @@
         <v>http://www.geonovum.nl/imkl2015/1.0/def/OilGasChemicalsProductTypeValue/argon</v>
       </c>
     </row>
-    <row r="133" spans="1:7" hidden="1">
+    <row r="133" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
         <v>372</v>
       </c>
@@ -5383,7 +5382,7 @@
         <v>http://www.geonovum.nl/imkl2015/1.0/def/OilGasChemicalsProductTypeValue/butadiene1.2</v>
       </c>
     </row>
-    <row r="134" spans="1:7" hidden="1">
+    <row r="134" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
         <v>372</v>
       </c>
@@ -5407,7 +5406,7 @@
         <v>http://www.geonovum.nl/imkl2015/1.0/def/OilGasChemicalsProductTypeValue/butadiene1.3</v>
       </c>
     </row>
-    <row r="135" spans="1:7" hidden="1">
+    <row r="135" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
         <v>372</v>
       </c>
@@ -5431,7 +5430,7 @@
         <v>http://www.geonovum.nl/imkl2015/1.0/def/OilGasChemicalsProductTypeValue/butane</v>
       </c>
     </row>
-    <row r="136" spans="1:7" hidden="1">
+    <row r="136" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
         <v>372</v>
       </c>
@@ -5455,7 +5454,7 @@
         <v>http://www.geonovum.nl/imkl2015/1.0/def/OilGasChemicalsProductTypeValue/carbonMonoxide</v>
       </c>
     </row>
-    <row r="137" spans="1:7" hidden="1">
+    <row r="137" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
         <v>372</v>
       </c>
@@ -5479,7 +5478,7 @@
         <v>http://www.geonovum.nl/imkl2015/1.0/def/OilGasChemicalsProductTypeValue/chlorine</v>
       </c>
     </row>
-    <row r="138" spans="1:7" hidden="1">
+    <row r="138" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
         <v>372</v>
       </c>
@@ -5503,7 +5502,7 @@
         <v>http://www.geonovum.nl/imkl2015/1.0/def/OilGasChemicalsProductTypeValue/concrete</v>
       </c>
     </row>
-    <row r="139" spans="1:7" hidden="1">
+    <row r="139" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
         <v>372</v>
       </c>
@@ -5527,7 +5526,7 @@
         <v>http://www.geonovum.nl/imkl2015/1.0/def/OilGasChemicalsProductTypeValue/crude</v>
       </c>
     </row>
-    <row r="140" spans="1:7" hidden="1">
+    <row r="140" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
         <v>372</v>
       </c>
@@ -5551,7 +5550,7 @@
         <v>http://www.geonovum.nl/imkl2015/1.0/def/OilGasChemicalsProductTypeValue/dichloroethane</v>
       </c>
     </row>
-    <row r="141" spans="1:7" hidden="1">
+    <row r="141" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
         <v>372</v>
       </c>
@@ -5575,7 +5574,7 @@
         <v>http://www.geonovum.nl/imkl2015/1.0/def/OilGasChemicalsProductTypeValue/diesel</v>
       </c>
     </row>
-    <row r="142" spans="1:7" hidden="1">
+    <row r="142" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
         <v>372</v>
       </c>
@@ -5599,7 +5598,7 @@
         <v>http://www.geonovum.nl/imkl2015/1.0/def/OilGasChemicalsProductTypeValue/ethylene</v>
       </c>
     </row>
-    <row r="143" spans="1:7" hidden="1">
+    <row r="143" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
         <v>372</v>
       </c>
@@ -5623,7 +5622,7 @@
         <v>http://www.geonovum.nl/imkl2015/1.0/def/OilGasChemicalsProductTypeValue/gasFabricationOfCocs</v>
       </c>
     </row>
-    <row r="144" spans="1:7" hidden="1">
+    <row r="144" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
         <v>372</v>
       </c>
@@ -5647,7 +5646,7 @@
         <v>http://www.geonovum.nl/imkl2015/1.0/def/OilGasChemicalsProductTypeValue/gasHFx</v>
       </c>
     </row>
-    <row r="145" spans="1:7" hidden="1">
+    <row r="145" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
         <v>372</v>
       </c>
@@ -5671,7 +5670,7 @@
         <v>http://www.geonovum.nl/imkl2015/1.0/def/OilGasChemicalsProductTypeValue/gasoil</v>
       </c>
     </row>
-    <row r="146" spans="1:7" hidden="1">
+    <row r="146" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
         <v>372</v>
       </c>
@@ -5695,7 +5694,7 @@
         <v>http://www.geonovum.nl/imkl2015/1.0/def/OilGasChemicalsProductTypeValue/hydrogen</v>
       </c>
     </row>
-    <row r="147" spans="1:7" hidden="1">
+    <row r="147" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
         <v>372</v>
       </c>
@@ -5719,7 +5718,7 @@
         <v>http://www.geonovum.nl/imkl2015/1.0/def/OilGasChemicalsProductTypeValue/isobutane</v>
       </c>
     </row>
-    <row r="148" spans="1:7" hidden="1">
+    <row r="148" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
         <v>372</v>
       </c>
@@ -5743,7 +5742,7 @@
         <v>http://www.geonovum.nl/imkl2015/1.0/def/OilGasChemicalsProductTypeValue/JET-A1</v>
       </c>
     </row>
-    <row r="149" spans="1:7" hidden="1">
+    <row r="149" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
         <v>372</v>
       </c>
@@ -5767,7 +5766,7 @@
         <v>http://www.geonovum.nl/imkl2015/1.0/def/OilGasChemicalsProductTypeValue/kerosene</v>
       </c>
     </row>
-    <row r="150" spans="1:7" hidden="1">
+    <row r="150" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
         <v>372</v>
       </c>
@@ -5791,7 +5790,7 @@
         <v>http://www.geonovum.nl/imkl2015/1.0/def/OilGasChemicalsProductTypeValue/liquidAmmonia</v>
       </c>
     </row>
-    <row r="151" spans="1:7" hidden="1">
+    <row r="151" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
         <v>372</v>
       </c>
@@ -5815,7 +5814,7 @@
         <v>http://www.geonovum.nl/imkl2015/1.0/def/OilGasChemicalsProductTypeValue/liquidHydrocarbon</v>
       </c>
     </row>
-    <row r="152" spans="1:7" hidden="1">
+    <row r="152" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
         <v>372</v>
       </c>
@@ -5839,7 +5838,7 @@
         <v>http://www.geonovum.nl/imkl2015/1.0/def/OilGasChemicalsProductTypeValue/multiProduct</v>
       </c>
     </row>
-    <row r="153" spans="1:7" hidden="1">
+    <row r="153" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
         <v>372</v>
       </c>
@@ -5863,7 +5862,7 @@
         <v>http://www.geonovum.nl/imkl2015/1.0/def/OilGasChemicalsProductTypeValue/MVC</v>
       </c>
     </row>
-    <row r="154" spans="1:7" hidden="1">
+    <row r="154" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
         <v>372</v>
       </c>
@@ -5887,7 +5886,7 @@
         <v>http://www.geonovum.nl/imkl2015/1.0/def/OilGasChemicalsProductTypeValue/nitrogen</v>
       </c>
     </row>
-    <row r="155" spans="1:7" hidden="1">
+    <row r="155" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
         <v>372</v>
       </c>
@@ -5911,7 +5910,7 @@
         <v>http://www.geonovum.nl/imkl2015/1.0/def/OilGasChemicalsProductTypeValue/oxygen</v>
       </c>
     </row>
-    <row r="156" spans="1:7" hidden="1">
+    <row r="156" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
         <v>372</v>
       </c>
@@ -5935,7 +5934,7 @@
         <v>http://www.geonovum.nl/imkl2015/1.0/def/OilGasChemicalsProductTypeValue/phenol</v>
       </c>
     </row>
-    <row r="157" spans="1:7" hidden="1">
+    <row r="157" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
         <v>372</v>
       </c>
@@ -5959,7 +5958,7 @@
         <v>http://www.geonovum.nl/imkl2015/1.0/def/OilGasChemicalsProductTypeValue/propane</v>
       </c>
     </row>
-    <row r="158" spans="1:7" hidden="1">
+    <row r="158" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
         <v>372</v>
       </c>
@@ -5983,7 +5982,7 @@
         <v>http://www.geonovum.nl/imkl2015/1.0/def/OilGasChemicalsProductTypeValue/propylene</v>
       </c>
     </row>
-    <row r="159" spans="1:7" hidden="1">
+    <row r="159" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
         <v>372</v>
       </c>
@@ -6007,7 +6006,7 @@
         <v>http://www.geonovum.nl/imkl2015/1.0/def/OilGasChemicalsProductTypeValue/saltWater</v>
       </c>
     </row>
-    <row r="160" spans="1:7" hidden="1">
+    <row r="160" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
         <v>372</v>
       </c>
@@ -6031,7 +6030,7 @@
         <v>http://www.geonovum.nl/imkl2015/1.0/def/OilGasChemicalsProductTypeValue/saumur</v>
       </c>
     </row>
-    <row r="161" spans="1:7" hidden="1">
+    <row r="161" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A161" t="s">
         <v>372</v>
       </c>
@@ -6055,7 +6054,7 @@
         <v>http://www.geonovum.nl/imkl2015/1.0/def/OilGasChemicalsProductTypeValue/sand</v>
       </c>
     </row>
-    <row r="162" spans="1:7" hidden="1">
+    <row r="162" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A162" t="s">
         <v>372</v>
       </c>
@@ -6079,7 +6078,7 @@
         <v>http://www.geonovum.nl/imkl2015/1.0/def/OilGasChemicalsProductTypeValue/tetrachloroide</v>
       </c>
     </row>
-    <row r="163" spans="1:7" hidden="1">
+    <row r="163" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A163" t="s">
         <v>372</v>
       </c>
@@ -6103,7 +6102,7 @@
         <v>http://www.geonovum.nl/imkl2015/1.0/def/OilGasChemicalsProductTypeValue/unknown</v>
       </c>
     </row>
-    <row r="164" spans="1:7" hidden="1">
+    <row r="164" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A164" t="s">
         <v>372</v>
       </c>
@@ -6127,7 +6126,7 @@
         <v>http://www.geonovum.nl/imkl2015/1.0/def/OilGasChemicalsProductTypeValue/water</v>
       </c>
     </row>
-    <row r="165" spans="1:7" hidden="1">
+    <row r="165" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A165" t="s">
         <v>372</v>
       </c>
@@ -6151,7 +6150,7 @@
         <v>http://www.geonovum.nl/imkl2015/1.0/def/OilGasChemicalsProductTypeValue/empty</v>
       </c>
     </row>
-    <row r="166" spans="1:7" ht="15" hidden="1" thickBot="1">
+    <row r="166" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A166" s="4" t="s">
         <v>114</v>
       </c>
@@ -6175,7 +6174,7 @@
         <v>http://www.geonovum.nl/imkl2015/1.0/def/WaterAppurtenanceTypeIMKLValue/afsluiter</v>
       </c>
     </row>
-    <row r="167" spans="1:7" ht="15" hidden="1" thickBot="1">
+    <row r="167" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A167" s="4" t="s">
         <v>114</v>
       </c>
@@ -6199,7 +6198,7 @@
         <v>http://www.geonovum.nl/imkl2015/1.0/def/WaterAppurtenanceTypeIMKLValue/diameterovergang</v>
       </c>
     </row>
-    <row r="168" spans="1:7" ht="15" hidden="1" thickBot="1">
+    <row r="168" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A168" s="4" t="s">
         <v>114</v>
       </c>
@@ -6223,7 +6222,7 @@
         <v>http://www.geonovum.nl/imkl2015/1.0/def/WaterAppurtenanceTypeIMKLValue/materiaalovergang</v>
       </c>
     </row>
-    <row r="169" spans="1:7" ht="15" hidden="1" thickBot="1">
+    <row r="169" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A169" s="4" t="s">
         <v>114</v>
       </c>
@@ -6247,7 +6246,7 @@
         <v>http://www.geonovum.nl/imkl2015/1.0/def/WaterAppurtenanceTypeIMKLValue/eindpunt</v>
       </c>
     </row>
-    <row r="170" spans="1:7" ht="15" hidden="1" thickBot="1">
+    <row r="170" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A170" s="4" t="s">
         <v>114</v>
       </c>
@@ -6271,7 +6270,7 @@
         <v>http://www.geonovum.nl/imkl2015/1.0/def/WaterAppurtenanceTypeIMKLValue/blindflens</v>
       </c>
     </row>
-    <row r="171" spans="1:7" ht="15" hidden="1" thickBot="1">
+    <row r="171" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A171" s="4" t="s">
         <v>114</v>
       </c>
@@ -6295,7 +6294,7 @@
         <v>http://inspire.ec.europa.eu/codelist/WaterAppurtenanceTypeValue/checkValve</v>
       </c>
     </row>
-    <row r="172" spans="1:7" ht="15" hidden="1" thickBot="1">
+    <row r="172" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A172" s="4" t="s">
         <v>114</v>
       </c>
@@ -6319,7 +6318,7 @@
         <v>http://inspire.ec.europa.eu/codelist/WaterAppurtenanceTypeValue/waterExhaustPoint</v>
       </c>
     </row>
-    <row r="173" spans="1:7" ht="15" hidden="1" thickBot="1">
+    <row r="173" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A173" s="4" t="s">
         <v>114</v>
       </c>
@@ -6343,7 +6342,7 @@
         <v>http://inspire.ec.europa.eu/codelist/WaterAppurtenanceTypeValue/waterDischargePoint</v>
       </c>
     </row>
-    <row r="174" spans="1:7" ht="15" hidden="1" thickBot="1">
+    <row r="174" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A174" s="4" t="s">
         <v>114</v>
       </c>
@@ -6367,7 +6366,7 @@
         <v>http://inspire.ec.europa.eu/codelist/WaterAppurtenanceTypeValue/anode</v>
       </c>
     </row>
-    <row r="175" spans="1:7" ht="15" hidden="1" thickBot="1">
+    <row r="175" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A175" s="4" t="s">
         <v>114</v>
       </c>
@@ -6391,7 +6390,7 @@
         <v>http://inspire.ec.europa.eu/codelist/WaterAppurtenanceTypeValue/fireHydrant</v>
       </c>
     </row>
-    <row r="176" spans="1:7" ht="15" hidden="1" thickBot="1">
+    <row r="176" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A176" s="4" t="s">
         <v>114</v>
       </c>
@@ -6415,7 +6414,7 @@
         <v>http://inspire.ec.europa.eu/codelist/WaterAppurtenanceTypeValue/well</v>
       </c>
     </row>
-    <row r="177" spans="1:7" ht="15" hidden="1" thickBot="1">
+    <row r="177" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A177" s="4" t="s">
         <v>114</v>
       </c>
@@ -6439,7 +6438,7 @@
         <v>http://inspire.ec.europa.eu/codelist/WaterAppurtenanceTypeValue/controlValve</v>
       </c>
     </row>
-    <row r="178" spans="1:7" ht="15" hidden="1" thickBot="1">
+    <row r="178" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A178" s="4" t="s">
         <v>114</v>
       </c>
@@ -6463,7 +6462,7 @@
         <v>http://inspire.ec.europa.eu/codelist/WaterAppurtenanceTypeValue/pressureController</v>
       </c>
     </row>
-    <row r="179" spans="1:7" ht="15" hidden="1" thickBot="1">
+    <row r="179" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A179" s="4" t="s">
         <v>114</v>
       </c>
@@ -6487,7 +6486,7 @@
         <v>http://inspire.ec.europa.eu/codelist/WaterAppurtenanceTypeValue/junction</v>
       </c>
     </row>
-    <row r="180" spans="1:7" ht="15" hidden="1" thickBot="1">
+    <row r="180" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A180" s="4" t="s">
         <v>114</v>
       </c>
@@ -6511,7 +6510,7 @@
         <v>http://inspire.ec.europa.eu/codelist/WaterAppurtenanceTypeValue/lateralPoint</v>
       </c>
     </row>
-    <row r="181" spans="1:7" ht="15" hidden="1" thickBot="1">
+    <row r="181" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A181" s="4" t="s">
         <v>114</v>
       </c>
@@ -6535,7 +6534,7 @@
         <v>http://inspire.ec.europa.eu/codelist/WaterAppurtenanceTypeValue/samplingStation</v>
       </c>
     </row>
-    <row r="182" spans="1:7" ht="15" hidden="1" thickBot="1">
+    <row r="182" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A182" s="4" t="s">
         <v>114</v>
       </c>
@@ -6559,7 +6558,7 @@
         <v>http://inspire.ec.europa.eu/codelist/WaterAppurtenanceTypeValue/meter</v>
       </c>
     </row>
-    <row r="183" spans="1:7" ht="15" hidden="1" thickBot="1">
+    <row r="183" spans="1:7" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A183" s="4" t="s">
         <v>114</v>
       </c>
@@ -6583,7 +6582,7 @@
         <v>http://inspire.ec.europa.eu/codelist/WaterAppurtenanceTypeValue/airRelieveValve</v>
       </c>
     </row>
-    <row r="184" spans="1:7" ht="15" hidden="1" thickBot="1">
+    <row r="184" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A184" s="4" t="s">
         <v>114</v>
       </c>
@@ -6607,7 +6606,7 @@
         <v>http://inspire.ec.europa.eu/codelist/WaterAppurtenanceTypeValue/storageFacility</v>
       </c>
     </row>
-    <row r="185" spans="1:7" ht="15" hidden="1" thickBot="1">
+    <row r="185" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A185" s="4" t="s">
         <v>114</v>
       </c>
@@ -6631,7 +6630,7 @@
         <v>http://inspire.ec.europa.eu/codelist/WaterAppurtenanceTypeValue/pumpStation</v>
       </c>
     </row>
-    <row r="186" spans="1:7" ht="15" hidden="1" thickBot="1">
+    <row r="186" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A186" s="4" t="s">
         <v>114</v>
       </c>
@@ -6655,7 +6654,7 @@
         <v>http://inspire.ec.europa.eu/codelist/WaterAppurtenanceTypeValue/waterServicePoint</v>
       </c>
     </row>
-    <row r="187" spans="1:7" ht="15" hidden="1" thickBot="1">
+    <row r="187" spans="1:7" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A187" s="4" t="s">
         <v>114</v>
       </c>
@@ -6679,7 +6678,7 @@
         <v>http://inspire.ec.europa.eu/codelist/WaterAppurtenanceTypeValue/treatmentPlant</v>
       </c>
     </row>
-    <row r="188" spans="1:7" ht="15" hidden="1" thickBot="1">
+    <row r="188" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A188" s="4" t="s">
         <v>114</v>
       </c>
@@ -6703,7 +6702,7 @@
         <v>http://www.geonovum.nl/imkl2015/1.0/def/WaterTypeValue/industrial</v>
       </c>
     </row>
-    <row r="189" spans="1:7" ht="15" hidden="1" thickBot="1">
+    <row r="189" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A189" s="4" t="s">
         <v>114</v>
       </c>
@@ -6727,7 +6726,7 @@
         <v>http://www.geonovum.nl/imkl2015/1.0/def/WaterTypeValue/waste</v>
       </c>
     </row>
-    <row r="190" spans="1:7" ht="15" hidden="1" thickBot="1">
+    <row r="190" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A190" s="4" t="s">
         <v>114</v>
       </c>
@@ -6751,7 +6750,7 @@
         <v>http://inspire.ec.europa.eu/codelist/WaterTypeValue/potable</v>
       </c>
     </row>
-    <row r="191" spans="1:7" ht="15" hidden="1" thickBot="1">
+    <row r="191" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A191" s="4" t="s">
         <v>114</v>
       </c>
@@ -6775,7 +6774,7 @@
         <v>http://inspire.ec.europa.eu/codelist/WaterTypeValue/raw</v>
       </c>
     </row>
-    <row r="192" spans="1:7" ht="15" hidden="1" thickBot="1">
+    <row r="192" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A192" s="4" t="s">
         <v>114</v>
       </c>
@@ -6799,7 +6798,7 @@
         <v>http://inspire.ec.europa.eu/codelist/WaterTypeValue/salt</v>
       </c>
     </row>
-    <row r="193" spans="1:7" ht="15" hidden="1" thickBot="1">
+    <row r="193" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A193" s="4" t="s">
         <v>114</v>
       </c>
@@ -6823,7 +6822,7 @@
         <v>http://inspire.ec.europa.eu/codelist/WaterTypeValue/treated</v>
       </c>
     </row>
-    <row r="194" spans="1:7" ht="15" hidden="1" thickBot="1">
+    <row r="194" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A194" s="4" t="s">
         <v>114</v>
       </c>
@@ -6843,7 +6842,7 @@
         <v>http://www.geonovum.nl/imkl2015/1.0/def/WaterAppurtenanceIMKLTypeValue/puntVanLevering</v>
       </c>
     </row>
-    <row r="195" spans="1:7" ht="15" hidden="1" thickBot="1">
+    <row r="195" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A195" s="4" t="s">
         <v>373</v>
       </c>
@@ -6867,7 +6866,7 @@
         <v>http://www.geonovum.nl/imkl2015/1.0/def/SewerAppurtenanceTypeIMKLValue/gemaal</v>
       </c>
     </row>
-    <row r="196" spans="1:7" ht="29" hidden="1" thickBot="1">
+    <row r="196" spans="1:7" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A196" s="4" t="s">
         <v>373</v>
       </c>
@@ -6891,7 +6890,7 @@
         <v>http://www.geonovum.nl/imkl2015/1.0/def/SewerAppurtenanceTypeIMKLValue/infiltratievoorziening</v>
       </c>
     </row>
-    <row r="197" spans="1:7" ht="15" hidden="1" thickBot="1">
+    <row r="197" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A197" s="4" t="s">
         <v>373</v>
       </c>
@@ -6915,7 +6914,7 @@
         <v>http://www.geonovum.nl/imkl2015/1.0/def/SewerAppurtenanceTypeIMKLValue/kolk</v>
       </c>
     </row>
-    <row r="198" spans="1:7" ht="15" hidden="1" thickBot="1">
+    <row r="198" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A198" s="4" t="s">
         <v>373</v>
       </c>
@@ -6939,7 +6938,7 @@
         <v>http://www.geonovum.nl/imkl2015/1.0/def/SewerAppurtenanceTypeIMKLValue/kunstwerk</v>
       </c>
     </row>
-    <row r="199" spans="1:7" hidden="1">
+    <row r="199" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A199" s="4" t="s">
         <v>373</v>
       </c>
@@ -6963,7 +6962,7 @@
         <v>http://www.geonovum.nl/imkl2015/1.0/def/SewerAppurtenanceTypeIMKLValue/reservoir</v>
       </c>
     </row>
-    <row r="200" spans="1:7" hidden="1">
+    <row r="200" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A200" s="4" t="s">
         <v>373</v>
       </c>
@@ -6987,7 +6986,7 @@
         <v>http://www.geonovum.nl/imkl2015/1.0/def/SewerAppurtenanceTypeIMKLValue/uitlaatconstructie</v>
       </c>
     </row>
-    <row r="201" spans="1:7" ht="15" hidden="1" thickBot="1">
+    <row r="201" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A201" s="4" t="s">
         <v>373</v>
       </c>
@@ -7011,7 +7010,7 @@
         <v>http://inspire.ec.europa.eu/codelist/SewerAppurtenanceTypeValue/connection</v>
       </c>
     </row>
-    <row r="202" spans="1:7" ht="15" hidden="1" thickBot="1">
+    <row r="202" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A202" s="4" t="s">
         <v>373</v>
       </c>
@@ -7035,7 +7034,7 @@
         <v>http://inspire.ec.europa.eu/codelist/SewerAppurtenanceTypeValue/cleanOut</v>
       </c>
     </row>
-    <row r="203" spans="1:7" ht="15" hidden="1" thickBot="1">
+    <row r="203" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A203" s="4" t="s">
         <v>373</v>
       </c>
@@ -7059,7 +7058,7 @@
         <v>http://inspire.ec.europa.eu/codelist/SewerAppurtenanceTypeValue/barrel</v>
       </c>
     </row>
-    <row r="204" spans="1:7" ht="15" hidden="1" thickBot="1">
+    <row r="204" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A204" s="4" t="s">
         <v>373</v>
       </c>
@@ -7083,7 +7082,7 @@
         <v>http://inspire.ec.europa.eu/codelist/SewerAppurtenanceTypeValue/catchBasin</v>
       </c>
     </row>
-    <row r="205" spans="1:7" ht="15" hidden="1" thickBot="1">
+    <row r="205" spans="1:7" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A205" s="4" t="s">
         <v>373</v>
       </c>
@@ -7107,7 +7106,7 @@
         <v>http://inspire.ec.europa.eu/codelist/SewerAppurtenanceTypeValue/watertankOrChamber</v>
       </c>
     </row>
-    <row r="206" spans="1:7" ht="15" hidden="1" thickBot="1">
+    <row r="206" spans="1:7" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A206" s="4" t="s">
         <v>373</v>
       </c>
@@ -7131,7 +7130,7 @@
         <v>http://inspire.ec.europa.eu/codelist/SewerAppurtenanceTypeValue/specificStructure</v>
       </c>
     </row>
-    <row r="207" spans="1:7" hidden="1">
+    <row r="207" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A207" s="4" t="s">
         <v>373</v>
       </c>
@@ -7155,7 +7154,7 @@
         <v>http://www.geonovum.nl/imkl2015/1.0/def/SewerAppurtenanceTypeIMKLValue/overstort</v>
       </c>
     </row>
-    <row r="208" spans="1:7" hidden="1">
+    <row r="208" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A208" s="4" t="s">
         <v>373</v>
       </c>
@@ -7179,7 +7178,7 @@
         <v>http://inspire.ec.europa.eu/codelist/SewerAppurtenanceTypeValue/thrustProtection</v>
       </c>
     </row>
-    <row r="209" spans="1:7" hidden="1">
+    <row r="209" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A209" s="4" t="s">
         <v>373</v>
       </c>
@@ -7203,7 +7202,7 @@
         <v>http://inspire.ec.europa.eu/codelist/SewerAppurtenanceTypeValue/tideGate</v>
       </c>
     </row>
-    <row r="210" spans="1:7" hidden="1">
+    <row r="210" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A210" s="4" t="s">
         <v>373</v>
       </c>
@@ -7227,7 +7226,7 @@
         <v>http://inspire.ec.europa.eu/codelist/SewerAppurtenanceTypeValue/dischargeStructure</v>
       </c>
     </row>
-    <row r="211" spans="1:7" ht="15" hidden="1" thickBot="1">
+    <row r="211" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A211" s="4" t="s">
         <v>373</v>
       </c>
@@ -7251,7 +7250,7 @@
         <v>http://inspire.ec.europa.eu/codelist/SewerWaterTypeValue/combined</v>
       </c>
     </row>
-    <row r="212" spans="1:7" ht="15" hidden="1" thickBot="1">
+    <row r="212" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A212" s="4" t="s">
         <v>373</v>
       </c>
@@ -7275,7 +7274,7 @@
         <v>http://inspire.ec.europa.eu/codelist/SewerWaterTypeValue/reclaimed</v>
       </c>
     </row>
-    <row r="213" spans="1:7" ht="15" hidden="1" thickBot="1">
+    <row r="213" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A213" s="4" t="s">
         <v>373</v>
       </c>
@@ -7299,7 +7298,7 @@
         <v>http://inspire.ec.europa.eu/codelist/SewerWaterTypeValue/sanitary</v>
       </c>
     </row>
-    <row r="214" spans="1:7" ht="15" hidden="1" thickBot="1">
+    <row r="214" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A214" s="4" t="s">
         <v>373</v>
       </c>
@@ -7323,7 +7322,7 @@
         <v>http://inspire.ec.europa.eu/codelist/SewerWaterTypeValue/storm</v>
       </c>
     </row>
-    <row r="215" spans="1:7" hidden="1">
+    <row r="215" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A215" s="4" t="s">
         <v>373</v>
       </c>
@@ -7344,7 +7343,7 @@
         <v>http://www.geonovum.nl/imkl2015/1.0/def/SewerAppurtenanceTypeIMKLValue/puntVanLevering</v>
       </c>
     </row>
-    <row r="216" spans="1:7" hidden="1">
+    <row r="216" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A216" s="4" t="s">
         <v>131</v>
       </c>
@@ -7368,7 +7367,7 @@
         <v>http://www.geonovum.nl/imkl2015/1.0/def/SewerAppurtenanceTypeIMKLValue/compensator</v>
       </c>
     </row>
-    <row r="217" spans="1:7" hidden="1">
+    <row r="217" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A217" s="4" t="s">
         <v>131</v>
       </c>
@@ -7392,7 +7391,7 @@
         <v>http://www.geonovum.nl/imkl2015/1.0/def/SewerAppurtenanceTypeIMKLValue/lekdetectiemeetpunt</v>
       </c>
     </row>
-    <row r="218" spans="1:7" hidden="1">
+    <row r="218" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A218" s="4" t="s">
         <v>131</v>
       </c>
@@ -7416,7 +7415,7 @@
         <v>http://www.geonovum.nl/imkl2015/1.0/def/SewerAppurtenanceTypeIMKLValue/putten</v>
       </c>
     </row>
-    <row r="219" spans="1:7" hidden="1">
+    <row r="219" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A219" s="4" t="s">
         <v>131</v>
       </c>
@@ -7440,7 +7439,7 @@
         <v>http://www.geonovum.nl/imkl2015/1.0/def/SewerAppurtenanceTypeIMKLValue/pompstation</v>
       </c>
     </row>
-    <row r="220" spans="1:7" hidden="1">
+    <row r="220" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A220" s="4" t="s">
         <v>131</v>
       </c>
@@ -7464,7 +7463,7 @@
         <v>http://www.geonovum.nl/imkl2015/1.0/def/SewerAppurtenanceTypeIMKLValue/overdrachtsstation</v>
       </c>
     </row>
-    <row r="221" spans="1:7" hidden="1">
+    <row r="221" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A221" s="4" t="s">
         <v>131</v>
       </c>
@@ -7479,7 +7478,7 @@
         <v>http://www.geonovum.nl/imkl2015/1.0/def/SewerAppurtenanceTypeIMKLValue/</v>
       </c>
     </row>
-    <row r="222" spans="1:7" hidden="1">
+    <row r="222" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A222" s="4" t="s">
         <v>131</v>
       </c>
@@ -7503,7 +7502,7 @@
         <v>http://www.geonovum.nl/imkl2015/1.0/def/SewerAppurtenanceTypeIMKLValue/mantelbuis</v>
       </c>
     </row>
-    <row r="223" spans="1:7" ht="70" hidden="1">
+    <row r="223" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="A223" s="4" t="s">
         <v>131</v>
       </c>
@@ -7527,7 +7526,7 @@
         <v>http://www.geonovum.nl/imkl2015/1.0/def/SewerAppurtenanceTypeIMKLValue/zinker</v>
       </c>
     </row>
-    <row r="224" spans="1:7" hidden="1">
+    <row r="224" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A224" s="4" t="s">
         <v>131</v>
       </c>
@@ -7551,7 +7550,7 @@
         <v>http://www.geonovum.nl/imkl2015/1.0/def/SewerAppurtenanceTypeIMKLValue/inEnUittredepuntBoringen</v>
       </c>
     </row>
-    <row r="225" spans="1:7" hidden="1">
+    <row r="225" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A225" s="4" t="s">
         <v>131</v>
       </c>
@@ -7575,7 +7574,7 @@
         <v>http://www.geonovum.nl/imkl2015/1.0/def/SewerAppurtenanceTypeIMKLValue/gestuurdeBoring</v>
       </c>
     </row>
-    <row r="226" spans="1:7" hidden="1">
+    <row r="226" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A226" s="4" t="s">
         <v>131</v>
       </c>
@@ -7590,7 +7589,7 @@
         <v>http://www.geonovum.nl/imkl2015/1.0/def/SewerAppurtenanceTypeIMKLValue/</v>
       </c>
     </row>
-    <row r="227" spans="1:7" hidden="1">
+    <row r="227" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A227" s="4" t="s">
         <v>131</v>
       </c>
@@ -7612,15 +7611,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:G227">
-    <filterColumn colId="5">
-      <filters>
-        <filter val="TelecommunicationsAppurtenanceIMKLTypeValue"/>
-        <filter val="TelecommunicationsCableMaterialTypeValue"/>
-        <filter val="UtilityNetworkTypeValue"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="A1:G227"/>
   <sortState ref="B2:F62">
     <sortCondition ref="C2:C62"/>
     <sortCondition ref="B2:B62"/>
@@ -7699,15 +7690,15 @@
       <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.83203125" customWidth="1"/>
-    <col min="2" max="2" width="40.1640625" customWidth="1"/>
-    <col min="3" max="3" width="37.5" customWidth="1"/>
-    <col min="4" max="4" width="22.6640625" customWidth="1"/>
+    <col min="1" max="1" width="13.85546875" customWidth="1"/>
+    <col min="2" max="2" width="40.140625" customWidth="1"/>
+    <col min="3" max="3" width="37.42578125" customWidth="1"/>
+    <col min="4" max="4" width="22.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="4" customFormat="1" ht="15" thickBot="1">
+    <row r="1" spans="1:5" s="4" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="5" t="s">
         <v>2</v>
       </c>
@@ -7724,7 +7715,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="15" thickBot="1">
+    <row r="2" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>28</v>
       </c>
@@ -7735,7 +7726,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="15" thickBot="1">
+    <row r="3" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>28</v>
       </c>
@@ -7746,7 +7737,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="15" thickBot="1">
+    <row r="4" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>28</v>
       </c>
@@ -7757,7 +7748,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="15" thickBot="1">
+    <row r="5" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>28</v>
       </c>
@@ -7768,7 +7759,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="15" thickBot="1">
+    <row r="6" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>28</v>
       </c>
@@ -7779,7 +7770,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="15" thickBot="1">
+    <row r="7" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>28</v>
       </c>
@@ -7790,7 +7781,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="15" thickBot="1">
+    <row r="8" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>28</v>
       </c>
@@ -7801,7 +7792,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="15" thickBot="1">
+    <row r="9" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>28</v>
       </c>
@@ -7812,7 +7803,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="15" thickBot="1">
+    <row r="10" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>28</v>
       </c>
@@ -7823,7 +7814,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="1:5" ht="15" thickBot="1">
+    <row r="11" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>28</v>
       </c>
@@ -7834,7 +7825,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="12" spans="1:5" ht="15" thickBot="1">
+    <row r="12" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>28</v>
       </c>
@@ -7845,7 +7836,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="13" spans="1:5" ht="15" thickBot="1">
+    <row r="13" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>28</v>
       </c>
@@ -7856,7 +7847,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="14" spans="1:5" ht="15" thickBot="1">
+    <row r="14" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>28</v>
       </c>
@@ -7867,7 +7858,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="15" spans="1:5" ht="15" thickBot="1">
+    <row r="15" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>28</v>
       </c>
@@ -7878,7 +7869,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="16" spans="1:5" ht="15" thickBot="1">
+    <row r="16" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>28</v>
       </c>
@@ -7889,7 +7880,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="17" spans="1:3" ht="15" thickBot="1">
+    <row r="17" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>28</v>
       </c>
@@ -7900,7 +7891,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="18" spans="1:3" ht="15" thickBot="1">
+    <row r="18" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>28</v>
       </c>
@@ -7911,7 +7902,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="19" spans="1:3" ht="15" thickBot="1">
+    <row r="19" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>28</v>
       </c>
@@ -7922,7 +7913,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="20" spans="1:3" ht="15" thickBot="1">
+    <row r="20" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>28</v>
       </c>
@@ -7933,7 +7924,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="21" spans="1:3" ht="15" thickBot="1">
+    <row r="21" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>28</v>
       </c>
@@ -7944,7 +7935,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="22" spans="1:3" ht="15" thickBot="1">
+    <row r="22" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>28</v>
       </c>
@@ -7955,7 +7946,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="23" spans="1:3" ht="15" thickBot="1">
+    <row r="23" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>28</v>
       </c>
@@ -7966,7 +7957,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="24" spans="1:3" ht="15" thickBot="1">
+    <row r="24" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>28</v>
       </c>
@@ -7977,7 +7968,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="25" spans="1:3" ht="15" thickBot="1">
+    <row r="25" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>28</v>
       </c>
@@ -7988,7 +7979,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="26" spans="1:3" ht="15" thickBot="1">
+    <row r="26" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>28</v>
       </c>
@@ -7999,7 +7990,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="27" spans="1:3" ht="15" thickBot="1">
+    <row r="27" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>28</v>
       </c>
@@ -8010,12 +8001,12 @@
         <v>27</v>
       </c>
     </row>
-    <row r="28" spans="1:3">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" s="1"/>
       <c r="B28" s="1"/>
       <c r="C28" s="1"/>
     </row>
-    <row r="29" spans="1:3">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>82</v>
       </c>
@@ -8026,7 +8017,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="30" spans="1:3">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
         <v>82</v>
       </c>
@@ -8037,12 +8028,12 @@
         <v>69</v>
       </c>
     </row>
-    <row r="31" spans="1:3">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" s="1"/>
       <c r="B31" s="1"/>
       <c r="C31" s="3"/>
     </row>
-    <row r="32" spans="1:3" ht="15" customHeight="1"/>
+    <row r="32" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="C2" r:id="rId1" display="http://inspire.ec.europa.eu/codelist/ElectricityAppurtenanceTypeValue/connectionBox"/>
@@ -8089,16 +8080,16 @@
       <selection activeCell="D1" sqref="D1:F1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.5" customWidth="1"/>
-    <col min="2" max="2" width="30.83203125" customWidth="1"/>
-    <col min="3" max="3" width="45.5" customWidth="1"/>
-    <col min="4" max="5" width="24.6640625" hidden="1" customWidth="1"/>
-    <col min="6" max="6" width="17.1640625" hidden="1" customWidth="1"/>
+    <col min="1" max="1" width="12.42578125" customWidth="1"/>
+    <col min="2" max="2" width="30.85546875" customWidth="1"/>
+    <col min="3" max="3" width="45.42578125" customWidth="1"/>
+    <col min="4" max="5" width="24.7109375" hidden="1" customWidth="1"/>
+    <col min="6" max="6" width="17.140625" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="4" customFormat="1" ht="15" thickBot="1">
+    <row r="1" spans="1:6" s="4" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="5" t="s">
         <v>2</v>
       </c>
@@ -8118,7 +8109,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="15" thickBot="1">
+    <row r="2" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="12" t="s">
         <v>206</v>
       </c>
@@ -8135,7 +8126,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="15" thickBot="1">
+    <row r="3" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="12" t="s">
         <v>206</v>
       </c>
@@ -8152,7 +8143,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="15" thickBot="1">
+    <row r="4" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="12" t="s">
         <v>206</v>
       </c>
@@ -8169,7 +8160,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="15" thickBot="1">
+    <row r="5" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="12" t="s">
         <v>206</v>
       </c>
@@ -8186,7 +8177,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="15" thickBot="1">
+    <row r="6" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="12" t="s">
         <v>206</v>
       </c>
@@ -8203,7 +8194,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="15" thickBot="1">
+    <row r="7" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="12" t="s">
         <v>206</v>
       </c>
@@ -8220,7 +8211,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="15" thickBot="1">
+    <row r="8" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="12" t="s">
         <v>206</v>
       </c>
@@ -8237,7 +8228,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="15" thickBot="1">
+    <row r="9" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="12" t="s">
         <v>206</v>
       </c>
@@ -8254,7 +8245,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="15" thickBot="1">
+    <row r="10" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="12" t="s">
         <v>206</v>
       </c>
@@ -8271,7 +8262,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="15" thickBot="1">
+    <row r="11" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="12" t="s">
         <v>206</v>
       </c>
@@ -8288,7 +8279,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="15" thickBot="1">
+    <row r="12" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="12" t="s">
         <v>206</v>
       </c>
@@ -8305,7 +8296,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="15" thickBot="1">
+    <row r="13" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="12" t="s">
         <v>206</v>
       </c>
@@ -8322,7 +8313,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="14" spans="1:6">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="12" t="s">
         <v>206</v>
       </c>
@@ -8339,7 +8330,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="15" spans="1:6">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="12" t="s">
         <v>206</v>
       </c>
@@ -8356,7 +8347,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="16" spans="1:6">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>82</v>
       </c>
@@ -8373,7 +8364,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="17" spans="1:3">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>82</v>
       </c>
@@ -8384,7 +8375,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="18" spans="1:3">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>82</v>
       </c>
@@ -8395,7 +8386,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="19" spans="1:3">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>82</v>
       </c>
@@ -8406,7 +8397,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="20" spans="1:3">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>82</v>
       </c>
@@ -8417,7 +8408,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="21" spans="1:3">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>82</v>
       </c>
@@ -8428,7 +8419,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="22" spans="1:3">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>82</v>
       </c>
@@ -8439,7 +8430,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="23" spans="1:3">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>82</v>
       </c>
@@ -8450,7 +8441,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="24" spans="1:3">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>82</v>
       </c>
@@ -8461,7 +8452,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="25" spans="1:3">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>82</v>
       </c>
@@ -8472,7 +8463,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="26" spans="1:3">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>82</v>
       </c>
@@ -8483,7 +8474,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="27" spans="1:3">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>82</v>
       </c>
@@ -8494,7 +8485,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="28" spans="1:3">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>82</v>
       </c>
@@ -8505,7 +8496,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="29" spans="1:3">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>28</v>
       </c>
@@ -8516,7 +8507,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="30" spans="1:3">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
         <v>28</v>
       </c>
@@ -8527,7 +8518,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="31" spans="1:3">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
         <v>28</v>
       </c>
@@ -8538,7 +8529,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="32" spans="1:3">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
         <v>28</v>
       </c>
@@ -8549,7 +8540,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="33" spans="1:3">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
         <v>28</v>
       </c>
@@ -8560,7 +8551,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="34" spans="1:3">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
         <v>28</v>
       </c>
@@ -8571,7 +8562,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="35" spans="1:3">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
         <v>28</v>
       </c>
@@ -8582,7 +8573,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="36" spans="1:3">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
         <v>28</v>
       </c>
@@ -8593,7 +8584,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="37" spans="1:3">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
         <v>28</v>
       </c>
@@ -8604,7 +8595,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="38" spans="1:3">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
         <v>28</v>
       </c>
@@ -8615,7 +8606,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="39" spans="1:3">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
         <v>28</v>
       </c>
@@ -8626,7 +8617,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="40" spans="1:3">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
         <v>28</v>
       </c>
@@ -8637,7 +8628,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="41" spans="1:3">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
         <v>82</v>
       </c>
@@ -8648,7 +8639,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="42" spans="1:3">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
         <v>82</v>
       </c>
@@ -8659,7 +8650,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="43" spans="1:3">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
         <v>82</v>
       </c>
@@ -8670,7 +8661,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="44" spans="1:3">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
         <v>82</v>
       </c>
@@ -8681,7 +8672,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="45" spans="1:3">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
         <v>82</v>
       </c>
@@ -8692,7 +8683,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="46" spans="1:3">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
         <v>82</v>
       </c>
@@ -8703,7 +8694,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="47" spans="1:3">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
         <v>82</v>
       </c>
@@ -8714,7 +8705,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="48" spans="1:3">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
         <v>82</v>
       </c>
@@ -8725,7 +8716,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="49" spans="1:3">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
         <v>82</v>
       </c>
@@ -8736,7 +8727,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="50" spans="1:3">
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
         <v>82</v>
       </c>
@@ -8747,7 +8738,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="51" spans="1:3">
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
         <v>82</v>
       </c>
@@ -8758,7 +8749,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="52" spans="1:3">
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
         <v>82</v>
       </c>
@@ -8769,7 +8760,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="53" spans="1:3">
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
         <v>82</v>
       </c>
@@ -8780,7 +8771,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="54" spans="1:3">
+    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
         <v>82</v>
       </c>
@@ -8791,7 +8782,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="55" spans="1:3">
+    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
         <v>82</v>
       </c>
@@ -8802,7 +8793,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="56" spans="1:3">
+    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
         <v>82</v>
       </c>
@@ -8813,7 +8804,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="57" spans="1:3">
+    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
         <v>82</v>
       </c>
@@ -8824,7 +8815,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="58" spans="1:3">
+    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="s">
         <v>82</v>
       </c>
@@ -8835,7 +8826,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="59" spans="1:3">
+    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A59" s="1" t="s">
         <v>82</v>
       </c>
@@ -8846,7 +8837,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="60" spans="1:3">
+    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A60" s="1" t="s">
         <v>82</v>
       </c>
@@ -8857,7 +8848,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="61" spans="1:3">
+    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A61" s="1" t="s">
         <v>82</v>
       </c>
@@ -8868,7 +8859,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="62" spans="1:3">
+    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A62" s="1" t="s">
         <v>82</v>
       </c>
@@ -8879,7 +8870,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="63" spans="1:3">
+    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A63" s="1" t="s">
         <v>82</v>
       </c>
@@ -8890,7 +8881,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="64" spans="1:3">
+    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A64" s="1" t="s">
         <v>82</v>
       </c>
@@ -8901,7 +8892,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="65" spans="1:3">
+    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A65" s="1" t="s">
         <v>82</v>
       </c>
@@ -8912,7 +8903,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="66" spans="1:3">
+    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A66" s="1" t="s">
         <v>82</v>
       </c>
@@ -8923,7 +8914,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="67" spans="1:3">
+    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A67" s="1" t="s">
         <v>82</v>
       </c>
@@ -8934,7 +8925,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="68" spans="1:3">
+    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A68" s="1" t="s">
         <v>82</v>
       </c>
@@ -8945,7 +8936,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="69" spans="1:3">
+    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A69" s="1" t="s">
         <v>82</v>
       </c>
@@ -8956,7 +8947,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="70" spans="1:3">
+    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A70" s="1" t="s">
         <v>82</v>
       </c>
@@ -8967,7 +8958,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="71" spans="1:3">
+    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A71" s="1" t="s">
         <v>82</v>
       </c>
@@ -8978,7 +8969,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="72" spans="1:3">
+    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A72" s="1" t="s">
         <v>82</v>
       </c>
@@ -8989,7 +8980,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="73" spans="1:3">
+    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A73" s="1" t="s">
         <v>82</v>
       </c>
@@ -9000,7 +8991,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="74" spans="1:3">
+    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A74" s="1" t="s">
         <v>82</v>
       </c>
@@ -9011,7 +9002,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="75" spans="1:3">
+    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A75" s="1" t="s">
         <v>82</v>
       </c>
@@ -9022,7 +9013,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="76" spans="1:3">
+    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A76" s="1" t="s">
         <v>82</v>
       </c>
@@ -9033,7 +9024,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="77" spans="1:3">
+    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A77" s="1" t="s">
         <v>82</v>
       </c>
@@ -9044,7 +9035,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="78" spans="1:3">
+    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A78" s="1" t="s">
         <v>82</v>
       </c>
@@ -9055,21 +9046,21 @@
         <v>176</v>
       </c>
     </row>
-    <row r="79" spans="1:3">
+    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A79" s="1"/>
       <c r="B79" s="1"/>
       <c r="C79" s="1"/>
     </row>
-    <row r="80" spans="1:3">
+    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A80" s="1"/>
       <c r="B80" s="1"/>
       <c r="C80" s="1"/>
     </row>
-    <row r="82" spans="4:5">
+    <row r="82" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D82" s="8"/>
       <c r="E82" s="8"/>
     </row>
-    <row r="83" spans="4:5">
+    <row r="83" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D83" s="8"/>
       <c r="E83" s="8"/>
     </row>
@@ -9111,15 +9102,15 @@
       <selection activeCell="B55" sqref="B55"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="30.83203125" customWidth="1"/>
-    <col min="3" max="3" width="30.33203125" customWidth="1"/>
-    <col min="4" max="4" width="24.6640625" customWidth="1"/>
-    <col min="5" max="5" width="17.1640625" customWidth="1"/>
+    <col min="2" max="2" width="30.85546875" customWidth="1"/>
+    <col min="3" max="3" width="30.28515625" customWidth="1"/>
+    <col min="4" max="4" width="24.7109375" customWidth="1"/>
+    <col min="5" max="5" width="17.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="4" customFormat="1" ht="15" thickBot="1">
+    <row r="1" spans="1:5" s="4" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="5" t="s">
         <v>2</v>
       </c>
@@ -9136,7 +9127,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="15" thickBot="1">
+    <row r="2" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>28</v>
       </c>
@@ -9147,7 +9138,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="15" thickBot="1">
+    <row r="3" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>28</v>
       </c>
@@ -9158,7 +9149,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="15" thickBot="1">
+    <row r="4" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>28</v>
       </c>
@@ -9169,7 +9160,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="15" thickBot="1">
+    <row r="5" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>28</v>
       </c>
@@ -9180,7 +9171,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="15" thickBot="1">
+    <row r="6" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>28</v>
       </c>
@@ -9191,7 +9182,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="15" thickBot="1">
+    <row r="7" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>28</v>
       </c>
@@ -9202,7 +9193,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="15" thickBot="1">
+    <row r="8" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>28</v>
       </c>
@@ -9213,7 +9204,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="15" thickBot="1">
+    <row r="9" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>28</v>
       </c>
@@ -9224,7 +9215,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="15" thickBot="1">
+    <row r="10" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>28</v>
       </c>
@@ -9235,7 +9226,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="11" spans="1:5" ht="15" thickBot="1">
+    <row r="11" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>28</v>
       </c>
@@ -9246,7 +9237,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="12" spans="1:5" ht="15" thickBot="1">
+    <row r="12" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>28</v>
       </c>
@@ -9257,7 +9248,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="13" spans="1:5" ht="15" thickBot="1">
+    <row r="13" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>28</v>
       </c>
@@ -9268,12 +9259,12 @@
         <v>42</v>
       </c>
     </row>
-    <row r="14" spans="1:5">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="1"/>
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
     </row>
-    <row r="15" spans="1:5">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>82</v>
       </c>
@@ -9284,7 +9275,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="16" spans="1:5">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>82</v>
       </c>
@@ -9295,7 +9286,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="17" spans="1:3">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>82</v>
       </c>
@@ -9306,7 +9297,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="18" spans="1:3">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>82</v>
       </c>
@@ -9317,7 +9308,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="19" spans="1:3">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>82</v>
       </c>
@@ -9328,7 +9319,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="20" spans="1:3">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>82</v>
       </c>
@@ -9339,7 +9330,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="21" spans="1:3">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>82</v>
       </c>
@@ -9350,7 +9341,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="22" spans="1:3">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>82</v>
       </c>
@@ -9361,7 +9352,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="23" spans="1:3">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>82</v>
       </c>
@@ -9372,7 +9363,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="24" spans="1:3">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>82</v>
       </c>
@@ -9383,7 +9374,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="25" spans="1:3" ht="14.25" customHeight="1">
+    <row r="25" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>82</v>
       </c>
@@ -9394,7 +9385,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="26" spans="1:3" ht="15.75" customHeight="1">
+    <row r="26" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>82</v>
       </c>
@@ -9405,7 +9396,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="27" spans="1:3">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>82</v>
       </c>
@@ -9416,12 +9407,12 @@
         <v>80</v>
       </c>
     </row>
-    <row r="28" spans="1:3">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" s="1"/>
       <c r="B28" s="1"/>
       <c r="C28" s="1"/>
     </row>
-    <row r="29" spans="1:3">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>82</v>
       </c>
@@ -9432,7 +9423,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="30" spans="1:3">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
         <v>82</v>
       </c>
@@ -9443,7 +9434,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="31" spans="1:3">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
         <v>82</v>
       </c>
@@ -9454,7 +9445,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="32" spans="1:3">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
         <v>82</v>
       </c>
@@ -9465,7 +9456,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="33" spans="1:3">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
         <v>82</v>
       </c>
@@ -9476,7 +9467,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="34" spans="1:3">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
         <v>82</v>
       </c>
@@ -9487,7 +9478,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="35" spans="1:3">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
         <v>82</v>
       </c>
@@ -9498,7 +9489,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="36" spans="1:3">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
         <v>82</v>
       </c>
@@ -9509,7 +9500,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="37" spans="1:3">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
         <v>82</v>
       </c>
@@ -9520,7 +9511,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="38" spans="1:3">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
         <v>82</v>
       </c>
@@ -9531,7 +9522,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="39" spans="1:3">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
         <v>82</v>
       </c>
@@ -9542,7 +9533,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="40" spans="1:3">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
         <v>82</v>
       </c>
@@ -9553,7 +9544,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="41" spans="1:3">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
         <v>82</v>
       </c>
@@ -9564,7 +9555,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="42" spans="1:3">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
         <v>82</v>
       </c>
@@ -9575,7 +9566,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="43" spans="1:3">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
         <v>82</v>
       </c>
@@ -9586,7 +9577,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="44" spans="1:3">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
         <v>82</v>
       </c>
@@ -9597,7 +9588,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="45" spans="1:3">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
         <v>82</v>
       </c>
@@ -9608,7 +9599,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="46" spans="1:3">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
         <v>82</v>
       </c>
@@ -9619,7 +9610,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="47" spans="1:3">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
         <v>82</v>
       </c>
@@ -9630,7 +9621,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="48" spans="1:3">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
         <v>82</v>
       </c>
@@ -9641,7 +9632,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="49" spans="1:3">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
         <v>82</v>
       </c>
@@ -9652,7 +9643,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="50" spans="1:3">
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
         <v>82</v>
       </c>
@@ -9663,7 +9654,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="51" spans="1:3">
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
         <v>82</v>
       </c>
@@ -9674,7 +9665,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="52" spans="1:3">
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
         <v>82</v>
       </c>
@@ -9685,7 +9676,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="53" spans="1:3">
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
         <v>82</v>
       </c>
@@ -9696,7 +9687,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="54" spans="1:3">
+    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
         <v>82</v>
       </c>
@@ -9707,7 +9698,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="55" spans="1:3">
+    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
         <v>82</v>
       </c>
@@ -9718,7 +9709,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="56" spans="1:3">
+    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
         <v>82</v>
       </c>
@@ -9729,7 +9720,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="57" spans="1:3">
+    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
         <v>82</v>
       </c>
@@ -9740,7 +9731,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="58" spans="1:3">
+    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="s">
         <v>82</v>
       </c>
@@ -9751,7 +9742,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="59" spans="1:3">
+    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A59" s="1" t="s">
         <v>82</v>
       </c>
@@ -9762,7 +9753,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="60" spans="1:3">
+    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A60" s="1" t="s">
         <v>82</v>
       </c>
@@ -9773,7 +9764,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="61" spans="1:3">
+    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A61" s="1" t="s">
         <v>82</v>
       </c>
@@ -9784,7 +9775,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="62" spans="1:3">
+    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A62" s="1" t="s">
         <v>82</v>
       </c>
@@ -9795,7 +9786,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="63" spans="1:3">
+    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A63" s="1" t="s">
         <v>82</v>
       </c>
@@ -9806,7 +9797,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="64" spans="1:3">
+    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A64" s="1" t="s">
         <v>82</v>
       </c>
@@ -9817,7 +9808,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="65" spans="1:3">
+    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A65" s="1" t="s">
         <v>82</v>
       </c>
@@ -9828,7 +9819,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="66" spans="1:3">
+    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A66" s="1" t="s">
         <v>82</v>
       </c>

</xml_diff>